<commit_message>
USD_YCSTD bootstrap - empty placeholder
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YCONBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YCONBootstrapping.xlsx
@@ -10,9 +10,9 @@
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
     <sheet name="RateHelpers" sheetId="4" r:id="rId2"/>
     <sheet name="Selected" sheetId="5" r:id="rId3"/>
-    <sheet name="ON" sheetId="9" r:id="rId4"/>
-    <sheet name="ON (2)" sheetId="17" r:id="rId5"/>
-    <sheet name="ON (3)" sheetId="30" r:id="rId6"/>
+    <sheet name="ON_Deposits" sheetId="9" r:id="rId4"/>
+    <sheet name="ON_FRAs" sheetId="17" r:id="rId5"/>
+    <sheet name="ON_Swaps" sheetId="30" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Accuracy">'General Settings'!$D$23</definedName>
@@ -24,7 +24,7 @@
     <definedName name="DepoInclusionCriteria">Selected!$B$5</definedName>
     <definedName name="Discounting">'General Settings'!$M$13</definedName>
     <definedName name="Discounting2">'General Settings'!$M$14</definedName>
-    <definedName name="DiscountingCurve" localSheetId="5">'ON (3)'!$L$2</definedName>
+    <definedName name="DiscountingCurve" localSheetId="5">ON_Swaps!$L$2</definedName>
     <definedName name="FamilyName">'General Settings'!$M$11</definedName>
     <definedName name="FileOverwrite">'General Settings'!$M$6</definedName>
     <definedName name="FrontFuturesRollingDays">Selected!$B$4</definedName>
@@ -1971,21 +1971,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2003,6 +1988,21 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="34" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2322,39 +2322,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="2.7109375" style="187" customWidth="1"/>
-    <col min="3" max="3" width="18" style="187" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="187" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="187" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="2.7109375" style="187" customWidth="1"/>
-    <col min="8" max="9" width="8" style="187"/>
-    <col min="10" max="11" width="2.7109375" style="187" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="187" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53.7109375" style="187" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.7109375" style="187" customWidth="1"/>
-    <col min="15" max="16384" width="8" style="187"/>
+    <col min="1" max="2" width="2.7109375" style="182" customWidth="1"/>
+    <col min="3" max="3" width="18" style="182" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="182" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="182" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="2.7109375" style="182" customWidth="1"/>
+    <col min="8" max="9" width="8" style="182"/>
+    <col min="10" max="11" width="2.7109375" style="182" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="182" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="53.7109375" style="182" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="182" customWidth="1"/>
+    <col min="15" max="16384" width="8" style="182"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="187" t="str">
+      <c r="B1" s="182" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
         <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Dec  5 2013 11:03:51</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="190" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="196"/>
-      <c r="D2" s="196"/>
-      <c r="E2" s="196"/>
-      <c r="F2" s="197"/>
-      <c r="K2" s="195" t="s">
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="192"/>
+      <c r="K2" s="190" t="s">
         <v>152</v>
       </c>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="198"/>
+      <c r="L2" s="191"/>
+      <c r="M2" s="191"/>
+      <c r="N2" s="193"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="61"/>
@@ -2377,10 +2377,10 @@
       </c>
       <c r="E4" s="58"/>
       <c r="F4" s="57"/>
-      <c r="H4" s="190" t="s">
+      <c r="H4" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="191"/>
+      <c r="I4" s="186"/>
       <c r="K4" s="135"/>
       <c r="L4" s="134" t="s">
         <v>151</v>
@@ -2398,10 +2398,10 @@
       <c r="D5" s="62"/>
       <c r="E5" s="58"/>
       <c r="F5" s="57"/>
-      <c r="H5" s="188" t="s">
+      <c r="H5" s="183" t="s">
         <v>135</v>
       </c>
-      <c r="I5" s="189" t="s">
+      <c r="I5" s="184" t="s">
         <v>134</v>
       </c>
       <c r="K5" s="135"/>
@@ -2424,10 +2424,10 @@
       </c>
       <c r="E6" s="58"/>
       <c r="F6" s="57"/>
-      <c r="H6" s="188" t="s">
+      <c r="H6" s="183" t="s">
         <v>131</v>
       </c>
-      <c r="I6" s="189"/>
+      <c r="I6" s="184"/>
       <c r="K6" s="135"/>
       <c r="L6" s="134" t="s">
         <v>149</v>
@@ -2447,10 +2447,10 @@
       </c>
       <c r="E7" s="58"/>
       <c r="F7" s="57"/>
-      <c r="H7" s="188" t="s">
+      <c r="H7" s="183" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="189"/>
+      <c r="I7" s="184"/>
       <c r="K7" s="132"/>
       <c r="L7" s="131"/>
       <c r="M7" s="131"/>
@@ -2466,16 +2466,16 @@
       </c>
       <c r="E8" s="58"/>
       <c r="F8" s="57"/>
-      <c r="H8" s="192" t="s">
+      <c r="H8" s="187" t="s">
         <v>126</v>
       </c>
-      <c r="I8" s="193" t="s">
+      <c r="I8" s="188" t="s">
         <v>125</v>
       </c>
-      <c r="K8" s="194"/>
-      <c r="L8" s="194"/>
-      <c r="M8" s="194"/>
-      <c r="N8" s="194"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="189"/>
+      <c r="M8" s="189"/>
+      <c r="N8" s="189"/>
     </row>
     <row r="9" spans="2:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
@@ -2488,12 +2488,12 @@
       </c>
       <c r="E9" s="58"/>
       <c r="F9" s="57"/>
-      <c r="K9" s="195" t="s">
+      <c r="K9" s="190" t="s">
         <v>148</v>
       </c>
-      <c r="L9" s="196"/>
-      <c r="M9" s="196"/>
-      <c r="N9" s="198"/>
+      <c r="L9" s="191"/>
+      <c r="M9" s="191"/>
+      <c r="N9" s="193"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="61"/>
@@ -2516,7 +2516,7 @@
         <v>122</v>
       </c>
       <c r="D11" s="86">
-        <v>41627.761770833335</v>
+        <v>41653.299837962964</v>
       </c>
       <c r="E11" s="58"/>
       <c r="F11" s="57"/>
@@ -2571,7 +2571,7 @@
       </c>
       <c r="D14" s="83" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYCON#0006</v>
+        <v>_USDYCON#0000</v>
       </c>
       <c r="E14" s="58"/>
       <c r="F14" s="57"/>
@@ -2660,11 +2660,11 @@
       </c>
       <c r="D21" s="75">
         <f>DATE(YEAR(_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),NDays&amp;"D")),12,31)</f>
-        <v>41639</v>
+        <v>42004</v>
       </c>
       <c r="E21" s="74">
         <f>DATE(YEAR(D21+1),12,31)</f>
-        <v>42004</v>
+        <v>42369</v>
       </c>
       <c r="F21" s="57"/>
     </row>
@@ -2725,7 +2725,7 @@
       <c r="B27" s="61"/>
       <c r="C27" s="65">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41627</v>
+        <v>41653</v>
       </c>
       <c r="D27" s="64">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2738,11 +2738,11 @@
       <c r="B28" s="61"/>
       <c r="C28" s="63">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>59894</v>
+        <v>59917</v>
       </c>
       <c r="D28" s="62">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.18593203137578257</v>
+        <v>0.18595467193896159</v>
       </c>
       <c r="E28" s="58"/>
       <c r="F28" s="57"/>
@@ -2827,11 +2827,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.5" x14ac:dyDescent="0.2">
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="194" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="183"/>
-      <c r="D1" s="184"/>
+      <c r="C1" s="195"/>
+      <c r="D1" s="196"/>
       <c r="E1" s="32" t="s">
         <v>96</v>
       </c>
@@ -2864,8 +2864,8 @@
         <v>88</v>
       </c>
       <c r="E2" s="14" t="str">
-        <f>ON!F3</f>
-        <v>USD_YCONRH_OND#0006</v>
+        <f>ON_Deposits!F3</f>
+        <v>USD_YCONRH_OND#0000</v>
       </c>
       <c r="F2" s="13">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
@@ -2883,11 +2883,11 @@
       </c>
       <c r="K2" s="12">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41627</v>
+        <v>41653</v>
       </c>
       <c r="L2" s="11">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41628</v>
+        <v>41654</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2897,8 +2897,8 @@
         <v>87</v>
       </c>
       <c r="E3" s="14" t="str">
-        <f>'ON (2)'!H3</f>
-        <v>USD_YCONRH_TND#0005</v>
+        <f>ON_FRAs!H3</f>
+        <v>USD_YCONRH_TND#0000</v>
       </c>
       <c r="F3" s="13">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
@@ -2916,11 +2916,11 @@
       </c>
       <c r="K3" s="12">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41628</v>
+        <v>41654</v>
       </c>
       <c r="L3" s="11">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2930,8 +2930,8 @@
         <v>86</v>
       </c>
       <c r="E4" s="14" t="str">
-        <f>'ON (2)'!H4</f>
-        <v>USD_YCONRH_SND#0005</v>
+        <f>ON_FRAs!H4</f>
+        <v>USD_YCONRH_SND#0000</v>
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
@@ -2949,11 +2949,11 @@
       </c>
       <c r="K4" s="12">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L4" s="11">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41632</v>
+        <v>41656</v>
       </c>
     </row>
     <row r="5" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4148,8 +4148,8 @@
         <v>68</v>
       </c>
       <c r="E35" s="21" t="str">
-        <f>'ON (3)'!L6</f>
-        <v>USD_YCONRH_OISSW#0006</v>
+        <f>ON_Swaps!L6</f>
+        <v>USD_YCONRH_OISSW#0000</v>
       </c>
       <c r="F35" s="20">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
@@ -4171,11 +4171,11 @@
       </c>
       <c r="K35" s="18">
         <f>_xll.qlRateHelperEarliestDate($E35,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L35" s="17">
         <f>_xll.qlRateHelperLatestDate($E35,Trigger)</f>
-        <v>41638</v>
+        <v>41662</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
@@ -4188,8 +4188,8 @@
         <v>67</v>
       </c>
       <c r="E36" s="14" t="str">
-        <f>'ON (3)'!L7</f>
-        <v>USD_YCONRH_OIS2W#0006</v>
+        <f>ON_Swaps!L7</f>
+        <v>USD_YCONRH_OIS2W#0000</v>
       </c>
       <c r="F36" s="13">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
@@ -4211,11 +4211,11 @@
       </c>
       <c r="K36" s="12">
         <f>_xll.qlRateHelperEarliestDate($E36,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L36" s="11">
         <f>_xll.qlRateHelperLatestDate($E36,Trigger)</f>
-        <v>41645</v>
+        <v>41669</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
@@ -4228,8 +4228,8 @@
         <v>66</v>
       </c>
       <c r="E37" s="14" t="str">
-        <f>'ON (3)'!L8</f>
-        <v>USD_YCONRH_OIS3W#0006</v>
+        <f>ON_Swaps!L8</f>
+        <v>USD_YCONRH_OIS3W#0000</v>
       </c>
       <c r="F37" s="13">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
@@ -4251,11 +4251,11 @@
       </c>
       <c r="K37" s="12">
         <f>_xll.qlRateHelperEarliestDate($E37,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L37" s="11">
         <f>_xll.qlRateHelperLatestDate($E37,Trigger)</f>
-        <v>41652</v>
+        <v>41676</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
@@ -4268,8 +4268,8 @@
         <v>65</v>
       </c>
       <c r="E38" s="14" t="str">
-        <f>'ON (3)'!L9</f>
-        <v>USD_YCONRH_OIS1M#0006</v>
+        <f>ON_Swaps!L9</f>
+        <v>USD_YCONRH_OIS1M#0000</v>
       </c>
       <c r="F38" s="13">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
@@ -4291,11 +4291,11 @@
       </c>
       <c r="K38" s="12">
         <f>_xll.qlRateHelperEarliestDate($E38,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L38" s="11">
         <f>_xll.qlRateHelperLatestDate($E38,Trigger)</f>
-        <v>41662</v>
+        <v>41687</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
@@ -4308,8 +4308,8 @@
         <v>64</v>
       </c>
       <c r="E39" s="14" t="str">
-        <f>'ON (3)'!L10</f>
-        <v>USD_YCONRH_OIS2M#0006</v>
+        <f>ON_Swaps!L10</f>
+        <v>USD_YCONRH_OIS2M#0000</v>
       </c>
       <c r="F39" s="13">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
@@ -4331,11 +4331,11 @@
       </c>
       <c r="K39" s="12">
         <f>_xll.qlRateHelperEarliestDate($E39,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L39" s="11">
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
-        <v>41694</v>
+        <v>41715</v>
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.2">
@@ -4348,8 +4348,8 @@
         <v>63</v>
       </c>
       <c r="E40" s="14" t="str">
-        <f>'ON (3)'!L11</f>
-        <v>USD_YCONRH_OIS3M#0006</v>
+        <f>ON_Swaps!L11</f>
+        <v>USD_YCONRH_OIS3M#0000</v>
       </c>
       <c r="F40" s="13">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
@@ -4371,11 +4371,11 @@
       </c>
       <c r="K40" s="12">
         <f>_xll.qlRateHelperEarliestDate($E40,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L40" s="11">
         <f>_xll.qlRateHelperLatestDate($E40,Trigger)</f>
-        <v>41722</v>
+        <v>41745</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
@@ -4388,8 +4388,8 @@
         <v>62</v>
       </c>
       <c r="E41" s="14" t="str">
-        <f>'ON (3)'!L12</f>
-        <v>USD_YCONRH_OIS4M#0006</v>
+        <f>ON_Swaps!L12</f>
+        <v>USD_YCONRH_OIS4M#0000</v>
       </c>
       <c r="F41" s="13">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
@@ -4411,11 +4411,11 @@
       </c>
       <c r="K41" s="12">
         <f>_xll.qlRateHelperEarliestDate($E41,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L41" s="11">
         <f>_xll.qlRateHelperLatestDate($E41,Trigger)</f>
-        <v>41752</v>
+        <v>41775</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
@@ -4428,8 +4428,8 @@
         <v>61</v>
       </c>
       <c r="E42" s="14" t="str">
-        <f>'ON (3)'!L13</f>
-        <v>USD_YCONRH_OIS5M#0006</v>
+        <f>ON_Swaps!L13</f>
+        <v>USD_YCONRH_OIS5M#0000</v>
       </c>
       <c r="F42" s="13">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
@@ -4451,11 +4451,11 @@
       </c>
       <c r="K42" s="12">
         <f>_xll.qlRateHelperEarliestDate($E42,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L42" s="11">
         <f>_xll.qlRateHelperLatestDate($E42,Trigger)</f>
-        <v>41782</v>
+        <v>41806</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
@@ -4468,8 +4468,8 @@
         <v>60</v>
       </c>
       <c r="E43" s="14" t="str">
-        <f>'ON (3)'!L14</f>
-        <v>USD_YCONRH_OIS6M#0006</v>
+        <f>ON_Swaps!L14</f>
+        <v>USD_YCONRH_OIS6M#0000</v>
       </c>
       <c r="F43" s="13">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
@@ -4491,11 +4491,11 @@
       </c>
       <c r="K43" s="12">
         <f>_xll.qlRateHelperEarliestDate($E43,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L43" s="11">
         <f>_xll.qlRateHelperLatestDate($E43,Trigger)</f>
-        <v>41813</v>
+        <v>41836</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
@@ -4508,8 +4508,8 @@
         <v>59</v>
       </c>
       <c r="E44" s="14" t="str">
-        <f>'ON (3)'!L15</f>
-        <v>USD_YCONRH_OIS7M#0006</v>
+        <f>ON_Swaps!L15</f>
+        <v>USD_YCONRH_OIS7M#0000</v>
       </c>
       <c r="F44" s="13">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
@@ -4531,11 +4531,11 @@
       </c>
       <c r="K44" s="12">
         <f>_xll.qlRateHelperEarliestDate($E44,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L44" s="11">
         <f>_xll.qlRateHelperLatestDate($E44,Trigger)</f>
-        <v>41843</v>
+        <v>41869</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.2">
@@ -4548,8 +4548,8 @@
         <v>58</v>
       </c>
       <c r="E45" s="14" t="str">
-        <f>'ON (3)'!L16</f>
-        <v>USD_YCONRH_OIS8M#0006</v>
+        <f>ON_Swaps!L16</f>
+        <v>USD_YCONRH_OIS8M#0000</v>
       </c>
       <c r="F45" s="13">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
@@ -4571,11 +4571,11 @@
       </c>
       <c r="K45" s="12">
         <f>_xll.qlRateHelperEarliestDate($E45,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L45" s="11">
         <f>_xll.qlRateHelperLatestDate($E45,Trigger)</f>
-        <v>41876</v>
+        <v>41898</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
@@ -4588,8 +4588,8 @@
         <v>57</v>
       </c>
       <c r="E46" s="14" t="str">
-        <f>'ON (3)'!L17</f>
-        <v>USD_YCONRH_OIS9M#0006</v>
+        <f>ON_Swaps!L17</f>
+        <v>USD_YCONRH_OIS9M#0000</v>
       </c>
       <c r="F46" s="13">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
@@ -4611,11 +4611,11 @@
       </c>
       <c r="K46" s="12">
         <f>_xll.qlRateHelperEarliestDate($E46,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L46" s="11">
         <f>_xll.qlRateHelperLatestDate($E46,Trigger)</f>
-        <v>41905</v>
+        <v>41928</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
@@ -4628,8 +4628,8 @@
         <v>56</v>
       </c>
       <c r="E47" s="14" t="str">
-        <f>'ON (3)'!L18</f>
-        <v>USD_YCONRH_OIS10M#0006</v>
+        <f>ON_Swaps!L18</f>
+        <v>USD_YCONRH_OIS10M#0000</v>
       </c>
       <c r="F47" s="13">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4651,11 +4651,11 @@
       </c>
       <c r="K47" s="12">
         <f>_xll.qlRateHelperEarliestDate($E47,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L47" s="11">
         <f>_xll.qlRateHelperLatestDate($E47,Trigger)</f>
-        <v>41935</v>
+        <v>41960</v>
       </c>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.2">
@@ -4668,8 +4668,8 @@
         <v>55</v>
       </c>
       <c r="E48" s="14" t="str">
-        <f>'ON (3)'!L19</f>
-        <v>USD_YCONRH_OIS11M#0006</v>
+        <f>ON_Swaps!L19</f>
+        <v>USD_YCONRH_OIS11M#0000</v>
       </c>
       <c r="F48" s="13">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
@@ -4691,11 +4691,11 @@
       </c>
       <c r="K48" s="12">
         <f>_xll.qlRateHelperEarliestDate($E48,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L48" s="11">
         <f>_xll.qlRateHelperLatestDate($E48,Trigger)</f>
-        <v>41967</v>
+        <v>41989</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
@@ -4708,8 +4708,8 @@
         <v>36</v>
       </c>
       <c r="E49" s="14" t="str">
-        <f>'ON (3)'!L20</f>
-        <v>USD_YCONRH_OIS1Y#0006</v>
+        <f>ON_Swaps!L20</f>
+        <v>USD_YCONRH_OIS1Y#0000</v>
       </c>
       <c r="F49" s="13">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
@@ -4731,11 +4731,11 @@
       </c>
       <c r="K49" s="12">
         <f>_xll.qlRateHelperEarliestDate($E49,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L49" s="11">
         <f>_xll.qlRateHelperLatestDate($E49,Trigger)</f>
-        <v>41996</v>
+        <v>42020</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
@@ -4751,8 +4751,8 @@
         <v>54</v>
       </c>
       <c r="E50" s="14" t="str">
-        <f>'ON (3)'!L21</f>
-        <v>USD_YCONRH_OIS13M#0006</v>
+        <f>ON_Swaps!L21</f>
+        <v>USD_YCONRH_OIS13M#0000</v>
       </c>
       <c r="F50" s="13">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
@@ -4774,11 +4774,11 @@
       </c>
       <c r="K50" s="12">
         <f>_xll.qlRateHelperEarliestDate($E50,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L50" s="11">
         <f>_xll.qlRateHelperLatestDate($E50,Trigger)</f>
-        <v>42027</v>
+        <v>42051</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
@@ -4794,8 +4794,8 @@
         <v>53</v>
       </c>
       <c r="E51" s="14" t="str">
-        <f>'ON (3)'!L22</f>
-        <v>USD_YCONRH_OIS14M#0006</v>
+        <f>ON_Swaps!L22</f>
+        <v>USD_YCONRH_OIS14M#0000</v>
       </c>
       <c r="F51" s="13">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
@@ -4817,11 +4817,11 @@
       </c>
       <c r="K51" s="12">
         <f>_xll.qlRateHelperEarliestDate($E51,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L51" s="11">
         <f>_xll.qlRateHelperLatestDate($E51,Trigger)</f>
-        <v>42058</v>
+        <v>42079</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
@@ -4837,8 +4837,8 @@
         <v>35</v>
       </c>
       <c r="E52" s="14" t="str">
-        <f>'ON (3)'!L23</f>
-        <v>USD_YCONRH_OIS15M#0006</v>
+        <f>ON_Swaps!L23</f>
+        <v>USD_YCONRH_OIS15M#0000</v>
       </c>
       <c r="F52" s="13">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
@@ -4860,11 +4860,11 @@
       </c>
       <c r="K52" s="12">
         <f>_xll.qlRateHelperEarliestDate($E52,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L52" s="11">
         <f>_xll.qlRateHelperLatestDate($E52,Trigger)</f>
-        <v>42086</v>
+        <v>42110</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
@@ -4880,8 +4880,8 @@
         <v>52</v>
       </c>
       <c r="E53" s="14" t="str">
-        <f>'ON (3)'!L24</f>
-        <v>USD_YCONRH_OIS16M#0006</v>
+        <f>ON_Swaps!L24</f>
+        <v>USD_YCONRH_OIS16M#0000</v>
       </c>
       <c r="F53" s="13">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
@@ -4903,11 +4903,11 @@
       </c>
       <c r="K53" s="12">
         <f>_xll.qlRateHelperEarliestDate($E53,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L53" s="11">
         <f>_xll.qlRateHelperLatestDate($E53,Trigger)</f>
-        <v>42117</v>
+        <v>42142</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
@@ -4923,8 +4923,8 @@
         <v>51</v>
       </c>
       <c r="E54" s="14" t="str">
-        <f>'ON (3)'!L25</f>
-        <v>USD_YCONRH_OIS17M#0006</v>
+        <f>ON_Swaps!L25</f>
+        <v>USD_YCONRH_OIS17M#0000</v>
       </c>
       <c r="F54" s="13">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
@@ -4946,11 +4946,11 @@
       </c>
       <c r="K54" s="12">
         <f>_xll.qlRateHelperEarliestDate($E54,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L54" s="11">
         <f>_xll.qlRateHelperLatestDate($E54,Trigger)</f>
-        <v>42149</v>
+        <v>42171</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
@@ -4966,8 +4966,8 @@
         <v>34</v>
       </c>
       <c r="E55" s="14" t="str">
-        <f>'ON (3)'!L26</f>
-        <v>USD_YCONRH_OIS18M#0006</v>
+        <f>ON_Swaps!L26</f>
+        <v>USD_YCONRH_OIS18M#0000</v>
       </c>
       <c r="F55" s="13">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
@@ -4989,11 +4989,11 @@
       </c>
       <c r="K55" s="12">
         <f>_xll.qlRateHelperEarliestDate($E55,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L55" s="11">
         <f>_xll.qlRateHelperLatestDate($E55,Trigger)</f>
-        <v>42178</v>
+        <v>42201</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
@@ -5009,8 +5009,8 @@
         <v>50</v>
       </c>
       <c r="E56" s="14" t="str">
-        <f>'ON (3)'!L27</f>
-        <v>USD_YCONRH_OIS19M#0006</v>
+        <f>ON_Swaps!L27</f>
+        <v>USD_YCONRH_OIS19M#0000</v>
       </c>
       <c r="F56" s="13">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
@@ -5032,11 +5032,11 @@
       </c>
       <c r="K56" s="12">
         <f>_xll.qlRateHelperEarliestDate($E56,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L56" s="11">
         <f>_xll.qlRateHelperLatestDate($E56,Trigger)</f>
-        <v>42208</v>
+        <v>42233</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.2">
@@ -5052,8 +5052,8 @@
         <v>49</v>
       </c>
       <c r="E57" s="14" t="str">
-        <f>'ON (3)'!L28</f>
-        <v>USD_YCONRH_OIS20M#0006</v>
+        <f>ON_Swaps!L28</f>
+        <v>USD_YCONRH_OIS20M#0000</v>
       </c>
       <c r="F57" s="13">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
@@ -5075,11 +5075,11 @@
       </c>
       <c r="K57" s="12">
         <f>_xll.qlRateHelperEarliestDate($E57,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L57" s="11">
         <f>_xll.qlRateHelperLatestDate($E57,Trigger)</f>
-        <v>42240</v>
+        <v>42263</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
@@ -5095,8 +5095,8 @@
         <v>33</v>
       </c>
       <c r="E58" s="14" t="str">
-        <f>'ON (3)'!L29</f>
-        <v>USD_YCONRH_OIS21M#0006</v>
+        <f>ON_Swaps!L29</f>
+        <v>USD_YCONRH_OIS21M#0000</v>
       </c>
       <c r="F58" s="13">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
@@ -5118,11 +5118,11 @@
       </c>
       <c r="K58" s="12">
         <f>_xll.qlRateHelperEarliestDate($E58,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L58" s="11">
         <f>_xll.qlRateHelperLatestDate($E58,Trigger)</f>
-        <v>42270</v>
+        <v>42293</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
@@ -5138,8 +5138,8 @@
         <v>48</v>
       </c>
       <c r="E59" s="14" t="str">
-        <f>'ON (3)'!L30</f>
-        <v>USD_YCONRH_OIS22M#0006</v>
+        <f>ON_Swaps!L30</f>
+        <v>USD_YCONRH_OIS22M#0000</v>
       </c>
       <c r="F59" s="13">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
@@ -5161,11 +5161,11 @@
       </c>
       <c r="K59" s="12">
         <f>_xll.qlRateHelperEarliestDate($E59,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L59" s="11">
         <f>_xll.qlRateHelperLatestDate($E59,Trigger)</f>
-        <v>42300</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.2">
@@ -5181,8 +5181,8 @@
         <v>47</v>
       </c>
       <c r="E60" s="14" t="str">
-        <f>'ON (3)'!L31</f>
-        <v>USD_YCONRH_OIS23M#0006</v>
+        <f>ON_Swaps!L31</f>
+        <v>USD_YCONRH_OIS23M#0000</v>
       </c>
       <c r="F60" s="13">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
@@ -5204,11 +5204,11 @@
       </c>
       <c r="K60" s="12">
         <f>_xll.qlRateHelperEarliestDate($E60,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L60" s="11">
         <f>_xll.qlRateHelperLatestDate($E60,Trigger)</f>
-        <v>42331</v>
+        <v>42354</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
@@ -5224,8 +5224,8 @@
         <v>32</v>
       </c>
       <c r="E61" s="14" t="str">
-        <f>'ON (3)'!L32</f>
-        <v>USD_YCONRH_OIS2Y#0006</v>
+        <f>ON_Swaps!L32</f>
+        <v>USD_YCONRH_OIS2Y#0000</v>
       </c>
       <c r="F61" s="13">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
@@ -5247,11 +5247,11 @@
       </c>
       <c r="K61" s="12">
         <f>_xll.qlRateHelperEarliestDate($E61,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L61" s="11">
         <f>_xll.qlRateHelperLatestDate($E61,Trigger)</f>
-        <v>42361</v>
+        <v>42387</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
@@ -5267,8 +5267,8 @@
         <v>46</v>
       </c>
       <c r="E62" s="14" t="str">
-        <f>'ON (3)'!L33</f>
-        <v>USD_YCONRH_OIS27M#0006</v>
+        <f>ON_Swaps!L33</f>
+        <v>USD_YCONRH_OIS27M#0000</v>
       </c>
       <c r="F62" s="13">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
@@ -5290,11 +5290,11 @@
       </c>
       <c r="K62" s="12">
         <f>_xll.qlRateHelperEarliestDate($E62,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L62" s="11">
         <f>_xll.qlRateHelperLatestDate($E62,Trigger)</f>
-        <v>42452</v>
+        <v>42478</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
@@ -5310,8 +5310,8 @@
         <v>45</v>
       </c>
       <c r="E63" s="14" t="str">
-        <f>'ON (3)'!L34</f>
-        <v>USD_YCONRH_OIS30M#0006</v>
+        <f>ON_Swaps!L34</f>
+        <v>USD_YCONRH_OIS30M#0000</v>
       </c>
       <c r="F63" s="13">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
@@ -5333,11 +5333,11 @@
       </c>
       <c r="K63" s="12">
         <f>_xll.qlRateHelperEarliestDate($E63,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L63" s="11">
         <f>_xll.qlRateHelperLatestDate($E63,Trigger)</f>
-        <v>42544</v>
+        <v>42569</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
@@ -5353,8 +5353,8 @@
         <v>44</v>
       </c>
       <c r="E64" s="14" t="str">
-        <f>'ON (3)'!L35</f>
-        <v>USD_YCONRH_OIS33M#0006</v>
+        <f>ON_Swaps!L35</f>
+        <v>USD_YCONRH_OIS33M#0000</v>
       </c>
       <c r="F64" s="13">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
@@ -5376,11 +5376,11 @@
       </c>
       <c r="K64" s="12">
         <f>_xll.qlRateHelperEarliestDate($E64,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L64" s="11">
         <f>_xll.qlRateHelperLatestDate($E64,Trigger)</f>
-        <v>42636</v>
+        <v>42660</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.2">
@@ -5396,8 +5396,8 @@
         <v>31</v>
       </c>
       <c r="E65" s="14" t="str">
-        <f>'ON (3)'!L36</f>
-        <v>USD_YCONRH_OIS3Y#0006</v>
+        <f>ON_Swaps!L36</f>
+        <v>USD_YCONRH_OIS3Y#0000</v>
       </c>
       <c r="F65" s="13">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
@@ -5418,11 +5418,11 @@
       </c>
       <c r="K65" s="12">
         <f>_xll.qlRateHelperEarliestDate($E65,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L65" s="11">
         <f>_xll.qlRateHelperLatestDate($E65,Trigger)</f>
-        <v>42727</v>
+        <v>42751</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
@@ -5438,8 +5438,8 @@
         <v>43</v>
       </c>
       <c r="E66" s="14" t="str">
-        <f>'ON (3)'!L37</f>
-        <v>USD_YCONRH_OIS39M#0006</v>
+        <f>ON_Swaps!L37</f>
+        <v>USD_YCONRH_OIS39M#0000</v>
       </c>
       <c r="F66" s="13">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
@@ -5460,11 +5460,11 @@
       </c>
       <c r="K66" s="12">
         <f>_xll.qlRateHelperEarliestDate($E66,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L66" s="11">
         <f>_xll.qlRateHelperLatestDate($E66,Trigger)</f>
-        <v>42817</v>
+        <v>42843</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
@@ -5480,8 +5480,8 @@
         <v>42</v>
       </c>
       <c r="E67" s="14" t="str">
-        <f>'ON (3)'!L38</f>
-        <v>USD_YCONRH_OIS42M#0006</v>
+        <f>ON_Swaps!L38</f>
+        <v>USD_YCONRH_OIS42M#0000</v>
       </c>
       <c r="F67" s="13">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
@@ -5502,11 +5502,11 @@
       </c>
       <c r="K67" s="12">
         <f>_xll.qlRateHelperEarliestDate($E67,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L67" s="11">
         <f>_xll.qlRateHelperLatestDate($E67,Trigger)</f>
-        <v>42909</v>
+        <v>42933</v>
       </c>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
@@ -5522,8 +5522,8 @@
         <v>41</v>
       </c>
       <c r="E68" s="14" t="str">
-        <f>'ON (3)'!L39</f>
-        <v>USD_YCONRH_OIS45M#0006</v>
+        <f>ON_Swaps!L39</f>
+        <v>USD_YCONRH_OIS45M#0000</v>
       </c>
       <c r="F68" s="13">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
@@ -5544,11 +5544,11 @@
       </c>
       <c r="K68" s="12">
         <f>_xll.qlRateHelperEarliestDate($E68,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L68" s="11">
         <f>_xll.qlRateHelperLatestDate($E68,Trigger)</f>
-        <v>43003</v>
+        <v>43024</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
@@ -5564,8 +5564,8 @@
         <v>30</v>
       </c>
       <c r="E69" s="14" t="str">
-        <f>'ON (3)'!L40</f>
-        <v>USD_YCONRH_OIS4Y#0006</v>
+        <f>ON_Swaps!L40</f>
+        <v>USD_YCONRH_OIS4Y#0000</v>
       </c>
       <c r="F69" s="13">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
@@ -5586,11 +5586,11 @@
       </c>
       <c r="K69" s="12">
         <f>_xll.qlRateHelperEarliestDate($E69,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L69" s="11">
         <f>_xll.qlRateHelperLatestDate($E69,Trigger)</f>
-        <v>43096</v>
+        <v>43116</v>
       </c>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
@@ -5606,8 +5606,8 @@
         <v>40</v>
       </c>
       <c r="E70" s="14" t="str">
-        <f>'ON (3)'!L41</f>
-        <v>USD_YCONRH_OIS51M#0006</v>
+        <f>ON_Swaps!L41</f>
+        <v>USD_YCONRH_OIS51M#0000</v>
       </c>
       <c r="F70" s="13">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
@@ -5628,11 +5628,11 @@
       </c>
       <c r="K70" s="12">
         <f>_xll.qlRateHelperEarliestDate($E70,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L70" s="11">
         <f>_xll.qlRateHelperLatestDate($E70,Trigger)</f>
-        <v>43182</v>
+        <v>43206</v>
       </c>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
@@ -5648,8 +5648,8 @@
         <v>39</v>
       </c>
       <c r="E71" s="14" t="str">
-        <f>'ON (3)'!L42</f>
-        <v>USD_YCONRH_OIS54M#0006</v>
+        <f>ON_Swaps!L42</f>
+        <v>USD_YCONRH_OIS54M#0000</v>
       </c>
       <c r="F71" s="13">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
@@ -5670,11 +5670,11 @@
       </c>
       <c r="K71" s="12">
         <f>_xll.qlRateHelperEarliestDate($E71,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L71" s="11">
         <f>_xll.qlRateHelperLatestDate($E71,Trigger)</f>
-        <v>43276</v>
+        <v>43297</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
@@ -5690,8 +5690,8 @@
         <v>38</v>
       </c>
       <c r="E72" s="14" t="str">
-        <f>'ON (3)'!L43</f>
-        <v>USD_YCONRH_OIS57M#0006</v>
+        <f>ON_Swaps!L43</f>
+        <v>USD_YCONRH_OIS57M#0000</v>
       </c>
       <c r="F72" s="13">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
@@ -5712,11 +5712,11 @@
       </c>
       <c r="K72" s="12">
         <f>_xll.qlRateHelperEarliestDate($E72,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L72" s="11">
         <f>_xll.qlRateHelperLatestDate($E72,Trigger)</f>
-        <v>43367</v>
+        <v>43389</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
@@ -5732,8 +5732,8 @@
         <v>29</v>
       </c>
       <c r="E73" s="14" t="str">
-        <f>'ON (3)'!L44</f>
-        <v>USD_YCONRH_OIS5Y#0006</v>
+        <f>ON_Swaps!L44</f>
+        <v>USD_YCONRH_OIS5Y#0000</v>
       </c>
       <c r="F73" s="13">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
@@ -5755,11 +5755,11 @@
       </c>
       <c r="K73" s="12">
         <f>_xll.qlRateHelperEarliestDate($E73,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L73" s="11">
         <f>_xll.qlRateHelperLatestDate($E73,Trigger)</f>
-        <v>43458</v>
+        <v>43481</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
@@ -5775,8 +5775,8 @@
         <v>28</v>
       </c>
       <c r="E74" s="14" t="str">
-        <f>'ON (3)'!L45</f>
-        <v>USD_YCONRH_OIS6Y#0006</v>
+        <f>ON_Swaps!L45</f>
+        <v>USD_YCONRH_OIS6Y#0000</v>
       </c>
       <c r="F74" s="13">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
@@ -5798,11 +5798,11 @@
       </c>
       <c r="K74" s="12">
         <f>_xll.qlRateHelperEarliestDate($E74,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L74" s="11">
         <f>_xll.qlRateHelperLatestDate($E74,Trigger)</f>
-        <v>43822</v>
+        <v>43846</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
@@ -5818,8 +5818,8 @@
         <v>27</v>
       </c>
       <c r="E75" s="14" t="str">
-        <f>'ON (3)'!L46</f>
-        <v>USD_YCONRH_OIS7Y#0006</v>
+        <f>ON_Swaps!L46</f>
+        <v>USD_YCONRH_OIS7Y#0000</v>
       </c>
       <c r="F75" s="13">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
@@ -5841,11 +5841,11 @@
       </c>
       <c r="K75" s="12">
         <f>_xll.qlRateHelperEarliestDate($E75,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L75" s="11">
         <f>_xll.qlRateHelperLatestDate($E75,Trigger)</f>
-        <v>44188</v>
+        <v>44214</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
@@ -5861,8 +5861,8 @@
         <v>26</v>
       </c>
       <c r="E76" s="14" t="str">
-        <f>'ON (3)'!L47</f>
-        <v>USD_YCONRH_OIS8Y#0006</v>
+        <f>ON_Swaps!L47</f>
+        <v>USD_YCONRH_OIS8Y#0000</v>
       </c>
       <c r="F76" s="13">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
@@ -5884,11 +5884,11 @@
       </c>
       <c r="K76" s="12">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L76" s="11">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>44553</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
@@ -5904,8 +5904,8 @@
         <v>25</v>
       </c>
       <c r="E77" s="14" t="str">
-        <f>'ON (3)'!L48</f>
-        <v>USD_YCONRH_OIS9Y#0006</v>
+        <f>ON_Swaps!L48</f>
+        <v>USD_YCONRH_OIS9Y#0000</v>
       </c>
       <c r="F77" s="13">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
@@ -5927,11 +5927,11 @@
       </c>
       <c r="K77" s="12">
         <f>_xll.qlRateHelperEarliestDate($E77,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L77" s="11">
         <f>_xll.qlRateHelperLatestDate($E77,Trigger)</f>
-        <v>44918</v>
+        <v>44942</v>
       </c>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.2">
@@ -5947,8 +5947,8 @@
         <v>24</v>
       </c>
       <c r="E78" s="14" t="str">
-        <f>'ON (3)'!L49</f>
-        <v>USD_YCONRH_OIS10Y#0006</v>
+        <f>ON_Swaps!L49</f>
+        <v>USD_YCONRH_OIS10Y#0000</v>
       </c>
       <c r="F78" s="13">
         <f>_xll.qlRateHelperQuoteValue($E78,Trigger)</f>
@@ -5970,11 +5970,11 @@
       </c>
       <c r="K78" s="12">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L78" s="11">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>45287</v>
+        <v>45307</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
@@ -5990,8 +5990,8 @@
         <v>22</v>
       </c>
       <c r="E79" s="14" t="str">
-        <f>'ON (3)'!L50</f>
-        <v>USD_YCONRH_OIS12Y#0006</v>
+        <f>ON_Swaps!L50</f>
+        <v>USD_YCONRH_OIS12Y#0000</v>
       </c>
       <c r="F79" s="13">
         <f>_xll.qlRateHelperQuoteValue($E79,Trigger)</f>
@@ -6013,11 +6013,11 @@
       </c>
       <c r="K79" s="12">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L79" s="11">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>46014</v>
+        <v>46038</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
@@ -6033,8 +6033,8 @@
         <v>19</v>
       </c>
       <c r="E80" s="14" t="str">
-        <f>'ON (3)'!L51</f>
-        <v>USD_YCONRH_OIS15Y#0006</v>
+        <f>ON_Swaps!L51</f>
+        <v>USD_YCONRH_OIS15Y#0000</v>
       </c>
       <c r="F80" s="13">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
@@ -6056,11 +6056,11 @@
       </c>
       <c r="K80" s="12">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L80" s="11">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
-        <v>47114</v>
+        <v>47134</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.2">
@@ -6073,8 +6073,8 @@
         <v>14</v>
       </c>
       <c r="E81" s="14" t="str">
-        <f>'ON (3)'!L52</f>
-        <v>USD_YCONRH_OIS20Y#0006</v>
+        <f>ON_Swaps!L52</f>
+        <v>USD_YCONRH_OIS20Y#0000</v>
       </c>
       <c r="F81" s="13">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
@@ -6096,11 +6096,11 @@
       </c>
       <c r="K81" s="12">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L81" s="11">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
-        <v>48936</v>
+        <v>48960</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.2">
@@ -6113,8 +6113,8 @@
         <v>9</v>
       </c>
       <c r="E82" s="14" t="str">
-        <f>'ON (3)'!L53</f>
-        <v>USD_YCONRH_OIS25Y#0006</v>
+        <f>ON_Swaps!L53</f>
+        <v>USD_YCONRH_OIS25Y#0000</v>
       </c>
       <c r="F82" s="13">
         <f>_xll.qlRateHelperQuoteValue($E82,Trigger)</f>
@@ -6135,11 +6135,11 @@
       </c>
       <c r="K82" s="12">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L82" s="11">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>50762</v>
+        <v>50787</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
@@ -6152,8 +6152,8 @@
         <v>7</v>
       </c>
       <c r="E83" s="14" t="str">
-        <f>'ON (3)'!L54</f>
-        <v>USD_YCONRH_OIS27Y#0006</v>
+        <f>ON_Swaps!L54</f>
+        <v>USD_YCONRH_OIS27Y#0000</v>
       </c>
       <c r="F83" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
@@ -6175,11 +6175,11 @@
       </c>
       <c r="K83" s="12">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L83" s="11">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>51494</v>
+        <v>51517</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
@@ -6195,8 +6195,8 @@
         <v>4</v>
       </c>
       <c r="E84" s="14" t="str">
-        <f>'ON (3)'!L55</f>
-        <v>USD_YCONRH_OIS30Y#0006</v>
+        <f>ON_Swaps!L55</f>
+        <v>USD_YCONRH_OIS30Y#0000</v>
       </c>
       <c r="F84" s="13">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
@@ -6218,11 +6218,11 @@
       </c>
       <c r="K84" s="12">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L84" s="11">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>52588</v>
+        <v>52614</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
@@ -6238,8 +6238,8 @@
         <v>3</v>
       </c>
       <c r="E85" s="14" t="str">
-        <f>'ON (3)'!L56</f>
-        <v>USD_YCONRH_OIS35Y#0006</v>
+        <f>ON_Swaps!L56</f>
+        <v>USD_YCONRH_OIS35Y#0000</v>
       </c>
       <c r="F85" s="13">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
@@ -6261,11 +6261,11 @@
       </c>
       <c r="K85" s="12">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L85" s="11">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>54415</v>
+        <v>54441</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
@@ -6281,8 +6281,8 @@
         <v>2</v>
       </c>
       <c r="E86" s="14" t="str">
-        <f>'ON (3)'!L57</f>
-        <v>USD_YCONRH_OIS40Y#0006</v>
+        <f>ON_Swaps!L57</f>
+        <v>USD_YCONRH_OIS40Y#0000</v>
       </c>
       <c r="F86" s="13">
         <f>_xll.qlRateHelperQuoteValue($E86,Trigger)</f>
@@ -6304,11 +6304,11 @@
       </c>
       <c r="K86" s="12">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L86" s="11">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>56241</v>
+        <v>56265</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
@@ -6324,8 +6324,8 @@
         <v>37</v>
       </c>
       <c r="E87" s="14" t="str">
-        <f>'ON (3)'!L58</f>
-        <v>USD_YCONRH_OIS45Y#0006</v>
+        <f>ON_Swaps!L58</f>
+        <v>USD_YCONRH_OIS45Y#0000</v>
       </c>
       <c r="F87" s="13">
         <f>_xll.qlRateHelperQuoteValue($E87,Trigger)</f>
@@ -6347,11 +6347,11 @@
       </c>
       <c r="K87" s="12">
         <f>_xll.qlRateHelperEarliestDate($E87,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L87" s="11">
         <f>_xll.qlRateHelperLatestDate($E87,Trigger)</f>
-        <v>58067</v>
+        <v>58091</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
@@ -6367,8 +6367,8 @@
         <v>1</v>
       </c>
       <c r="E88" s="8" t="str">
-        <f>'ON (3)'!L59</f>
-        <v>USD_YCONRH_OIS50Y#0006</v>
+        <f>ON_Swaps!L59</f>
+        <v>USD_YCONRH_OIS50Y#0000</v>
       </c>
       <c r="F88" s="7">
         <f>_xll.qlRateHelperQuoteValue($E88,Trigger)</f>
@@ -6390,11 +6390,11 @@
       </c>
       <c r="K88" s="4">
         <f>_xll.qlRateHelperEarliestDate($E88,Trigger)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="L88" s="3">
         <f>_xll.qlRateHelperLatestDate($E88,Trigger)</f>
-        <v>59894</v>
+        <v>59917</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
@@ -8026,10 +8026,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="185" t="s">
+      <c r="A1" s="197" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="186"/>
+      <c r="B1" s="198"/>
       <c r="D1" s="52" t="s">
         <v>105</v>
       </c>
@@ -8069,11 +8069,11 @@
       </c>
       <c r="G2" s="39">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41627</v>
+        <v>41653</v>
       </c>
       <c r="H2" s="38">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41628</v>
+        <v>41654</v>
       </c>
       <c r="I2" s="33">
         <v>0.9999955555753085</v>
@@ -8105,18 +8105,18 @@
       </c>
       <c r="G3" s="39">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41628</v>
+        <v>41654</v>
       </c>
       <c r="H3" s="38">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="I3" s="33">
-        <v>0.99998222247899815</v>
+        <v>0.99999111117036987</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J37" si="0">H3-H2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L3" s="179" t="s">
         <v>174</v>
@@ -8145,14 +8145,14 @@
       </c>
       <c r="G4" s="39">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H4" s="38">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41638</v>
+        <v>41662</v>
       </c>
       <c r="I4" s="33">
-        <v>0.9999647230963441</v>
+        <v>0.99997361163216636</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
@@ -8185,14 +8185,14 @@
       </c>
       <c r="G5" s="39">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H5" s="38">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41645</v>
+        <v>41669</v>
       </c>
       <c r="I5" s="33">
-        <v>0.99994877974758656</v>
+        <v>0.99995766814159714</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
@@ -8226,14 +8226,14 @@
       </c>
       <c r="G6" s="39">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H6" s="38">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41652</v>
+        <v>41676</v>
       </c>
       <c r="I6" s="33">
-        <v>0.9999326424852516</v>
+        <v>0.99994153073624759</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
@@ -8249,7 +8249,7 @@
     <row r="7" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="43" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_RateHelpersSelected#0006</v>
+        <v>USD_YCONRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="42" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -8268,18 +8268,18 @@
       </c>
       <c r="G7" s="39">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H7" s="38">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41662</v>
+        <v>41687</v>
       </c>
       <c r="I7" s="33">
-        <v>0.99990989566320054</v>
+        <v>0.9999164507418018</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L7" s="179" t="s">
         <v>178</v>
@@ -8302,18 +8302,18 @@
       </c>
       <c r="G8" s="39">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H8" s="38">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
-        <v>41694</v>
+        <v>41715</v>
       </c>
       <c r="I8" s="33">
-        <v>0.9998352466977336</v>
+        <v>0.99985113201188813</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L8" s="179" t="s">
         <v>179</v>
@@ -8336,18 +8336,18 @@
       </c>
       <c r="G9" s="39">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H9" s="38">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41722</v>
+        <v>41745</v>
       </c>
       <c r="I9" s="33">
-        <v>0.99976993799549718</v>
+        <v>0.99978115712723314</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L9" s="179" t="s">
         <v>180</v>
@@ -8370,14 +8370,14 @@
       </c>
       <c r="G10" s="39">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H10" s="38">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41752</v>
+        <v>41775</v>
       </c>
       <c r="I10" s="33">
-        <v>0.99968653741648683</v>
+        <v>0.99969786646287406</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="0"/>
@@ -8404,18 +8404,18 @@
       </c>
       <c r="G11" s="39">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H11" s="38">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41782</v>
+        <v>41806</v>
       </c>
       <c r="I11" s="33">
-        <v>0.99960487164019596</v>
+        <v>0.99961375697725363</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L11" s="179" t="s">
         <v>182</v>
@@ -8438,18 +8438,18 @@
       </c>
       <c r="G12" s="39">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H12" s="38">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41813</v>
+        <v>41836</v>
       </c>
       <c r="I12" s="33">
-        <v>0.9995122851196111</v>
+        <v>0.99952375052335429</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="179" t="s">
         <v>183</v>
@@ -8472,18 +8472,18 @@
       </c>
       <c r="G13" s="39">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H13" s="38">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
-        <v>41843</v>
+        <v>41869</v>
       </c>
       <c r="I13" s="33">
-        <v>0.99941133651444025</v>
+        <v>0.9994148374704751</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L13" s="179" t="s">
         <v>184</v>
@@ -8506,18 +8506,18 @@
       </c>
       <c r="G14" s="39">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H14" s="38">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>41876</v>
+        <v>41898</v>
       </c>
       <c r="I14" s="33">
-        <v>0.99930214185468036</v>
+        <v>0.99931657248394312</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L14" s="179" t="s">
         <v>185</v>
@@ -8540,18 +8540,18 @@
       </c>
       <c r="G15" s="39">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H15" s="38">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>41905</v>
+        <v>41928</v>
       </c>
       <c r="I15" s="33">
-        <v>0.9991837081655558</v>
+        <v>0.9991955017520997</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L15" s="179" t="s">
         <v>186</v>
@@ -8574,18 +8574,18 @@
       </c>
       <c r="G16" s="39">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H16" s="38">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>41935</v>
+        <v>41960</v>
       </c>
       <c r="I16" s="33">
-        <v>0.9990626408216019</v>
+        <v>0.99906849916329532</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L16" s="179" t="s">
         <v>187</v>
@@ -8608,18 +8608,18 @@
       </c>
       <c r="G17" s="39">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H17" s="38">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>41967</v>
+        <v>41989</v>
       </c>
       <c r="I17" s="33">
-        <v>0.9989193722669063</v>
+        <v>0.99893457137204866</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L17" s="179" t="s">
         <v>188</v>
@@ -8642,18 +8642,18 @@
       </c>
       <c r="G18" s="39">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H18" s="38">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>41996</v>
+        <v>42020</v>
       </c>
       <c r="I18" s="33">
-        <v>0.99877717007948696</v>
+        <v>0.99878604805932936</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L18" s="179" t="s">
         <v>189</v>
@@ -8676,14 +8676,14 @@
       </c>
       <c r="G19" s="39">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H19" s="38">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42027</v>
+        <v>42051</v>
       </c>
       <c r="I19" s="33">
-        <v>0.99861990721117977</v>
+        <v>0.99862878379313613</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="0"/>
@@ -8710,18 +8710,18 @@
       </c>
       <c r="G20" s="39">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H20" s="38">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>42058</v>
+        <v>42079</v>
       </c>
       <c r="I20" s="33">
-        <v>0.99845408195668661</v>
+        <v>0.99847368827269933</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L20" s="179" t="s">
         <v>191</v>
@@ -8744,18 +8744,18 @@
       </c>
       <c r="G21" s="39">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H21" s="38">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>42086</v>
+        <v>42110</v>
       </c>
       <c r="I21" s="33">
-        <v>0.99826560942966769</v>
+        <v>0.99827448286225307</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L21" s="179" t="s">
         <v>192</v>
@@ -8778,18 +8778,18 @@
       </c>
       <c r="G22" s="39">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H22" s="38">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>42117</v>
+        <v>42142</v>
       </c>
       <c r="I22" s="33">
-        <v>0.9980544305288942</v>
+        <v>0.99805933947551029</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L22" s="179" t="s">
         <v>193</v>
@@ -8812,18 +8812,18 @@
       </c>
       <c r="G23" s="39">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H23" s="38">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>42149</v>
+        <v>42171</v>
       </c>
       <c r="I23" s="33">
-        <v>0.99782713406820045</v>
+        <v>0.99784431367492565</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L23" s="179" t="s">
         <v>194</v>
@@ -8846,18 +8846,18 @@
       </c>
       <c r="G24" s="39">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H24" s="38">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>42178</v>
+        <v>42201</v>
       </c>
       <c r="I24" s="33">
-        <v>0.99758538790086038</v>
+        <v>0.9975986301421369</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L24" s="179" t="s">
         <v>195</v>
@@ -8880,18 +8880,18 @@
       </c>
       <c r="G25" s="39">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H25" s="38">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
-        <v>42208</v>
+        <v>42233</v>
       </c>
       <c r="I25" s="33">
-        <v>0.99731029925019687</v>
+        <v>0.99731454230526428</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L25" s="179" t="s">
         <v>196</v>
@@ -8914,18 +8914,18 @@
       </c>
       <c r="G26" s="39">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H26" s="38">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>42240</v>
+        <v>42263</v>
       </c>
       <c r="I26" s="33">
-        <v>0.99699377341901463</v>
+        <v>0.99700753162654587</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L26" s="179" t="s">
         <v>197</v>
@@ -8948,14 +8948,14 @@
       </c>
       <c r="G27" s="39">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H27" s="38">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>42270</v>
+        <v>42293</v>
       </c>
       <c r="I27" s="33">
-        <v>0.99667003040228908</v>
+        <v>0.9966840595139107</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="0"/>
@@ -8982,18 +8982,18 @@
       </c>
       <c r="G28" s="39">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H28" s="38">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>42300</v>
+        <v>42324</v>
       </c>
       <c r="I28" s="33">
-        <v>0.99631134474165561</v>
+        <v>0.99632020080314798</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L28" s="179" t="s">
         <v>199</v>
@@ -9016,18 +9016,18 @@
       </c>
       <c r="G29" s="39">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H29" s="38">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>42331</v>
+        <v>42354</v>
       </c>
       <c r="I29" s="33">
-        <v>0.99590948629989307</v>
+        <v>0.99592413701609062</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L29" s="179" t="s">
         <v>200</v>
@@ -9050,18 +9050,18 @@
       </c>
       <c r="G30" s="39">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H30" s="38">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>42361</v>
+        <v>42387</v>
       </c>
       <c r="I30" s="33">
-        <v>0.99547327761261239</v>
+        <v>0.99546982128078054</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="L30" s="179" t="s">
         <v>201</v>
@@ -9084,14 +9084,14 @@
       </c>
       <c r="G31" s="39">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H31" s="38">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
-        <v>42452</v>
+        <v>42478</v>
       </c>
       <c r="I31" s="33">
-        <v>0.99393552860755652</v>
+        <v>0.99392969576717849</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="0"/>
@@ -9118,18 +9118,18 @@
       </c>
       <c r="G32" s="39">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H32" s="38">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
-        <v>42544</v>
+        <v>42569</v>
       </c>
       <c r="I32" s="33">
-        <v>0.99192372020424557</v>
+        <v>0.99192373893904673</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L32" s="179" t="s">
         <v>203</v>
@@ -9152,18 +9152,18 @@
       </c>
       <c r="G33" s="39">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H33" s="38">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>42636</v>
+        <v>42660</v>
       </c>
       <c r="I33" s="33">
-        <v>0.98939903574357235</v>
+        <v>0.98940774981613588</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L33" s="179" t="s">
         <v>204</v>
@@ -9186,14 +9186,14 @@
       </c>
       <c r="G34" s="39">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H34" s="38">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>42727</v>
+        <v>42751</v>
       </c>
       <c r="I34" s="33">
-        <v>0.98634069883332964</v>
+        <v>0.98634929479965516</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
@@ -9220,18 +9220,18 @@
       </c>
       <c r="G35" s="39">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H35" s="38">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>43096</v>
+        <v>43116</v>
       </c>
       <c r="I35" s="33">
-        <v>0.96868488409925069</v>
+        <v>0.96877638950546374</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="0"/>
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="L35" s="179" t="s">
         <v>206</v>
@@ -9254,18 +9254,18 @@
       </c>
       <c r="G36" s="39">
         <f>_xll.qlRateHelperEarliestDate($D36)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H36" s="38">
         <f>_xll.qlRateHelperLatestDate($D36)</f>
-        <v>43458</v>
+        <v>43481</v>
       </c>
       <c r="I36" s="33">
-        <v>0.94410371076925725</v>
+        <v>0.94414295380885427</v>
       </c>
       <c r="J36" s="1">
         <f t="shared" si="0"/>
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="L36" s="179" t="s">
         <v>207</v>
@@ -9288,18 +9288,18 @@
       </c>
       <c r="G37" s="39">
         <f>_xll.qlRateHelperEarliestDate($D37)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H37" s="38">
         <f>_xll.qlRateHelperLatestDate($D37)</f>
-        <v>43822</v>
+        <v>43846</v>
       </c>
       <c r="I37" s="33">
-        <v>0.91513338539911859</v>
+        <v>0.91514436206153138</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="0"/>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L37" s="179" t="s">
         <v>208</v>
@@ -9322,14 +9322,14 @@
       </c>
       <c r="G38" s="39">
         <f>_xll.qlRateHelperEarliestDate($D38)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H38" s="38">
         <f>_xll.qlRateHelperLatestDate($D38)</f>
-        <v>44188</v>
+        <v>44214</v>
       </c>
       <c r="I38" s="33">
-        <v>0.88365811218332935</v>
+        <v>0.88358664139440379</v>
       </c>
       <c r="L38" s="179" t="s">
         <v>209</v>
@@ -9352,14 +9352,14 @@
       </c>
       <c r="G39" s="39">
         <f>_xll.qlRateHelperEarliestDate($D39)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H39" s="38">
         <f>_xll.qlRateHelperLatestDate($D39)</f>
-        <v>44553</v>
+        <v>44578</v>
       </c>
       <c r="I39" s="33">
-        <v>0.85126968557896621</v>
+        <v>0.85123406975534666</v>
       </c>
       <c r="L39" s="179" t="s">
         <v>210</v>
@@ -9382,14 +9382,14 @@
       </c>
       <c r="G40" s="39">
         <f>_xll.qlRateHelperEarliestDate($D40)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H40" s="38">
         <f>_xll.qlRateHelperLatestDate($D40)</f>
-        <v>44918</v>
+        <v>44942</v>
       </c>
       <c r="I40" s="33">
-        <v>0.81876618442168947</v>
+        <v>0.81877454743137246</v>
       </c>
       <c r="L40" s="179" t="s">
         <v>211</v>
@@ -9412,14 +9412,14 @@
       </c>
       <c r="G41" s="39">
         <f>_xll.qlRateHelperEarliestDate($D41)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H41" s="38">
         <f>_xll.qlRateHelperLatestDate($D41)</f>
-        <v>45287</v>
+        <v>45307</v>
       </c>
       <c r="I41" s="33">
-        <v>0.78613369787816501</v>
+        <v>0.78633831974700852</v>
       </c>
       <c r="L41" s="179" t="s">
         <v>212</v>
@@ -9442,14 +9442,14 @@
       </c>
       <c r="G42" s="39">
         <f>_xll.qlRateHelperEarliestDate($D42)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H42" s="38">
         <f>_xll.qlRateHelperLatestDate($D42)</f>
-        <v>46014</v>
+        <v>46038</v>
       </c>
       <c r="I42" s="33">
-        <v>0.72218920785326379</v>
+        <v>0.72220291732629871</v>
       </c>
       <c r="L42" s="179" t="s">
         <v>213</v>
@@ -9472,14 +9472,14 @@
       </c>
       <c r="G43" s="39">
         <f>_xll.qlRateHelperEarliestDate($D43)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H43" s="38">
         <f>_xll.qlRateHelperLatestDate($D43)</f>
-        <v>47114</v>
+        <v>47134</v>
       </c>
       <c r="I43" s="33">
-        <v>0.63633326708315707</v>
+        <v>0.63654437091187077</v>
       </c>
       <c r="L43" s="179" t="s">
         <v>214</v>
@@ -9502,14 +9502,14 @@
       </c>
       <c r="G44" s="39">
         <f>_xll.qlRateHelperEarliestDate($D44)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H44" s="38">
         <f>_xll.qlRateHelperLatestDate($D44)</f>
-        <v>48936</v>
+        <v>48960</v>
       </c>
       <c r="I44" s="33">
-        <v>0.51981190212580974</v>
+        <v>0.51983295988516209</v>
       </c>
       <c r="L44" s="179" t="s">
         <v>215</v>
@@ -9532,14 +9532,14 @@
       </c>
       <c r="G45" s="39">
         <f>_xll.qlRateHelperEarliestDate($D45)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H45" s="38">
         <f>_xll.qlRateHelperLatestDate($D45)</f>
-        <v>50762</v>
+        <v>50787</v>
       </c>
       <c r="I45" s="33">
-        <v>0.42715385408353196</v>
+        <v>0.42713494873619162</v>
       </c>
       <c r="L45" s="179" t="s">
         <v>216</v>
@@ -9562,14 +9562,14 @@
       </c>
       <c r="G46" s="39">
         <f>_xll.qlRateHelperEarliestDate($D46)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H46" s="38">
         <f>_xll.qlRateHelperLatestDate($D46)</f>
-        <v>52588</v>
+        <v>52614</v>
       </c>
       <c r="I46" s="33">
-        <v>0.35268078633895616</v>
+        <v>0.35263290293667265</v>
       </c>
       <c r="L46" s="179" t="s">
         <v>217</v>
@@ -9592,14 +9592,14 @@
       </c>
       <c r="G47" s="39">
         <f>_xll.qlRateHelperEarliestDate($D47)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H47" s="38">
         <f>_xll.qlRateHelperLatestDate($D47)</f>
-        <v>54415</v>
+        <v>54441</v>
       </c>
       <c r="I47" s="33">
-        <v>0.29640805123074765</v>
+        <v>0.29636685104324823</v>
       </c>
       <c r="L47" s="179" t="s">
         <v>218</v>
@@ -9622,14 +9622,14 @@
       </c>
       <c r="G48" s="39">
         <f>_xll.qlRateHelperEarliestDate($D48)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H48" s="38">
         <f>_xll.qlRateHelperLatestDate($D48)</f>
-        <v>56241</v>
+        <v>56265</v>
       </c>
       <c r="I48" s="33">
-        <v>0.25166175637453525</v>
+        <v>0.25167081466775604</v>
       </c>
       <c r="L48" s="179" t="s">
         <v>219</v>
@@ -9652,14 +9652,14 @@
       </c>
       <c r="G49" s="39">
         <f>_xll.qlRateHelperEarliestDate($D49)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H49" s="38">
         <f>_xll.qlRateHelperLatestDate($D49)</f>
-        <v>58067</v>
+        <v>58091</v>
       </c>
       <c r="I49" s="33">
-        <v>0.21580083775898115</v>
+        <v>0.21580849836211913</v>
       </c>
       <c r="L49" s="179" t="s">
         <v>220</v>
@@ -9682,14 +9682,14 @@
       </c>
       <c r="G50" s="39">
         <f>_xll.qlRateHelperEarliestDate($D50)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="H50" s="38">
         <f>_xll.qlRateHelperLatestDate($D50)</f>
-        <v>59894</v>
+        <v>59917</v>
       </c>
       <c r="I50" s="33">
-        <v>0.18593203137578257</v>
+        <v>0.18595467193896159</v>
       </c>
       <c r="L50" s="179" t="s">
         <v>221</v>
@@ -11616,7 +11616,7 @@
       </c>
       <c r="F3" s="105" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OND#0006</v>
+        <v>USD_YCONRH_OND#0000</v>
       </c>
       <c r="G3" s="104" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -11730,7 +11730,7 @@
       </c>
       <c r="H3" s="146" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_TND#0005</v>
+        <v>USD_YCONRH_TND#0000</v>
       </c>
       <c r="I3" s="145" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -11762,7 +11762,7 @@
       </c>
       <c r="H4" s="143" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_SND#0005</v>
+        <v>USD_YCONRH_SND#0000</v>
       </c>
       <c r="I4" s="142" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -11918,7 +11918,7 @@
       </c>
       <c r="L4" s="172" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS_LiborON#0006</v>
+        <v>USD_YCONRH_OIS_LiborON#0000</v>
       </c>
       <c r="M4" s="171" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -11977,7 +11977,7 @@
       </c>
       <c r="L6" s="164" t="str">
         <f>_xll.qlOISRateHelper(K6,2,C6,J6,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OISSW#0006</v>
+        <v>USD_YCONRH_OISSW#0000</v>
       </c>
       <c r="M6" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -11986,11 +11986,11 @@
       <c r="N6" s="161"/>
       <c r="P6" s="163">
         <f>_xll.qlRateHelperEarliestDate($L6)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q6" s="163">
         <f>_xll.qlRateHelperLatestDate($L6)</f>
-        <v>41638</v>
+        <v>41662</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -12029,7 +12029,7 @@
       </c>
       <c r="L7" s="164" t="str">
         <f>_xll.qlOISRateHelper(K7,2,C7,J7,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2W#0006</v>
+        <v>USD_YCONRH_OIS2W#0000</v>
       </c>
       <c r="M7" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -12038,11 +12038,11 @@
       <c r="N7" s="161"/>
       <c r="P7" s="163">
         <f>_xll.qlRateHelperEarliestDate(L7)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q7" s="163">
         <f>_xll.qlRateHelperLatestDate($L7)</f>
-        <v>41645</v>
+        <v>41669</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -12081,7 +12081,7 @@
       </c>
       <c r="L8" s="164" t="str">
         <f>_xll.qlOISRateHelper(K8,2,C8,J8,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3W#0006</v>
+        <v>USD_YCONRH_OIS3W#0000</v>
       </c>
       <c r="M8" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -12090,11 +12090,11 @@
       <c r="N8" s="161"/>
       <c r="P8" s="163">
         <f>_xll.qlRateHelperEarliestDate(L8)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q8" s="163">
         <f>_xll.qlRateHelperLatestDate($L8)</f>
-        <v>41652</v>
+        <v>41676</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -12133,7 +12133,7 @@
       </c>
       <c r="L9" s="164" t="str">
         <f>_xll.qlOISRateHelper(K9,2,C9,J9,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS1M#0006</v>
+        <v>USD_YCONRH_OIS1M#0000</v>
       </c>
       <c r="M9" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -12142,11 +12142,11 @@
       <c r="N9" s="161"/>
       <c r="P9" s="163">
         <f>_xll.qlRateHelperEarliestDate(L9)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q9" s="163">
         <f>_xll.qlRateHelperLatestDate($L9)</f>
-        <v>41662</v>
+        <v>41687</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -12185,7 +12185,7 @@
       </c>
       <c r="L10" s="164" t="str">
         <f>_xll.qlOISRateHelper(K10,2,C10,J10,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2M#0006</v>
+        <v>USD_YCONRH_OIS2M#0000</v>
       </c>
       <c r="M10" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -12194,11 +12194,11 @@
       <c r="N10" s="161"/>
       <c r="P10" s="163">
         <f>_xll.qlRateHelperEarliestDate(L10)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q10" s="163">
         <f>_xll.qlRateHelperLatestDate($L10)</f>
-        <v>41694</v>
+        <v>41715</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -12237,7 +12237,7 @@
       </c>
       <c r="L11" s="164" t="str">
         <f>_xll.qlOISRateHelper(K11,2,C11,J11,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3M#0006</v>
+        <v>USD_YCONRH_OIS3M#0000</v>
       </c>
       <c r="M11" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -12246,11 +12246,11 @@
       <c r="N11" s="161"/>
       <c r="P11" s="163">
         <f>_xll.qlRateHelperEarliestDate(L11)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q11" s="163">
         <f>_xll.qlRateHelperLatestDate($L11)</f>
-        <v>41722</v>
+        <v>41745</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -12289,7 +12289,7 @@
       </c>
       <c r="L12" s="164" t="str">
         <f>_xll.qlOISRateHelper(K12,2,C12,J12,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS4M#0006</v>
+        <v>USD_YCONRH_OIS4M#0000</v>
       </c>
       <c r="M12" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -12298,11 +12298,11 @@
       <c r="N12" s="161"/>
       <c r="P12" s="163">
         <f>_xll.qlRateHelperEarliestDate(L12)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q12" s="163">
         <f>_xll.qlRateHelperLatestDate($L12)</f>
-        <v>41752</v>
+        <v>41775</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -12341,7 +12341,7 @@
       </c>
       <c r="L13" s="164" t="str">
         <f>_xll.qlOISRateHelper(K13,2,C13,J13,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS5M#0006</v>
+        <v>USD_YCONRH_OIS5M#0000</v>
       </c>
       <c r="M13" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -12350,11 +12350,11 @@
       <c r="N13" s="161"/>
       <c r="P13" s="163">
         <f>_xll.qlRateHelperEarliestDate(L13)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q13" s="163">
         <f>_xll.qlRateHelperLatestDate($L13)</f>
-        <v>41782</v>
+        <v>41806</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -12393,7 +12393,7 @@
       </c>
       <c r="L14" s="164" t="str">
         <f>_xll.qlOISRateHelper(K14,2,C14,J14,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS6M#0006</v>
+        <v>USD_YCONRH_OIS6M#0000</v>
       </c>
       <c r="M14" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -12402,11 +12402,11 @@
       <c r="N14" s="161"/>
       <c r="P14" s="163">
         <f>_xll.qlRateHelperEarliestDate(L14)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q14" s="163">
         <f>_xll.qlRateHelperLatestDate($L14)</f>
-        <v>41813</v>
+        <v>41836</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -12445,7 +12445,7 @@
       </c>
       <c r="L15" s="164" t="str">
         <f>_xll.qlOISRateHelper(K15,2,C15,J15,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS7M#0006</v>
+        <v>USD_YCONRH_OIS7M#0000</v>
       </c>
       <c r="M15" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -12454,11 +12454,11 @@
       <c r="N15" s="161"/>
       <c r="P15" s="163">
         <f>_xll.qlRateHelperEarliestDate(L15)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q15" s="163">
         <f>_xll.qlRateHelperLatestDate($L15)</f>
-        <v>41843</v>
+        <v>41869</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -12497,7 +12497,7 @@
       </c>
       <c r="L16" s="164" t="str">
         <f>_xll.qlOISRateHelper(K16,2,C16,J16,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS8M#0006</v>
+        <v>USD_YCONRH_OIS8M#0000</v>
       </c>
       <c r="M16" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -12506,11 +12506,11 @@
       <c r="N16" s="161"/>
       <c r="P16" s="163">
         <f>_xll.qlRateHelperEarliestDate(L16)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q16" s="163">
         <f>_xll.qlRateHelperLatestDate($L16)</f>
-        <v>41876</v>
+        <v>41898</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -12549,7 +12549,7 @@
       </c>
       <c r="L17" s="164" t="str">
         <f>_xll.qlOISRateHelper(K17,2,C17,J17,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS9M#0006</v>
+        <v>USD_YCONRH_OIS9M#0000</v>
       </c>
       <c r="M17" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -12558,11 +12558,11 @@
       <c r="N17" s="161"/>
       <c r="P17" s="163">
         <f>_xll.qlRateHelperEarliestDate(L17)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q17" s="163">
         <f>_xll.qlRateHelperLatestDate($L17)</f>
-        <v>41905</v>
+        <v>41928</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -12601,7 +12601,7 @@
       </c>
       <c r="L18" s="164" t="str">
         <f>_xll.qlOISRateHelper(K18,2,C18,J18,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS10M#0006</v>
+        <v>USD_YCONRH_OIS10M#0000</v>
       </c>
       <c r="M18" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -12610,11 +12610,11 @@
       <c r="N18" s="161"/>
       <c r="P18" s="163">
         <f>_xll.qlRateHelperEarliestDate(L18)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q18" s="163">
         <f>_xll.qlRateHelperLatestDate($L18)</f>
-        <v>41935</v>
+        <v>41960</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -12653,7 +12653,7 @@
       </c>
       <c r="L19" s="164" t="str">
         <f>_xll.qlOISRateHelper(K19,2,C19,J19,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS11M#0006</v>
+        <v>USD_YCONRH_OIS11M#0000</v>
       </c>
       <c r="M19" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -12662,11 +12662,11 @@
       <c r="N19" s="161"/>
       <c r="P19" s="163">
         <f>_xll.qlRateHelperEarliestDate(L19)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q19" s="163">
         <f>_xll.qlRateHelperLatestDate($L19)</f>
-        <v>41967</v>
+        <v>41989</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -12705,7 +12705,7 @@
       </c>
       <c r="L20" s="164" t="str">
         <f>_xll.qlOISRateHelper(K20,2,C20,J20,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS1Y#0006</v>
+        <v>USD_YCONRH_OIS1Y#0000</v>
       </c>
       <c r="M20" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -12714,11 +12714,11 @@
       <c r="N20" s="161"/>
       <c r="P20" s="163">
         <f>_xll.qlRateHelperEarliestDate(L20)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q20" s="163">
         <f>_xll.qlRateHelperLatestDate($L20)</f>
-        <v>41996</v>
+        <v>42020</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -12757,7 +12757,7 @@
       </c>
       <c r="L21" s="164" t="str">
         <f>_xll.qlOISRateHelper(K21,2,C21,J21,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS13M#0006</v>
+        <v>USD_YCONRH_OIS13M#0000</v>
       </c>
       <c r="M21" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -12766,11 +12766,11 @@
       <c r="N21" s="161"/>
       <c r="P21" s="163">
         <f>_xll.qlRateHelperEarliestDate(L21)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q21" s="163">
         <f>_xll.qlRateHelperLatestDate($L21)</f>
-        <v>42027</v>
+        <v>42051</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -12809,7 +12809,7 @@
       </c>
       <c r="L22" s="164" t="str">
         <f>_xll.qlOISRateHelper(K22,2,C22,J22,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS14M#0006</v>
+        <v>USD_YCONRH_OIS14M#0000</v>
       </c>
       <c r="M22" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -12818,11 +12818,11 @@
       <c r="N22" s="161"/>
       <c r="P22" s="163">
         <f>_xll.qlRateHelperEarliestDate(L22)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q22" s="163">
         <f>_xll.qlRateHelperLatestDate($L22)</f>
-        <v>42058</v>
+        <v>42079</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -12861,7 +12861,7 @@
       </c>
       <c r="L23" s="164" t="str">
         <f>_xll.qlOISRateHelper(K23,2,C23,J23,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS15M#0006</v>
+        <v>USD_YCONRH_OIS15M#0000</v>
       </c>
       <c r="M23" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -12870,11 +12870,11 @@
       <c r="N23" s="161"/>
       <c r="P23" s="163">
         <f>_xll.qlRateHelperEarliestDate(L23)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q23" s="163">
         <f>_xll.qlRateHelperLatestDate($L23)</f>
-        <v>42086</v>
+        <v>42110</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -12913,7 +12913,7 @@
       </c>
       <c r="L24" s="164" t="str">
         <f>_xll.qlOISRateHelper(K24,2,C24,J24,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS16M#0006</v>
+        <v>USD_YCONRH_OIS16M#0000</v>
       </c>
       <c r="M24" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -12922,11 +12922,11 @@
       <c r="N24" s="161"/>
       <c r="P24" s="163">
         <f>_xll.qlRateHelperEarliestDate(L24)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q24" s="163">
         <f>_xll.qlRateHelperLatestDate($L24)</f>
-        <v>42117</v>
+        <v>42142</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -12965,7 +12965,7 @@
       </c>
       <c r="L25" s="164" t="str">
         <f>_xll.qlOISRateHelper(K25,2,C25,J25,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS17M#0006</v>
+        <v>USD_YCONRH_OIS17M#0000</v>
       </c>
       <c r="M25" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -12974,11 +12974,11 @@
       <c r="N25" s="161"/>
       <c r="P25" s="163">
         <f>_xll.qlRateHelperEarliestDate(L25)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q25" s="163">
         <f>_xll.qlRateHelperLatestDate($L25)</f>
-        <v>42149</v>
+        <v>42171</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -13017,7 +13017,7 @@
       </c>
       <c r="L26" s="164" t="str">
         <f>_xll.qlOISRateHelper(K26,2,C26,J26,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS18M#0006</v>
+        <v>USD_YCONRH_OIS18M#0000</v>
       </c>
       <c r="M26" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -13026,11 +13026,11 @@
       <c r="N26" s="161"/>
       <c r="P26" s="163">
         <f>_xll.qlRateHelperEarliestDate(L26)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q26" s="163">
         <f>_xll.qlRateHelperLatestDate($L26)</f>
-        <v>42178</v>
+        <v>42201</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -13069,7 +13069,7 @@
       </c>
       <c r="L27" s="164" t="str">
         <f>_xll.qlOISRateHelper(K27,2,C27,J27,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS19M#0006</v>
+        <v>USD_YCONRH_OIS19M#0000</v>
       </c>
       <c r="M27" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -13078,11 +13078,11 @@
       <c r="N27" s="161"/>
       <c r="P27" s="163">
         <f>_xll.qlRateHelperEarliestDate(L27)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q27" s="163">
         <f>_xll.qlRateHelperLatestDate($L27)</f>
-        <v>42208</v>
+        <v>42233</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
@@ -13121,7 +13121,7 @@
       </c>
       <c r="L28" s="164" t="str">
         <f>_xll.qlOISRateHelper(K28,2,C28,J28,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS20M#0006</v>
+        <v>USD_YCONRH_OIS20M#0000</v>
       </c>
       <c r="M28" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -13130,11 +13130,11 @@
       <c r="N28" s="161"/>
       <c r="P28" s="163">
         <f>_xll.qlRateHelperEarliestDate(L28)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q28" s="163">
         <f>_xll.qlRateHelperLatestDate($L28)</f>
-        <v>42240</v>
+        <v>42263</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -13173,7 +13173,7 @@
       </c>
       <c r="L29" s="164" t="str">
         <f>_xll.qlOISRateHelper(K29,2,C29,J29,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS21M#0006</v>
+        <v>USD_YCONRH_OIS21M#0000</v>
       </c>
       <c r="M29" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -13182,11 +13182,11 @@
       <c r="N29" s="161"/>
       <c r="P29" s="163">
         <f>_xll.qlRateHelperEarliestDate(L29)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q29" s="163">
         <f>_xll.qlRateHelperLatestDate($L29)</f>
-        <v>42270</v>
+        <v>42293</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -13225,7 +13225,7 @@
       </c>
       <c r="L30" s="164" t="str">
         <f>_xll.qlOISRateHelper(K30,2,C30,J30,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS22M#0006</v>
+        <v>USD_YCONRH_OIS22M#0000</v>
       </c>
       <c r="M30" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -13234,11 +13234,11 @@
       <c r="N30" s="161"/>
       <c r="P30" s="163">
         <f>_xll.qlRateHelperEarliestDate(L30)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q30" s="163">
         <f>_xll.qlRateHelperLatestDate($L30)</f>
-        <v>42300</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -13277,7 +13277,7 @@
       </c>
       <c r="L31" s="164" t="str">
         <f>_xll.qlOISRateHelper(K31,2,C31,J31,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS23M#0006</v>
+        <v>USD_YCONRH_OIS23M#0000</v>
       </c>
       <c r="M31" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -13286,11 +13286,11 @@
       <c r="N31" s="161"/>
       <c r="P31" s="163">
         <f>_xll.qlRateHelperEarliestDate(L31)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q31" s="163">
         <f>_xll.qlRateHelperLatestDate($L31)</f>
-        <v>42331</v>
+        <v>42354</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -13329,7 +13329,7 @@
       </c>
       <c r="L32" s="164" t="str">
         <f>_xll.qlOISRateHelper(K32,2,C32,J32,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2Y#0006</v>
+        <v>USD_YCONRH_OIS2Y#0000</v>
       </c>
       <c r="M32" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -13338,11 +13338,11 @@
       <c r="N32" s="161"/>
       <c r="P32" s="163">
         <f>_xll.qlRateHelperEarliestDate(L32)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q32" s="163">
         <f>_xll.qlRateHelperLatestDate($L32)</f>
-        <v>42361</v>
+        <v>42387</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -13381,7 +13381,7 @@
       </c>
       <c r="L33" s="164" t="str">
         <f>_xll.qlOISRateHelper(K33,2,C33,J33,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS27M#0006</v>
+        <v>USD_YCONRH_OIS27M#0000</v>
       </c>
       <c r="M33" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -13390,11 +13390,11 @@
       <c r="N33" s="161"/>
       <c r="P33" s="163">
         <f>_xll.qlRateHelperEarliestDate(L33)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q33" s="163">
         <f>_xll.qlRateHelperLatestDate($L33)</f>
-        <v>42452</v>
+        <v>42478</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -13433,7 +13433,7 @@
       </c>
       <c r="L34" s="164" t="str">
         <f>_xll.qlOISRateHelper(K34,2,C34,J34,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS30M#0006</v>
+        <v>USD_YCONRH_OIS30M#0000</v>
       </c>
       <c r="M34" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -13442,11 +13442,11 @@
       <c r="N34" s="161"/>
       <c r="P34" s="163">
         <f>_xll.qlRateHelperEarliestDate(L34)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q34" s="163">
         <f>_xll.qlRateHelperLatestDate($L34)</f>
-        <v>42544</v>
+        <v>42569</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -13485,7 +13485,7 @@
       </c>
       <c r="L35" s="164" t="str">
         <f>_xll.qlOISRateHelper(K35,2,C35,J35,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS33M#0006</v>
+        <v>USD_YCONRH_OIS33M#0000</v>
       </c>
       <c r="M35" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -13494,11 +13494,11 @@
       <c r="N35" s="161"/>
       <c r="P35" s="163">
         <f>_xll.qlRateHelperEarliestDate(L35)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q35" s="163">
         <f>_xll.qlRateHelperLatestDate($L35)</f>
-        <v>42636</v>
+        <v>42660</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -13537,7 +13537,7 @@
       </c>
       <c r="L36" s="164" t="str">
         <f>_xll.qlOISRateHelper(K36,2,C36,J36,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3Y#0006</v>
+        <v>USD_YCONRH_OIS3Y#0000</v>
       </c>
       <c r="M36" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -13546,11 +13546,11 @@
       <c r="N36" s="161"/>
       <c r="P36" s="163">
         <f>_xll.qlRateHelperEarliestDate(L36)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q36" s="163">
         <f>_xll.qlRateHelperLatestDate($L36)</f>
-        <v>42727</v>
+        <v>42751</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -13589,7 +13589,7 @@
       </c>
       <c r="L37" s="164" t="str">
         <f>_xll.qlOISRateHelper(K37,2,C37,J37,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS39M#0006</v>
+        <v>USD_YCONRH_OIS39M#0000</v>
       </c>
       <c r="M37" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -13598,11 +13598,11 @@
       <c r="N37" s="161"/>
       <c r="P37" s="163">
         <f>_xll.qlRateHelperEarliestDate(L37)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q37" s="163">
         <f>_xll.qlRateHelperLatestDate($L37)</f>
-        <v>42817</v>
+        <v>42843</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -13641,7 +13641,7 @@
       </c>
       <c r="L38" s="164" t="str">
         <f>_xll.qlOISRateHelper(K38,2,C38,J38,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS42M#0006</v>
+        <v>USD_YCONRH_OIS42M#0000</v>
       </c>
       <c r="M38" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -13687,7 +13687,7 @@
       </c>
       <c r="L39" s="164" t="str">
         <f>_xll.qlOISRateHelper(K39,2,C39,J39,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS45M#0006</v>
+        <v>USD_YCONRH_OIS45M#0000</v>
       </c>
       <c r="M39" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -13733,7 +13733,7 @@
       </c>
       <c r="L40" s="164" t="str">
         <f>_xll.qlOISRateHelper(K40,2,C40,J40,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS4Y#0006</v>
+        <v>USD_YCONRH_OIS4Y#0000</v>
       </c>
       <c r="M40" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -13779,7 +13779,7 @@
       </c>
       <c r="L41" s="164" t="str">
         <f>_xll.qlOISRateHelper(K41,2,C41,J41,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS51M#0006</v>
+        <v>USD_YCONRH_OIS51M#0000</v>
       </c>
       <c r="M41" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -13825,7 +13825,7 @@
       </c>
       <c r="L42" s="164" t="str">
         <f>_xll.qlOISRateHelper(K42,2,C42,J42,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS54M#0006</v>
+        <v>USD_YCONRH_OIS54M#0000</v>
       </c>
       <c r="M42" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -13871,7 +13871,7 @@
       </c>
       <c r="L43" s="164" t="str">
         <f>_xll.qlOISRateHelper(K43,2,C43,J43,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS57M#0006</v>
+        <v>USD_YCONRH_OIS57M#0000</v>
       </c>
       <c r="M43" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -13917,7 +13917,7 @@
       </c>
       <c r="L44" s="164" t="str">
         <f>_xll.qlOISRateHelper(K44,2,C44,J44,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS5Y#0006</v>
+        <v>USD_YCONRH_OIS5Y#0000</v>
       </c>
       <c r="M44" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -13963,7 +13963,7 @@
       </c>
       <c r="L45" s="164" t="str">
         <f>_xll.qlOISRateHelper(K45,2,C45,J45,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS6Y#0006</v>
+        <v>USD_YCONRH_OIS6Y#0000</v>
       </c>
       <c r="M45" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -14009,7 +14009,7 @@
       </c>
       <c r="L46" s="164" t="str">
         <f>_xll.qlOISRateHelper(K46,2,C46,J46,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS7Y#0006</v>
+        <v>USD_YCONRH_OIS7Y#0000</v>
       </c>
       <c r="M46" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -14055,7 +14055,7 @@
       </c>
       <c r="L47" s="164" t="str">
         <f>_xll.qlOISRateHelper(K47,2,C47,J47,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS8Y#0006</v>
+        <v>USD_YCONRH_OIS8Y#0000</v>
       </c>
       <c r="M47" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -14101,7 +14101,7 @@
       </c>
       <c r="L48" s="164" t="str">
         <f>_xll.qlOISRateHelper(K48,2,C48,J48,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS9Y#0006</v>
+        <v>USD_YCONRH_OIS9Y#0000</v>
       </c>
       <c r="M48" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -14147,7 +14147,7 @@
       </c>
       <c r="L49" s="164" t="str">
         <f>_xll.qlOISRateHelper(K49,2,C49,J49,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS10Y#0006</v>
+        <v>USD_YCONRH_OIS10Y#0000</v>
       </c>
       <c r="M49" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -14193,7 +14193,7 @@
       </c>
       <c r="L50" s="164" t="str">
         <f>_xll.qlOISRateHelper(K50,2,C50,J50,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS12Y#0006</v>
+        <v>USD_YCONRH_OIS12Y#0000</v>
       </c>
       <c r="M50" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -14239,7 +14239,7 @@
       </c>
       <c r="L51" s="164" t="str">
         <f>_xll.qlOISRateHelper(K51,2,C51,J51,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS15Y#0006</v>
+        <v>USD_YCONRH_OIS15Y#0000</v>
       </c>
       <c r="M51" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -14285,7 +14285,7 @@
       </c>
       <c r="L52" s="164" t="str">
         <f>_xll.qlOISRateHelper(K52,2,C52,J52,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS20Y#0006</v>
+        <v>USD_YCONRH_OIS20Y#0000</v>
       </c>
       <c r="M52" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L52)</f>
@@ -14331,7 +14331,7 @@
       </c>
       <c r="L53" s="164" t="str">
         <f>_xll.qlOISRateHelper(K53,2,C53,J53,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS25Y#0006</v>
+        <v>USD_YCONRH_OIS25Y#0000</v>
       </c>
       <c r="M53" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L53)</f>
@@ -14377,7 +14377,7 @@
       </c>
       <c r="L54" s="164" t="str">
         <f>_xll.qlOISRateHelper(K54,2,C54,J54,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS27Y#0006</v>
+        <v>USD_YCONRH_OIS27Y#0000</v>
       </c>
       <c r="M54" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L54)</f>
@@ -14423,7 +14423,7 @@
       </c>
       <c r="L55" s="164" t="str">
         <f>_xll.qlOISRateHelper(K55,2,C55,J55,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS30Y#0006</v>
+        <v>USD_YCONRH_OIS30Y#0000</v>
       </c>
       <c r="M55" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L55)</f>
@@ -14469,7 +14469,7 @@
       </c>
       <c r="L56" s="164" t="str">
         <f>_xll.qlOISRateHelper(K56,2,C56,J56,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS35Y#0006</v>
+        <v>USD_YCONRH_OIS35Y#0000</v>
       </c>
       <c r="M56" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L56)</f>
@@ -14515,7 +14515,7 @@
       </c>
       <c r="L57" s="164" t="str">
         <f>_xll.qlOISRateHelper(K57,2,C57,J57,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS40Y#0006</v>
+        <v>USD_YCONRH_OIS40Y#0000</v>
       </c>
       <c r="M57" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L57)</f>
@@ -14561,7 +14561,7 @@
       </c>
       <c r="L58" s="164" t="str">
         <f>_xll.qlOISRateHelper(K58,2,C58,J58,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS45Y#0006</v>
+        <v>USD_YCONRH_OIS45Y#0000</v>
       </c>
       <c r="M58" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L58)</f>
@@ -14607,7 +14607,7 @@
       </c>
       <c r="L59" s="164" t="str">
         <f>_xll.qlOISRateHelper(K59,2,C59,J59,$L$4,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS50Y#0006</v>
+        <v>USD_YCONRH_OIS50Y#0000</v>
       </c>
       <c r="M59" s="95" t="str">
         <f>_xll.ohRangeRetrieveError(L59)</f>
@@ -14616,11 +14616,11 @@
       <c r="N59" s="161"/>
       <c r="P59" s="163">
         <f>_xll.qlRateHelperEarliestDate(L59)</f>
-        <v>41631</v>
+        <v>41655</v>
       </c>
       <c r="Q59" s="163">
         <f>_xll.qlRateHelperLatestDate($L59)</f>
-        <v>59894</v>
+        <v>59917</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
@@ -14680,9 +14680,9 @@
         <f>_xll.qlDatedOISRateHelper(K61,B61,B62,J61,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M61" s="95" t="e">
+      <c r="M61" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L61)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N61" s="161"/>
       <c r="P61" s="163" t="e">
@@ -14733,9 +14733,9 @@
         <f>_xll.qlDatedOISRateHelper(K62,B62,B63,J62,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M62" s="95" t="e">
+      <c r="M62" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L62)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N62" s="161"/>
       <c r="P62" s="163" t="e">
@@ -14786,9 +14786,9 @@
         <f>_xll.qlDatedOISRateHelper(K63,B63,B64,J63,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M63" s="95" t="e">
+      <c r="M63" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L63)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N63" s="161"/>
       <c r="P63" s="163" t="e">
@@ -14839,9 +14839,9 @@
         <f>_xll.qlDatedOISRateHelper(K64,B64,B65,J64,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M64" s="95" t="e">
+      <c r="M64" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L64)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N64" s="161"/>
       <c r="P64" s="163" t="e">
@@ -14892,9 +14892,9 @@
         <f>_xll.qlDatedOISRateHelper(K65,B65,B66,J65,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M65" s="95" t="e">
+      <c r="M65" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L65)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N65" s="161"/>
       <c r="P65" s="163" t="e">
@@ -14945,9 +14945,9 @@
         <f>_xll.qlDatedOISRateHelper(K66,B66,B67,J66,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M66" s="95" t="e">
+      <c r="M66" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L66)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N66" s="161"/>
       <c r="P66" s="163" t="e">
@@ -14998,9 +14998,9 @@
         <f>_xll.qlDatedOISRateHelper(K67,B67,B68,J67,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M67" s="95" t="e">
+      <c r="M67" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L67)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N67" s="161"/>
       <c r="P67" s="163" t="e">
@@ -15051,9 +15051,9 @@
         <f>_xll.qlDatedOISRateHelper(K68,B68,B69,J68,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M68" s="95" t="e">
+      <c r="M68" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L68)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N68" s="161"/>
       <c r="P68" s="163" t="e">
@@ -15104,9 +15104,9 @@
         <f>_xll.qlDatedOISRateHelper(K69,B69,B70,J69,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M69" s="95" t="e">
+      <c r="M69" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L69)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N69" s="161"/>
       <c r="P69" s="163" t="e">
@@ -15157,9 +15157,9 @@
         <f>_xll.qlDatedOISRateHelper(K70,B70,B71,J70,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M70" s="95" t="e">
+      <c r="M70" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L70)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N70" s="161"/>
       <c r="P70" s="163" t="e">
@@ -15210,9 +15210,9 @@
         <f>_xll.qlDatedOISRateHelper(K71,B71,B72,J71,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M71" s="95" t="e">
+      <c r="M71" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L71)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N71" s="161"/>
       <c r="P71" s="163" t="e">
@@ -15263,9 +15263,9 @@
         <f>_xll.qlDatedOISRateHelper(K72,B72,B73,J72,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#NUM!</v>
       </c>
-      <c r="M72" s="95" t="e">
+      <c r="M72" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L72)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N72" s="161"/>
       <c r="P72" s="163" t="e">
@@ -15316,9 +15316,9 @@
         <f>_xll.qlDatedOISRateHelper(K73,B73,B74,J73,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M73" s="95" t="e">
+      <c r="M73" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L73)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N73" s="161"/>
       <c r="P73" s="163" t="e">
@@ -15369,9 +15369,9 @@
         <f>_xll.qlDatedOISRateHelper(K74,B74,B75,J74,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M74" s="95" t="e">
+      <c r="M74" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L74)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N74" s="161"/>
       <c r="P74" s="163" t="e">
@@ -15422,9 +15422,9 @@
         <f>_xll.qlDatedOISRateHelper(K75,B75,B76,J75,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M75" s="95" t="e">
+      <c r="M75" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L75)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N75" s="161"/>
       <c r="P75" s="163" t="e">
@@ -15475,9 +15475,9 @@
         <f>_xll.qlDatedOISRateHelper(K76,B76,B77,J76,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M76" s="95" t="e">
+      <c r="M76" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L76)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N76" s="161"/>
       <c r="P76" s="163" t="e">
@@ -15528,9 +15528,9 @@
         <f>_xll.qlDatedOISRateHelper(K77,B77,B78,J77,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M77" s="95" t="e">
+      <c r="M77" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L77)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N77" s="161"/>
       <c r="P77" s="163" t="e">
@@ -15581,9 +15581,9 @@
         <f>_xll.qlDatedOISRateHelper(K78,B78,B79,J78,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M78" s="95" t="e">
+      <c r="M78" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L78)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N78" s="161"/>
       <c r="P78" s="163" t="e">
@@ -15634,9 +15634,9 @@
         <f>_xll.qlDatedOISRateHelper(K79,B79,B80,J79,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M79" s="95" t="e">
+      <c r="M79" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L79)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N79" s="161"/>
       <c r="P79" s="163" t="e">
@@ -15687,9 +15687,9 @@
         <f>_xll.qlDatedOISRateHelper(K80,B80,B81,J80,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M80" s="95" t="e">
+      <c r="M80" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L80)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N80" s="161"/>
       <c r="P80" s="163" t="e">
@@ -15740,9 +15740,9 @@
         <f>_xll.qlDatedOISRateHelper(K81,B81,B82,J81,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M81" s="95" t="e">
+      <c r="M81" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L81)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N81" s="161"/>
       <c r="P81" s="163" t="e">
@@ -15793,9 +15793,9 @@
         <f>_xll.qlDatedOISRateHelper(K82,B82,B83,J82,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M82" s="95" t="e">
+      <c r="M82" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L82)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N82" s="161"/>
       <c r="P82" s="163" t="e">
@@ -15846,9 +15846,9 @@
         <f>_xll.qlDatedOISRateHelper(K83,B83,B84,J83,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M83" s="95" t="e">
+      <c r="M83" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L83)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N83" s="161"/>
       <c r="P83" s="163" t="e">
@@ -15899,9 +15899,9 @@
         <f>_xll.qlDatedOISRateHelper(K84,B84,B85,J84,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M84" s="95" t="e">
+      <c r="M84" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L84)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N84" s="161"/>
       <c r="P84" s="163" t="e">
@@ -15952,9 +15952,9 @@
         <f>_xll.qlDatedOISRateHelper(K85,B85,B86,J85,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M85" s="95" t="e">
+      <c r="M85" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L85)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N85" s="161"/>
       <c r="P85" s="163" t="e">
@@ -16005,9 +16005,9 @@
         <f>_xll.qlDatedOISRateHelper(K86,B86,B87,J86,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M86" s="95" t="e">
+      <c r="M86" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L86)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N86" s="161"/>
       <c r="P86" s="163" t="e">
@@ -16058,9 +16058,9 @@
         <f>_xll.qlDatedOISRateHelper(K87,B87,B88,J87,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M87" s="95" t="e">
+      <c r="M87" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L87)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N87" s="161"/>
       <c r="P87" s="163" t="e">
@@ -16111,9 +16111,9 @@
         <f>_xll.qlDatedOISRateHelper(K88,B88,B89,J88,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M88" s="95" t="e">
+      <c r="M88" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L88)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N88" s="161"/>
       <c r="P88" s="163" t="e">
@@ -16164,9 +16164,9 @@
         <f>_xll.qlDatedOISRateHelper(K89,B89,B90,J89,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M89" s="95" t="e">
+      <c r="M89" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L89)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N89" s="161"/>
       <c r="P89" s="163" t="e">
@@ -16217,9 +16217,9 @@
         <f>_xll.qlDatedOISRateHelper(K90,B90,B91,J90,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M90" s="95" t="e">
+      <c r="M90" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L90)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N90" s="161"/>
       <c r="P90" s="163" t="e">
@@ -16270,9 +16270,9 @@
         <f>_xll.qlDatedOISRateHelper(K91,B91,B92,J91,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M91" s="95" t="e">
+      <c r="M91" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L91)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N91" s="161"/>
       <c r="P91" s="163" t="e">
@@ -16323,9 +16323,9 @@
         <f>_xll.qlDatedOISRateHelper(K92,B92,B93,J92,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M92" s="95" t="e">
+      <c r="M92" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L92)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N92" s="161"/>
       <c r="P92" s="163" t="e">
@@ -16376,9 +16376,9 @@
         <f>_xll.qlDatedOISRateHelper(K93,B93,B94,J93,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M93" s="95" t="e">
+      <c r="M93" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L93)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N93" s="161"/>
       <c r="P93" s="163" t="e">
@@ -16429,9 +16429,9 @@
         <f>_xll.qlDatedOISRateHelper(K94,B94,B95,J94,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M94" s="95" t="e">
+      <c r="M94" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L94)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N94" s="161"/>
       <c r="P94" s="163" t="e">
@@ -16482,9 +16482,9 @@
         <f>_xll.qlDatedOISRateHelper(K95,B95,#REF!,J95,$L$4,Permanent,,ObjectOverwrite)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M95" s="95" t="e">
+      <c r="M95" s="95" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(L95)</f>
-        <v>#NUM!</v>
+        <v/>
       </c>
       <c r="N95" s="161"/>
       <c r="P95" s="163" t="e">

</xml_diff>

<commit_message>
USD work in progress: cleaned up unused ratehelpers
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YCONBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YCONBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="375" windowWidth="25635" windowHeight="11025" tabRatio="821"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15300" windowHeight="7995" tabRatio="821" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="224">
   <si>
     <t>60Y</t>
   </si>
@@ -882,6 +882,12 @@
   </si>
   <si>
     <t>MonotonicLogCubicNaturalSpline</t>
+  </si>
+  <si>
+    <t>UnitedStates::Settlement</t>
+  </si>
+  <si>
+    <t>JoinHolidays</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1547,7 @@
     <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1984,6 +1990,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="4"/>
@@ -2298,15 +2307,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="2.7109375" style="180" customWidth="1"/>
     <col min="3" max="3" width="18" style="180" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="180" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="180" customWidth="1"/>
     <col min="5" max="5" width="22" style="180" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="2.7109375" style="180" customWidth="1"/>
     <col min="8" max="8" width="4" style="180" bestFit="1" customWidth="1"/>
@@ -2495,9 +2504,7 @@
       <c r="C11" s="85" t="s">
         <v>121</v>
       </c>
-      <c r="D11" s="84">
-        <v>41753.680752314816</v>
-      </c>
+      <c r="D11" s="84"/>
       <c r="E11" s="57"/>
       <c r="F11" s="56"/>
       <c r="K11" s="125"/>
@@ -2553,7 +2560,9 @@
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,,,Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
         <v>_USDYCON#0002</v>
       </c>
-      <c r="E14" s="57"/>
+      <c r="E14" s="57" t="s">
+        <v>223</v>
+      </c>
       <c r="F14" s="56"/>
       <c r="K14" s="125"/>
       <c r="L14" s="124" t="s">
@@ -2574,7 +2583,9 @@
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
-      <c r="E15" s="57"/>
+      <c r="E15" s="57" t="s">
+        <v>115</v>
+      </c>
       <c r="F15" s="56"/>
       <c r="K15" s="121"/>
       <c r="L15" s="120"/>
@@ -2590,7 +2601,9 @@
         <f>"_"&amp;Currency&amp;"YC"&amp;IndexTenor</f>
         <v>_USDYCON</v>
       </c>
-      <c r="E16" s="57"/>
+      <c r="E16" s="57" t="s">
+        <v>222</v>
+      </c>
       <c r="F16" s="56"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
@@ -2609,8 +2622,9 @@
       <c r="C18" s="68" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="76" t="s">
-        <v>115</v>
+      <c r="D18" s="200" t="str">
+        <f>E14&amp;"("&amp;E15&amp;","&amp;E16&amp;")"</f>
+        <v>JoinHolidays(UnitedKingdom::Exchange,UnitedStates::Settlement)</v>
       </c>
       <c r="E18" s="57"/>
       <c r="F18" s="56"/>
@@ -2705,7 +2719,7 @@
       <c r="B27" s="59"/>
       <c r="C27" s="63">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41753</v>
+        <v>41757</v>
       </c>
       <c r="D27" s="62">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2718,11 +2732,11 @@
       <c r="B28" s="59"/>
       <c r="C28" s="61">
         <f>MAX(_xll.ohPack(Selected!H2:H126))</f>
-        <v>60020</v>
+        <v>60022</v>
       </c>
       <c r="D28" s="60">
         <f>MIN(_xll.ohPack(Selected!I1:I126))</f>
-        <v>0.16020945108279799</v>
+        <v>0.19692498522639698</v>
       </c>
       <c r="E28" s="57"/>
       <c r="F28" s="56"/>
@@ -2765,7 +2779,7 @@
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="K9:N9"/>
   </mergeCells>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25">
       <formula1>"Linear,BackwardFlat,ForwardFlat,Linear,LogLinear,CubicNaturalSpline,LogCubicNaturalSpline,MonotonicCubicNaturalSpline,MonotonicLogCubicNaturalSpline,FritschButlandCubic,FritschButlandLogCubic,KrugerCubic,KrugerLogCubic"</formula1>
     </dataValidation>
@@ -2778,11 +2792,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4">
       <formula1>"EUR,USD,GBP,JPY,CHF"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
-      <formula1>"TARGET,UnitedKingdom::Exchange,UnitedKingdom::Metals,UnitedKingdom::Settlement,UnitedStates::GovernmentBond,UnitedStates::NERC,UnitedStates::NYSE,UnitedStates::Settlement,Switzerland,Japan,Italy::Exchange"</formula1>
-    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M11">
       <formula1>"Libor,ibor"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E15:E16">
+      <formula1>"TARGET,UnitedKingdom::Exchange,UnitedKingdom::Metals,UnitedKingdom::Settlement,UnitedStates::GovernmentBond,UnitedStates::NERC,UnitedStates::NYSE,UnitedStates::Settlement,Switzerland,Japan,Italy::Exchange,NullCalendar"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E14">
+      <formula1>"JoinBusinessDays,JoinHolidays"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2858,11 +2875,11 @@
       </c>
       <c r="E2" s="14" t="str">
         <f>ON_Deposits!F3</f>
-        <v>USD_YCONRH_OND#0000</v>
+        <v>USD_YCONRH_OND#0001</v>
       </c>
       <c r="F2" s="13">
         <f>_xll.qlRateHelperQuoteValue($E2,Trigger)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="179" t="b">
@@ -2876,11 +2893,11 @@
       </c>
       <c r="K2" s="12">
         <f>_xll.qlRateHelperEarliestDate($E2,Trigger)</f>
-        <v>41753</v>
+        <v>41757</v>
       </c>
       <c r="L2" s="11">
         <f>_xll.qlRateHelperLatestDate($E2,Trigger)</f>
-        <v>41754</v>
+        <v>41758</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2891,11 +2908,11 @@
       </c>
       <c r="E3" s="14" t="str">
         <f>ON_FRAs!H3</f>
-        <v>USD_YCONRH_TND#0000</v>
+        <v>USD_YCONRH_TND#0001</v>
       </c>
       <c r="F3" s="13">
         <f>_xll.qlRateHelperQuoteValue($E3,Trigger)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="179" t="b">
@@ -2909,11 +2926,11 @@
       </c>
       <c r="K3" s="12">
         <f>_xll.qlRateHelperEarliestDate($E3,Trigger)</f>
-        <v>41754</v>
+        <v>41758</v>
       </c>
       <c r="L3" s="11">
         <f>_xll.qlRateHelperLatestDate($E3,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -2924,11 +2941,11 @@
       </c>
       <c r="E4" s="14" t="str">
         <f>ON_FRAs!H4</f>
-        <v>USD_YCONRH_SND#0000</v>
+        <v>USD_YCONRH_SND#0001</v>
       </c>
       <c r="F4" s="13">
         <f>_xll.qlRateHelperQuoteValue($E4,Trigger)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="6" t="b">
@@ -2942,11 +2959,11 @@
       </c>
       <c r="K4" s="12">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L4" s="11">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41758</v>
+        <v>41761</v>
       </c>
     </row>
     <row r="5" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4142,11 +4159,11 @@
       </c>
       <c r="E35" s="21" t="str">
         <f>ON_Swaps!L6</f>
-        <v>USD_YCONRH_OISSW#0000</v>
+        <v>USD_YCONRH_OISSW#0004</v>
       </c>
       <c r="F35" s="20">
         <f>_xll.qlRateHelperQuoteValue($E35,Trigger)</f>
-        <v>7.9000000000000001E-4</v>
+        <v>1.06E-3</v>
       </c>
       <c r="G35" s="20" t="e">
         <f>_xll.qlSwapRateHelperSpread($E35,Trigger)</f>
@@ -4164,11 +4181,11 @@
       </c>
       <c r="K35" s="18">
         <f>_xll.qlRateHelperEarliestDate($E35,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L35" s="17">
         <f>_xll.qlRateHelperLatestDate($E35,Trigger)</f>
-        <v>41764</v>
+        <v>41766</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.2">
@@ -4182,11 +4199,11 @@
       </c>
       <c r="E36" s="14" t="str">
         <f>ON_Swaps!L7</f>
-        <v>USD_YCONRH_OIS2W#0000</v>
+        <v>USD_YCONRH_OIS2W#0001</v>
       </c>
       <c r="F36" s="13">
         <f>_xll.qlRateHelperQuoteValue($E36,Trigger)</f>
-        <v>7.9000000000000001E-4</v>
+        <v>9.8999999999999999E-4</v>
       </c>
       <c r="G36" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E36,Trigger)</f>
@@ -4204,11 +4221,11 @@
       </c>
       <c r="K36" s="12">
         <f>_xll.qlRateHelperEarliestDate($E36,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L36" s="11">
         <f>_xll.qlRateHelperLatestDate($E36,Trigger)</f>
-        <v>41771</v>
+        <v>41773</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.2">
@@ -4222,11 +4239,11 @@
       </c>
       <c r="E37" s="14" t="str">
         <f>ON_Swaps!L8</f>
-        <v>USD_YCONRH_OIS3W#0000</v>
+        <v>USD_YCONRH_OIS3W#0001</v>
       </c>
       <c r="F37" s="13">
         <f>_xll.qlRateHelperQuoteValue($E37,Trigger)</f>
-        <v>8.0000000000000004E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
       <c r="G37" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E37,Trigger)</f>
@@ -4244,11 +4261,11 @@
       </c>
       <c r="K37" s="12">
         <f>_xll.qlRateHelperEarliestDate($E37,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L37" s="11">
         <f>_xll.qlRateHelperLatestDate($E37,Trigger)</f>
-        <v>41778</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.2">
@@ -4262,11 +4279,11 @@
       </c>
       <c r="E38" s="14" t="str">
         <f>ON_Swaps!L9</f>
-        <v>USD_YCONRH_OIS1M#0000</v>
+        <v>USD_YCONRH_OIS1M#0001</v>
       </c>
       <c r="F38" s="13">
         <f>_xll.qlRateHelperQuoteValue($E38,Trigger)</f>
-        <v>8.1000000000000006E-4</v>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="G38" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E38,Trigger)</f>
@@ -4284,11 +4301,11 @@
       </c>
       <c r="K38" s="12">
         <f>_xll.qlRateHelperEarliestDate($E38,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L38" s="11">
         <f>_xll.qlRateHelperLatestDate($E38,Trigger)</f>
-        <v>41787</v>
+        <v>41789</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.2">
@@ -4302,11 +4319,11 @@
       </c>
       <c r="E39" s="14" t="str">
         <f>ON_Swaps!L10</f>
-        <v>USD_YCONRH_OIS2M#0000</v>
+        <v>USD_YCONRH_OIS2M#0001</v>
       </c>
       <c r="F39" s="13">
         <f>_xll.qlRateHelperQuoteValue($E39,Trigger)</f>
-        <v>8.1999999999999998E-4</v>
+        <v>9.5E-4</v>
       </c>
       <c r="G39" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E39,Trigger)</f>
@@ -4324,7 +4341,7 @@
       </c>
       <c r="K39" s="12">
         <f>_xll.qlRateHelperEarliestDate($E39,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L39" s="11">
         <f>_xll.qlRateHelperLatestDate($E39,Trigger)</f>
@@ -4342,11 +4359,11 @@
       </c>
       <c r="E40" s="14" t="str">
         <f>ON_Swaps!L11</f>
-        <v>USD_YCONRH_OIS3M#0000</v>
+        <v>USD_YCONRH_OIS3M#0001</v>
       </c>
       <c r="F40" s="13">
         <f>_xll.qlRateHelperQuoteValue($E40,Trigger)</f>
-        <v>8.7999999999999992E-4</v>
+        <v>9.5E-4</v>
       </c>
       <c r="G40" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E40,Trigger)</f>
@@ -4364,11 +4381,11 @@
       </c>
       <c r="K40" s="12">
         <f>_xll.qlRateHelperEarliestDate($E40,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L40" s="11">
         <f>_xll.qlRateHelperLatestDate($E40,Trigger)</f>
-        <v>41848</v>
+        <v>41851</v>
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.2">
@@ -4382,11 +4399,11 @@
       </c>
       <c r="E41" s="14" t="str">
         <f>ON_Swaps!L12</f>
-        <v>USD_YCONRH_OIS4M#0000</v>
+        <v>USD_YCONRH_OIS4M#0001</v>
       </c>
       <c r="F41" s="13">
         <f>_xll.qlRateHelperQuoteValue($E41,Trigger)</f>
-        <v>9.1E-4</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="G41" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E41,Trigger)</f>
@@ -4404,11 +4421,11 @@
       </c>
       <c r="K41" s="12">
         <f>_xll.qlRateHelperEarliestDate($E41,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L41" s="11">
         <f>_xll.qlRateHelperLatestDate($E41,Trigger)</f>
-        <v>41879</v>
+        <v>41880</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.2">
@@ -4422,11 +4439,11 @@
       </c>
       <c r="E42" s="14" t="str">
         <f>ON_Swaps!L13</f>
-        <v>USD_YCONRH_OIS5M#0000</v>
+        <v>USD_YCONRH_OIS5M#0001</v>
       </c>
       <c r="F42" s="13">
         <f>_xll.qlRateHelperQuoteValue($E42,Trigger)</f>
-        <v>9.2999999999999995E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G42" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E42,Trigger)</f>
@@ -4444,11 +4461,11 @@
       </c>
       <c r="K42" s="12">
         <f>_xll.qlRateHelperEarliestDate($E42,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L42" s="11">
         <f>_xll.qlRateHelperLatestDate($E42,Trigger)</f>
-        <v>41911</v>
+        <v>41912</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.2">
@@ -4462,11 +4479,11 @@
       </c>
       <c r="E43" s="14" t="str">
         <f>ON_Swaps!L14</f>
-        <v>USD_YCONRH_OIS6M#0000</v>
+        <v>USD_YCONRH_OIS6M#0001</v>
       </c>
       <c r="F43" s="13">
         <f>_xll.qlRateHelperQuoteValue($E43,Trigger)</f>
-        <v>9.6000000000000002E-4</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="G43" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E43,Trigger)</f>
@@ -4484,11 +4501,11 @@
       </c>
       <c r="K43" s="12">
         <f>_xll.qlRateHelperEarliestDate($E43,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L43" s="11">
         <f>_xll.qlRateHelperLatestDate($E43,Trigger)</f>
-        <v>41940</v>
+        <v>41943</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.2">
@@ -4502,11 +4519,11 @@
       </c>
       <c r="E44" s="14" t="str">
         <f>ON_Swaps!L15</f>
-        <v>USD_YCONRH_OIS7M#0000</v>
+        <v>USD_YCONRH_OIS7M#0001</v>
       </c>
       <c r="F44" s="13">
         <f>_xll.qlRateHelperQuoteValue($E44,Trigger)</f>
-        <v>1.01E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="G44" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E44,Trigger)</f>
@@ -4524,7 +4541,7 @@
       </c>
       <c r="K44" s="12">
         <f>_xll.qlRateHelperEarliestDate($E44,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L44" s="11">
         <f>_xll.qlRateHelperLatestDate($E44,Trigger)</f>
@@ -4542,11 +4559,11 @@
       </c>
       <c r="E45" s="14" t="str">
         <f>ON_Swaps!L16</f>
-        <v>USD_YCONRH_OIS8M#0000</v>
+        <v>USD_YCONRH_OIS8M#0001</v>
       </c>
       <c r="F45" s="13">
         <f>_xll.qlRateHelperQuoteValue($E45,Trigger)</f>
-        <v>1.0499999999999999E-3</v>
+        <v>1.08E-3</v>
       </c>
       <c r="G45" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E45,Trigger)</f>
@@ -4564,11 +4581,11 @@
       </c>
       <c r="K45" s="12">
         <f>_xll.qlRateHelperEarliestDate($E45,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L45" s="11">
         <f>_xll.qlRateHelperLatestDate($E45,Trigger)</f>
-        <v>42002</v>
+        <v>42004</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.2">
@@ -4582,11 +4599,11 @@
       </c>
       <c r="E46" s="14" t="str">
         <f>ON_Swaps!L17</f>
-        <v>USD_YCONRH_OIS9M#0000</v>
+        <v>USD_YCONRH_OIS9M#0001</v>
       </c>
       <c r="F46" s="13">
         <f>_xll.qlRateHelperQuoteValue($E46,Trigger)</f>
-        <v>1.1100000000000001E-3</v>
+        <v>1.1200000000000001E-3</v>
       </c>
       <c r="G46" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E46,Trigger)</f>
@@ -4604,11 +4621,11 @@
       </c>
       <c r="K46" s="12">
         <f>_xll.qlRateHelperEarliestDate($E46,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L46" s="11">
         <f>_xll.qlRateHelperLatestDate($E46,Trigger)</f>
-        <v>42032</v>
+        <v>42034</v>
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.2">
@@ -4622,7 +4639,7 @@
       </c>
       <c r="E47" s="14" t="str">
         <f>ON_Swaps!L18</f>
-        <v>USD_YCONRH_OIS10M#0000</v>
+        <v>USD_YCONRH_OIS10M#0001</v>
       </c>
       <c r="F47" s="13">
         <f>_xll.qlRateHelperQuoteValue($E47,Trigger)</f>
@@ -4644,7 +4661,7 @@
       </c>
       <c r="K47" s="12">
         <f>_xll.qlRateHelperEarliestDate($E47,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L47" s="11">
         <f>_xll.qlRateHelperLatestDate($E47,Trigger)</f>
@@ -4662,11 +4679,11 @@
       </c>
       <c r="E48" s="14" t="str">
         <f>ON_Swaps!L19</f>
-        <v>USD_YCONRH_OIS11M#0000</v>
+        <v>USD_YCONRH_OIS11M#0001</v>
       </c>
       <c r="F48" s="13">
         <f>_xll.qlRateHelperQuoteValue($E48,Trigger)</f>
-        <v>1.2099999999999999E-3</v>
+        <v>1.23E-3</v>
       </c>
       <c r="G48" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E48,Trigger)</f>
@@ -4684,11 +4701,11 @@
       </c>
       <c r="K48" s="12">
         <f>_xll.qlRateHelperEarliestDate($E48,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L48" s="11">
         <f>_xll.qlRateHelperLatestDate($E48,Trigger)</f>
-        <v>42093</v>
+        <v>42094</v>
       </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.2">
@@ -4702,11 +4719,11 @@
       </c>
       <c r="E49" s="14" t="str">
         <f>ON_Swaps!L20</f>
-        <v>USD_YCONRH_OIS1Y#0000</v>
+        <v>USD_YCONRH_OIS1Y#0001</v>
       </c>
       <c r="F49" s="13">
         <f>_xll.qlRateHelperQuoteValue($E49,Trigger)</f>
-        <v>1.2900000000000001E-3</v>
+        <v>1.31E-3</v>
       </c>
       <c r="G49" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E49,Trigger)</f>
@@ -4724,11 +4741,11 @@
       </c>
       <c r="K49" s="12">
         <f>_xll.qlRateHelperEarliestDate($E49,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L49" s="11">
         <f>_xll.qlRateHelperLatestDate($E49,Trigger)</f>
-        <v>42122</v>
+        <v>42124</v>
       </c>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.2">
@@ -4745,11 +4762,11 @@
       </c>
       <c r="E50" s="14" t="str">
         <f>ON_Swaps!L21</f>
-        <v>USD_YCONRH_OIS13M#0000</v>
+        <v>USD_YCONRH_OIS13M#0001</v>
       </c>
       <c r="F50" s="13">
         <f>_xll.qlRateHelperQuoteValue($E50,Trigger)</f>
-        <v>1.3700000000000001E-3</v>
+        <v>1.4000000000000002E-3</v>
       </c>
       <c r="G50" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E50,Trigger)</f>
@@ -4767,11 +4784,11 @@
       </c>
       <c r="K50" s="12">
         <f>_xll.qlRateHelperEarliestDate($E50,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L50" s="11">
         <f>_xll.qlRateHelperLatestDate($E50,Trigger)</f>
-        <v>42152</v>
+        <v>42153</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.2">
@@ -4788,11 +4805,11 @@
       </c>
       <c r="E51" s="14" t="str">
         <f>ON_Swaps!L22</f>
-        <v>USD_YCONRH_OIS14M#0000</v>
+        <v>USD_YCONRH_OIS14M#0001</v>
       </c>
       <c r="F51" s="13">
         <f>_xll.qlRateHelperQuoteValue($E51,Trigger)</f>
-        <v>1.4599999999999999E-3</v>
+        <v>1.5200000000000003E-3</v>
       </c>
       <c r="G51" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E51,Trigger)</f>
@@ -4810,11 +4827,11 @@
       </c>
       <c r="K51" s="12">
         <f>_xll.qlRateHelperEarliestDate($E51,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L51" s="11">
         <f>_xll.qlRateHelperLatestDate($E51,Trigger)</f>
-        <v>42184</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.2">
@@ -4831,11 +4848,11 @@
       </c>
       <c r="E52" s="14" t="str">
         <f>ON_Swaps!L23</f>
-        <v>USD_YCONRH_OIS15M#0000</v>
+        <v>USD_YCONRH_OIS15M#0001</v>
       </c>
       <c r="F52" s="13">
         <f>_xll.qlRateHelperQuoteValue($E52,Trigger)</f>
-        <v>1.56E-3</v>
+        <v>1.6599999999999998E-3</v>
       </c>
       <c r="G52" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E52,Trigger)</f>
@@ -4853,11 +4870,11 @@
       </c>
       <c r="K52" s="12">
         <f>_xll.qlRateHelperEarliestDate($E52,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L52" s="11">
         <f>_xll.qlRateHelperLatestDate($E52,Trigger)</f>
-        <v>42213</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.2">
@@ -4874,11 +4891,11 @@
       </c>
       <c r="E53" s="14" t="str">
         <f>ON_Swaps!L24</f>
-        <v>USD_YCONRH_OIS16M#0000</v>
+        <v>USD_YCONRH_OIS16M#0001</v>
       </c>
       <c r="F53" s="13">
         <f>_xll.qlRateHelperQuoteValue($E53,Trigger)</f>
-        <v>1.6800000000000001E-3</v>
+        <v>1.83E-3</v>
       </c>
       <c r="G53" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E53,Trigger)</f>
@@ -4896,11 +4913,11 @@
       </c>
       <c r="K53" s="12">
         <f>_xll.qlRateHelperEarliestDate($E53,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L53" s="11">
         <f>_xll.qlRateHelperLatestDate($E53,Trigger)</f>
-        <v>42244</v>
+        <v>42247</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.2">
@@ -4917,11 +4934,11 @@
       </c>
       <c r="E54" s="14" t="str">
         <f>ON_Swaps!L25</f>
-        <v>USD_YCONRH_OIS17M#0000</v>
+        <v>USD_YCONRH_OIS17M#0001</v>
       </c>
       <c r="F54" s="13">
         <f>_xll.qlRateHelperQuoteValue($E54,Trigger)</f>
-        <v>1.81E-3</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="G54" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E54,Trigger)</f>
@@ -4939,11 +4956,11 @@
       </c>
       <c r="K54" s="12">
         <f>_xll.qlRateHelperEarliestDate($E54,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L54" s="11">
         <f>_xll.qlRateHelperLatestDate($E54,Trigger)</f>
-        <v>42275</v>
+        <v>42277</v>
       </c>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.2">
@@ -4960,11 +4977,11 @@
       </c>
       <c r="E55" s="14" t="str">
         <f>ON_Swaps!L26</f>
-        <v>USD_YCONRH_OIS18M#0000</v>
+        <v>USD_YCONRH_OIS18M#0001</v>
       </c>
       <c r="F55" s="13">
         <f>_xll.qlRateHelperQuoteValue($E55,Trigger)</f>
-        <v>1.9500000000000001E-3</v>
+        <v>2.2099999999999997E-3</v>
       </c>
       <c r="G55" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E55,Trigger)</f>
@@ -4982,11 +4999,11 @@
       </c>
       <c r="K55" s="12">
         <f>_xll.qlRateHelperEarliestDate($E55,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L55" s="11">
         <f>_xll.qlRateHelperLatestDate($E55,Trigger)</f>
-        <v>42305</v>
+        <v>42307</v>
       </c>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.2">
@@ -5003,11 +5020,11 @@
       </c>
       <c r="E56" s="14" t="str">
         <f>ON_Swaps!L27</f>
-        <v>USD_YCONRH_OIS19M#0000</v>
+        <v>USD_YCONRH_OIS19M#0001</v>
       </c>
       <c r="F56" s="13">
         <f>_xll.qlRateHelperQuoteValue($E56,Trigger)</f>
-        <v>2.1099999999999999E-3</v>
+        <v>2.4499999999999999E-3</v>
       </c>
       <c r="G56" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E56,Trigger)</f>
@@ -5025,7 +5042,7 @@
       </c>
       <c r="K56" s="12">
         <f>_xll.qlRateHelperEarliestDate($E56,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L56" s="11">
         <f>_xll.qlRateHelperLatestDate($E56,Trigger)</f>
@@ -5046,11 +5063,11 @@
       </c>
       <c r="E57" s="14" t="str">
         <f>ON_Swaps!L28</f>
-        <v>USD_YCONRH_OIS20M#0000</v>
+        <v>USD_YCONRH_OIS20M#0001</v>
       </c>
       <c r="F57" s="13">
         <f>_xll.qlRateHelperQuoteValue($E57,Trigger)</f>
-        <v>2.2899999999999999E-3</v>
+        <v>2.6900000000000001E-3</v>
       </c>
       <c r="G57" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E57,Trigger)</f>
@@ -5068,11 +5085,11 @@
       </c>
       <c r="K57" s="12">
         <f>_xll.qlRateHelperEarliestDate($E57,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L57" s="11">
         <f>_xll.qlRateHelperLatestDate($E57,Trigger)</f>
-        <v>42366</v>
+        <v>42369</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.2">
@@ -5089,11 +5106,11 @@
       </c>
       <c r="E58" s="14" t="str">
         <f>ON_Swaps!L29</f>
-        <v>USD_YCONRH_OIS21M#0000</v>
+        <v>USD_YCONRH_OIS21M#0001</v>
       </c>
       <c r="F58" s="13">
         <f>_xll.qlRateHelperQuoteValue($E58,Trigger)</f>
-        <v>2.48E-3</v>
+        <v>2.9500000000000004E-3</v>
       </c>
       <c r="G58" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E58,Trigger)</f>
@@ -5111,11 +5128,11 @@
       </c>
       <c r="K58" s="12">
         <f>_xll.qlRateHelperEarliestDate($E58,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L58" s="11">
         <f>_xll.qlRateHelperLatestDate($E58,Trigger)</f>
-        <v>42397</v>
+        <v>42398</v>
       </c>
     </row>
     <row r="59" spans="2:12" x14ac:dyDescent="0.2">
@@ -5132,11 +5149,11 @@
       </c>
       <c r="E59" s="14" t="str">
         <f>ON_Swaps!L30</f>
-        <v>USD_YCONRH_OIS22M#0000</v>
+        <v>USD_YCONRH_OIS22M#0001</v>
       </c>
       <c r="F59" s="13">
         <f>_xll.qlRateHelperQuoteValue($E59,Trigger)</f>
-        <v>2.6800000000000001E-3</v>
+        <v>3.2400000000000003E-3</v>
       </c>
       <c r="G59" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E59,Trigger)</f>
@@ -5154,7 +5171,7 @@
       </c>
       <c r="K59" s="12">
         <f>_xll.qlRateHelperEarliestDate($E59,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L59" s="11">
         <f>_xll.qlRateHelperLatestDate($E59,Trigger)</f>
@@ -5175,11 +5192,11 @@
       </c>
       <c r="E60" s="14" t="str">
         <f>ON_Swaps!L31</f>
-        <v>USD_YCONRH_OIS23M#0000</v>
+        <v>USD_YCONRH_OIS23M#0001</v>
       </c>
       <c r="F60" s="13">
         <f>_xll.qlRateHelperQuoteValue($E60,Trigger)</f>
-        <v>2.8899999999999998E-3</v>
+        <v>3.5499999999999998E-3</v>
       </c>
       <c r="G60" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E60,Trigger)</f>
@@ -5197,11 +5214,11 @@
       </c>
       <c r="K60" s="12">
         <f>_xll.qlRateHelperEarliestDate($E60,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L60" s="11">
         <f>_xll.qlRateHelperLatestDate($E60,Trigger)</f>
-        <v>42458</v>
+        <v>42460</v>
       </c>
     </row>
     <row r="61" spans="2:12" x14ac:dyDescent="0.2">
@@ -5218,11 +5235,11 @@
       </c>
       <c r="E61" s="14" t="str">
         <f>ON_Swaps!L32</f>
-        <v>USD_YCONRH_OIS2Y#0000</v>
+        <v>USD_YCONRH_OIS2Y#0001</v>
       </c>
       <c r="F61" s="13">
         <f>_xll.qlRateHelperQuoteValue($E61,Trigger)</f>
-        <v>3.14E-3</v>
+        <v>3.8500000000000001E-3</v>
       </c>
       <c r="G61" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E61,Trigger)</f>
@@ -5240,11 +5257,11 @@
       </c>
       <c r="K61" s="12">
         <f>_xll.qlRateHelperEarliestDate($E61,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L61" s="11">
         <f>_xll.qlRateHelperLatestDate($E61,Trigger)</f>
-        <v>42488</v>
+        <v>42489</v>
       </c>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.2">
@@ -5261,11 +5278,11 @@
       </c>
       <c r="E62" s="14" t="str">
         <f>ON_Swaps!L33</f>
-        <v>USD_YCONRH_OIS27M#0000</v>
+        <v>USD_YCONRH_OIS27M#0001</v>
       </c>
       <c r="F62" s="13">
         <f>_xll.qlRateHelperQuoteValue($E62,Trigger)</f>
-        <v>3.9000000000000003E-3</v>
+        <v>4.8799999999999998E-3</v>
       </c>
       <c r="G62" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E62,Trigger)</f>
@@ -5282,11 +5299,11 @@
       </c>
       <c r="K62" s="12">
         <f>_xll.qlRateHelperEarliestDate($E62,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L62" s="11">
         <f>_xll.qlRateHelperLatestDate($E62,Trigger)</f>
-        <v>42579</v>
+        <v>42580</v>
       </c>
     </row>
     <row r="63" spans="2:12" x14ac:dyDescent="0.2">
@@ -5303,11 +5320,11 @@
       </c>
       <c r="E63" s="14" t="str">
         <f>ON_Swaps!L34</f>
-        <v>USD_YCONRH_OIS30M#0000</v>
+        <v>USD_YCONRH_OIS30M#0001</v>
       </c>
       <c r="F63" s="13">
         <f>_xll.qlRateHelperQuoteValue($E63,Trigger)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>5.9899999999999997E-3</v>
       </c>
       <c r="G63" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E63,Trigger)</f>
@@ -5324,11 +5341,11 @@
       </c>
       <c r="K63" s="12">
         <f>_xll.qlRateHelperEarliestDate($E63,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L63" s="11">
         <f>_xll.qlRateHelperLatestDate($E63,Trigger)</f>
-        <v>42671</v>
+        <v>42674</v>
       </c>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.2">
@@ -5345,11 +5362,11 @@
       </c>
       <c r="E64" s="14" t="str">
         <f>ON_Swaps!L35</f>
-        <v>USD_YCONRH_OIS33M#0000</v>
+        <v>USD_YCONRH_OIS33M#0001</v>
       </c>
       <c r="F64" s="13">
         <f>_xll.qlRateHelperQuoteValue($E64,Trigger)</f>
-        <v>5.77E-3</v>
+        <v>7.1100000000000009E-3</v>
       </c>
       <c r="G64" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E64,Trigger)</f>
@@ -5366,7 +5383,7 @@
       </c>
       <c r="K64" s="12">
         <f>_xll.qlRateHelperEarliestDate($E64,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L64" s="11">
         <f>_xll.qlRateHelperLatestDate($E64,Trigger)</f>
@@ -5387,11 +5404,11 @@
       </c>
       <c r="E65" s="14" t="str">
         <f>ON_Swaps!L36</f>
-        <v>USD_YCONRH_OIS3Y#0000</v>
+        <v>USD_YCONRH_OIS3Y#0001</v>
       </c>
       <c r="F65" s="13">
         <f>_xll.qlRateHelperQuoteValue($E65,Trigger)</f>
-        <v>6.7900000000000009E-3</v>
+        <v>8.1799999999999998E-3</v>
       </c>
       <c r="G65" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E65,Trigger)</f>
@@ -5408,7 +5425,7 @@
       </c>
       <c r="K65" s="12">
         <f>_xll.qlRateHelperEarliestDate($E65,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L65" s="11">
         <f>_xll.qlRateHelperLatestDate($E65,Trigger)</f>
@@ -5429,11 +5446,11 @@
       </c>
       <c r="E66" s="14" t="str">
         <f>ON_Swaps!L37</f>
-        <v>USD_YCONRH_OIS39M#0000</v>
+        <v>USD_YCONRH_OIS39M#0001</v>
       </c>
       <c r="F66" s="13">
         <f>_xll.qlRateHelperQuoteValue($E66,Trigger)</f>
-        <v>7.8300000000000002E-3</v>
+        <v>9.3200000000000002E-3</v>
       </c>
       <c r="G66" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E66,Trigger)</f>
@@ -5450,11 +5467,11 @@
       </c>
       <c r="K66" s="12">
         <f>_xll.qlRateHelperEarliestDate($E66,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L66" s="11">
         <f>_xll.qlRateHelperLatestDate($E66,Trigger)</f>
-        <v>42944</v>
+        <v>42947</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
@@ -5471,11 +5488,11 @@
       </c>
       <c r="E67" s="14" t="str">
         <f>ON_Swaps!L38</f>
-        <v>USD_YCONRH_OIS42M#0000</v>
+        <v>USD_YCONRH_OIS42M#0001</v>
       </c>
       <c r="F67" s="13">
         <f>_xll.qlRateHelperQuoteValue($E67,Trigger)</f>
-        <v>8.9499999999999996E-3</v>
+        <v>1.0470000000000002E-2</v>
       </c>
       <c r="G67" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E67,Trigger)</f>
@@ -5492,7 +5509,7 @@
       </c>
       <c r="K67" s="12">
         <f>_xll.qlRateHelperEarliestDate($E67,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L67" s="11">
         <f>_xll.qlRateHelperLatestDate($E67,Trigger)</f>
@@ -5513,11 +5530,11 @@
       </c>
       <c r="E68" s="14" t="str">
         <f>ON_Swaps!L39</f>
-        <v>USD_YCONRH_OIS45M#0000</v>
+        <v>USD_YCONRH_OIS45M#0001</v>
       </c>
       <c r="F68" s="13">
         <f>_xll.qlRateHelperQuoteValue($E68,Trigger)</f>
-        <v>9.9699999999999997E-3</v>
+        <v>1.1440000000000001E-2</v>
       </c>
       <c r="G68" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E68,Trigger)</f>
@@ -5534,11 +5551,11 @@
       </c>
       <c r="K68" s="12">
         <f>_xll.qlRateHelperEarliestDate($E68,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L68" s="11">
         <f>_xll.qlRateHelperLatestDate($E68,Trigger)</f>
-        <v>43129</v>
+        <v>43130</v>
       </c>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
@@ -5555,11 +5572,11 @@
       </c>
       <c r="E69" s="14" t="str">
         <f>ON_Swaps!L40</f>
-        <v>USD_YCONRH_OIS4Y#0000</v>
+        <v>USD_YCONRH_OIS4Y#0001</v>
       </c>
       <c r="F69" s="13">
         <f>_xll.qlRateHelperQuoteValue($E69,Trigger)</f>
-        <v>1.1089999999999999E-2</v>
+        <v>1.2460000000000001E-2</v>
       </c>
       <c r="G69" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E69,Trigger)</f>
@@ -5576,7 +5593,7 @@
       </c>
       <c r="K69" s="12">
         <f>_xll.qlRateHelperEarliestDate($E69,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L69" s="11">
         <f>_xll.qlRateHelperLatestDate($E69,Trigger)</f>
@@ -5597,11 +5614,11 @@
       </c>
       <c r="E70" s="14" t="str">
         <f>ON_Swaps!L41</f>
-        <v>USD_YCONRH_OIS51M#0000</v>
+        <v>USD_YCONRH_OIS51M#0001</v>
       </c>
       <c r="F70" s="13">
         <f>_xll.qlRateHelperQuoteValue($E70,Trigger)</f>
-        <v>1.2070000000000001E-2</v>
+        <v>1.3380000000000001E-2</v>
       </c>
       <c r="G70" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E70,Trigger)</f>
@@ -5618,7 +5635,7 @@
       </c>
       <c r="K70" s="12">
         <f>_xll.qlRateHelperEarliestDate($E70,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L70" s="11">
         <f>_xll.qlRateHelperLatestDate($E70,Trigger)</f>
@@ -5639,11 +5656,11 @@
       </c>
       <c r="E71" s="14" t="str">
         <f>ON_Swaps!L42</f>
-        <v>USD_YCONRH_OIS54M#0000</v>
+        <v>USD_YCONRH_OIS54M#0001</v>
       </c>
       <c r="F71" s="13">
         <f>_xll.qlRateHelperQuoteValue($E71,Trigger)</f>
-        <v>1.3140000000000001E-2</v>
+        <v>1.4329999999999999E-2</v>
       </c>
       <c r="G71" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E71,Trigger)</f>
@@ -5660,11 +5677,11 @@
       </c>
       <c r="K71" s="12">
         <f>_xll.qlRateHelperEarliestDate($E71,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L71" s="11">
         <f>_xll.qlRateHelperLatestDate($E71,Trigger)</f>
-        <v>43402</v>
+        <v>43403</v>
       </c>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
@@ -5681,11 +5698,11 @@
       </c>
       <c r="E72" s="14" t="str">
         <f>ON_Swaps!L43</f>
-        <v>USD_YCONRH_OIS57M#0000</v>
+        <v>USD_YCONRH_OIS57M#0001</v>
       </c>
       <c r="F72" s="13">
         <f>_xll.qlRateHelperQuoteValue($E72,Trigger)</f>
-        <v>1.4079999999999999E-2</v>
+        <v>1.5190000000000002E-2</v>
       </c>
       <c r="G72" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E72,Trigger)</f>
@@ -5702,11 +5719,11 @@
       </c>
       <c r="K72" s="12">
         <f>_xll.qlRateHelperEarliestDate($E72,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L72" s="11">
         <f>_xll.qlRateHelperLatestDate($E72,Trigger)</f>
-        <v>43493</v>
+        <v>43495</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
@@ -5723,11 +5740,11 @@
       </c>
       <c r="E73" s="14" t="str">
         <f>ON_Swaps!L44</f>
-        <v>USD_YCONRH_OIS5Y#0000</v>
+        <v>USD_YCONRH_OIS5Y#0001</v>
       </c>
       <c r="F73" s="13">
         <f>_xll.qlRateHelperQuoteValue($E73,Trigger)</f>
-        <v>1.5069999999999998E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="G73" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E73,Trigger)</f>
@@ -5745,11 +5762,11 @@
       </c>
       <c r="K73" s="12">
         <f>_xll.qlRateHelperEarliestDate($E73,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L73" s="11">
         <f>_xll.qlRateHelperLatestDate($E73,Trigger)</f>
-        <v>43584</v>
+        <v>43585</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
@@ -5766,11 +5783,11 @@
       </c>
       <c r="E74" s="14" t="str">
         <f>ON_Swaps!L45</f>
-        <v>USD_YCONRH_OIS6Y#0000</v>
+        <v>USD_YCONRH_OIS6Y#0001</v>
       </c>
       <c r="F74" s="13">
         <f>_xll.qlRateHelperQuoteValue($E74,Trigger)</f>
-        <v>1.8530000000000001E-2</v>
+        <v>1.881E-2</v>
       </c>
       <c r="G74" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E74,Trigger)</f>
@@ -5788,11 +5805,11 @@
       </c>
       <c r="K74" s="12">
         <f>_xll.qlRateHelperEarliestDate($E74,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L74" s="11">
         <f>_xll.qlRateHelperLatestDate($E74,Trigger)</f>
-        <v>43949</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
@@ -5809,11 +5826,11 @@
       </c>
       <c r="E75" s="14" t="str">
         <f>ON_Swaps!L46</f>
-        <v>USD_YCONRH_OIS7Y#0000</v>
+        <v>USD_YCONRH_OIS7Y#0001</v>
       </c>
       <c r="F75" s="13">
         <f>_xll.qlRateHelperQuoteValue($E75,Trigger)</f>
-        <v>2.1360000000000001E-2</v>
+        <v>2.0979999999999999E-2</v>
       </c>
       <c r="G75" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E75,Trigger)</f>
@@ -5831,11 +5848,11 @@
       </c>
       <c r="K75" s="12">
         <f>_xll.qlRateHelperEarliestDate($E75,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L75" s="11">
         <f>_xll.qlRateHelperLatestDate($E75,Trigger)</f>
-        <v>44314</v>
+        <v>44316</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.2">
@@ -5852,11 +5869,11 @@
       </c>
       <c r="E76" s="14" t="str">
         <f>ON_Swaps!L47</f>
-        <v>USD_YCONRH_OIS8Y#0000</v>
+        <v>USD_YCONRH_OIS8Y#0001</v>
       </c>
       <c r="F76" s="13">
         <f>_xll.qlRateHelperQuoteValue($E76,Trigger)</f>
-        <v>2.3700000000000002E-2</v>
+        <v>2.274E-2</v>
       </c>
       <c r="G76" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E76,Trigger)</f>
@@ -5874,11 +5891,11 @@
       </c>
       <c r="K76" s="12">
         <f>_xll.qlRateHelperEarliestDate($E76,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L76" s="11">
         <f>_xll.qlRateHelperLatestDate($E76,Trigger)</f>
-        <v>44679</v>
+        <v>44680</v>
       </c>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.2">
@@ -5895,11 +5912,11 @@
       </c>
       <c r="E77" s="14" t="str">
         <f>ON_Swaps!L48</f>
-        <v>USD_YCONRH_OIS9Y#0000</v>
+        <v>USD_YCONRH_OIS9Y#0001</v>
       </c>
       <c r="F77" s="13">
         <f>_xll.qlRateHelperQuoteValue($E77,Trigger)</f>
-        <v>2.5600000000000001E-2</v>
+        <v>2.4150000000000001E-2</v>
       </c>
       <c r="G77" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E77,Trigger)</f>
@@ -5917,7 +5934,7 @@
       </c>
       <c r="K77" s="12">
         <f>_xll.qlRateHelperEarliestDate($E77,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L77" s="11">
         <f>_xll.qlRateHelperLatestDate($E77,Trigger)</f>
@@ -5938,11 +5955,11 @@
       </c>
       <c r="E78" s="14" t="str">
         <f>ON_Swaps!L49</f>
-        <v>USD_YCONRH_OIS10Y#0000</v>
+        <v>USD_YCONRH_OIS10Y#0001</v>
       </c>
       <c r="F78" s="13">
         <f>_xll.qlRateHelperQuoteValue($E78,Trigger)</f>
-        <v>2.7160000000000004E-2</v>
+        <v>2.5329999999999998E-2</v>
       </c>
       <c r="G78" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E78,Trigger)</f>
@@ -5960,11 +5977,11 @@
       </c>
       <c r="K78" s="12">
         <f>_xll.qlRateHelperEarliestDate($E78,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L78" s="11">
         <f>_xll.qlRateHelperLatestDate($E78,Trigger)</f>
-        <v>45411</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.2">
@@ -5981,11 +5998,11 @@
       </c>
       <c r="E79" s="14" t="str">
         <f>ON_Swaps!L50</f>
-        <v>USD_YCONRH_OIS12Y#0000</v>
+        <v>USD_YCONRH_OIS12Y#0001</v>
       </c>
       <c r="F79" s="13">
         <f>_xll.qlRateHelperQuoteValue($E79,Trigger)</f>
-        <v>2.9679999999999998E-2</v>
+        <v>2.724E-2</v>
       </c>
       <c r="G79" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E79,Trigger)</f>
@@ -6003,11 +6020,11 @@
       </c>
       <c r="K79" s="12">
         <f>_xll.qlRateHelperEarliestDate($E79,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L79" s="11">
         <f>_xll.qlRateHelperLatestDate($E79,Trigger)</f>
-        <v>46140</v>
+        <v>46142</v>
       </c>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.2">
@@ -6024,11 +6041,11 @@
       </c>
       <c r="E80" s="14" t="str">
         <f>ON_Swaps!L51</f>
-        <v>USD_YCONRH_OIS15Y#0000</v>
+        <v>USD_YCONRH_OIS15Y#0001</v>
       </c>
       <c r="F80" s="13">
         <f>_xll.qlRateHelperQuoteValue($E80,Trigger)</f>
-        <v>3.2070000000000001E-2</v>
+        <v>2.92E-2</v>
       </c>
       <c r="G80" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E80,Trigger)</f>
@@ -6046,7 +6063,7 @@
       </c>
       <c r="K80" s="12">
         <f>_xll.qlRateHelperEarliestDate($E80,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L80" s="11">
         <f>_xll.qlRateHelperLatestDate($E80,Trigger)</f>
@@ -6064,11 +6081,11 @@
       </c>
       <c r="E81" s="14" t="str">
         <f>ON_Swaps!L52</f>
-        <v>USD_YCONRH_OIS20Y#0000</v>
+        <v>USD_YCONRH_OIS20Y#0001</v>
       </c>
       <c r="F81" s="13">
         <f>_xll.qlRateHelperQuoteValue($E81,Trigger)</f>
-        <v>3.4079999999999999E-2</v>
+        <v>3.0869999999999998E-2</v>
       </c>
       <c r="G81" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E81,Trigger)</f>
@@ -6086,7 +6103,7 @@
       </c>
       <c r="K81" s="12">
         <f>_xll.qlRateHelperEarliestDate($E81,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L81" s="11">
         <f>_xll.qlRateHelperLatestDate($E81,Trigger)</f>
@@ -6104,11 +6121,11 @@
       </c>
       <c r="E82" s="14" t="str">
         <f>ON_Swaps!L53</f>
-        <v>USD_YCONRH_OIS25Y#0000</v>
+        <v>USD_YCONRH_OIS25Y#0001</v>
       </c>
       <c r="F82" s="13">
         <f>_xll.qlRateHelperQuoteValue($E82,Trigger)</f>
-        <v>3.4970000000000001E-2</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="G82" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E82,Trigger)</f>
@@ -6125,11 +6142,11 @@
       </c>
       <c r="K82" s="12">
         <f>_xll.qlRateHelperEarliestDate($E82,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L82" s="11">
         <f>_xll.qlRateHelperLatestDate($E82,Trigger)</f>
-        <v>50888</v>
+        <v>50889</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.2">
@@ -6143,7 +6160,7 @@
       </c>
       <c r="E83" s="14" t="str">
         <f>ON_Swaps!L54</f>
-        <v>USD_YCONRH_OIS27Y#0000</v>
+        <v>USD_YCONRH_OIS27Y#0001</v>
       </c>
       <c r="F83" s="13" t="e">
         <f>_xll.qlRateHelperQuoteValue($E83,Trigger)</f>
@@ -6165,11 +6182,11 @@
       </c>
       <c r="K83" s="12">
         <f>_xll.qlRateHelperEarliestDate($E83,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L83" s="11">
         <f>_xll.qlRateHelperLatestDate($E83,Trigger)</f>
-        <v>51620</v>
+        <v>51621</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.2">
@@ -6186,11 +6203,11 @@
       </c>
       <c r="E84" s="14" t="str">
         <f>ON_Swaps!L55</f>
-        <v>USD_YCONRH_OIS30Y#0000</v>
+        <v>USD_YCONRH_OIS30Y#0001</v>
       </c>
       <c r="F84" s="13">
         <f>_xll.qlRateHelperQuoteValue($E84,Trigger)</f>
-        <v>3.5490000000000001E-2</v>
+        <v>3.1910000000000001E-2</v>
       </c>
       <c r="G84" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E84,Trigger)</f>
@@ -6207,11 +6224,11 @@
       </c>
       <c r="K84" s="12">
         <f>_xll.qlRateHelperEarliestDate($E84,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L84" s="11">
         <f>_xll.qlRateHelperLatestDate($E84,Trigger)</f>
-        <v>52715</v>
+        <v>52716</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.2">
@@ -6228,11 +6245,11 @@
       </c>
       <c r="E85" s="14" t="str">
         <f>ON_Swaps!L56</f>
-        <v>USD_YCONRH_OIS35Y#0000</v>
+        <v>USD_YCONRH_OIS35Y#0001</v>
       </c>
       <c r="F85" s="13">
         <f>_xll.qlRateHelperQuoteValue($E85,Trigger)</f>
-        <v>3.567E-2</v>
+        <v>3.1959999999999995E-2</v>
       </c>
       <c r="G85" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E85,Trigger)</f>
@@ -6250,11 +6267,11 @@
       </c>
       <c r="K85" s="12">
         <f>_xll.qlRateHelperEarliestDate($E85,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L85" s="11">
         <f>_xll.qlRateHelperLatestDate($E85,Trigger)</f>
-        <v>54541</v>
+        <v>54543</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.2">
@@ -6271,11 +6288,11 @@
       </c>
       <c r="E86" s="14" t="str">
         <f>ON_Swaps!L57</f>
-        <v>USD_YCONRH_OIS40Y#0000</v>
+        <v>USD_YCONRH_OIS40Y#0001</v>
       </c>
       <c r="F86" s="13">
         <f>_xll.qlRateHelperQuoteValue($E86,Trigger)</f>
-        <v>3.5680000000000003E-2</v>
+        <v>3.1989999999999998E-2</v>
       </c>
       <c r="G86" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E86,Trigger)</f>
@@ -6293,11 +6310,11 @@
       </c>
       <c r="K86" s="12">
         <f>_xll.qlRateHelperEarliestDate($E86,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L86" s="11">
         <f>_xll.qlRateHelperLatestDate($E86,Trigger)</f>
-        <v>56367</v>
+        <v>56369</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.2">
@@ -6314,11 +6331,11 @@
       </c>
       <c r="E87" s="14" t="str">
         <f>ON_Swaps!L58</f>
-        <v>USD_YCONRH_OIS45Y#0000</v>
+        <v>USD_YCONRH_OIS45Y#0001</v>
       </c>
       <c r="F87" s="13">
         <f>_xll.qlRateHelperQuoteValue($E87,Trigger)</f>
-        <v>3.5590000000000004E-2</v>
+        <v>3.1910000000000001E-2</v>
       </c>
       <c r="G87" s="13" t="e">
         <f>_xll.qlSwapRateHelperSpread($E87,Trigger)</f>
@@ -6336,11 +6353,11 @@
       </c>
       <c r="K87" s="12">
         <f>_xll.qlRateHelperEarliestDate($E87,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L87" s="11">
         <f>_xll.qlRateHelperLatestDate($E87,Trigger)</f>
-        <v>58193</v>
+        <v>58195</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.2">
@@ -6357,11 +6374,11 @@
       </c>
       <c r="E88" s="8" t="str">
         <f>ON_Swaps!L59</f>
-        <v>USD_YCONRH_OIS50Y#0000</v>
+        <v>USD_YCONRH_OIS50Y#0001</v>
       </c>
       <c r="F88" s="7">
         <f>_xll.qlRateHelperQuoteValue($E88,Trigger)</f>
-        <v>3.5499999999999997E-2</v>
+        <v>3.1799999999999995E-2</v>
       </c>
       <c r="G88" s="7" t="e">
         <f>_xll.qlSwapRateHelperSpread($E88,Trigger)</f>
@@ -6379,11 +6396,11 @@
       </c>
       <c r="K88" s="4">
         <f>_xll.qlRateHelperEarliestDate($E88,Trigger)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="L88" s="3">
         <f>_xll.qlRateHelperLatestDate($E88,Trigger)</f>
-        <v>60020</v>
+        <v>60022</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.2">
@@ -7993,8 +8010,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M126"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -8050,7 +8067,7 @@
       </c>
       <c r="E2" s="39">
         <f>_xll.qlRateHelperRate($D2)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F2" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D2)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D2)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D2)),_xll.qlSwapRateHelperSpread($D2))</f>
@@ -8058,14 +8075,14 @@
       </c>
       <c r="G2" s="38">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41753</v>
+        <v>41757</v>
       </c>
       <c r="H2" s="37">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41754</v>
+        <v>41758</v>
       </c>
       <c r="I2" s="190">
-        <v>0.99999583335069442</v>
+        <v>0.99999638890192899</v>
       </c>
       <c r="L2" s="177" t="s">
         <v>171</v>
@@ -8086,7 +8103,7 @@
       </c>
       <c r="E3" s="39">
         <f>_xll.qlRateHelperRate($D3)</f>
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F3" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D3)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D3)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D3)),_xll.qlSwapRateHelperSpread($D3))</f>
@@ -8094,18 +8111,18 @@
       </c>
       <c r="G3" s="38">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41754</v>
+        <v>41758</v>
       </c>
       <c r="H3" s="37">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="I3" s="190">
-        <v>0.99998333355895508</v>
+        <v>0.99999277781689799</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J37" si="0">H3-H2</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L3" s="177" t="s">
         <v>172</v>
@@ -8126,7 +8143,7 @@
       </c>
       <c r="E4" s="39">
         <f>_xll.qlRateHelperRate($D4)</f>
-        <v>7.9000000000000001E-4</v>
+        <v>1.06E-3</v>
       </c>
       <c r="F4" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D4)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D4)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D4)),_xll.qlSwapRateHelperSpread($D4))</f>
@@ -8134,14 +8151,14 @@
       </c>
       <c r="G4" s="38">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H4" s="37">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41764</v>
+        <v>41766</v>
       </c>
       <c r="I4" s="190">
-        <v>0.99996797293981521</v>
+        <v>0.99997216727937177</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" si="0"/>
@@ -8166,7 +8183,7 @@
       </c>
       <c r="E5" s="39">
         <f>_xll.qlRateHelperRate($D5)</f>
-        <v>7.9000000000000001E-4</v>
+        <v>9.8999999999999999E-4</v>
       </c>
       <c r="F5" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D5)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D5)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D5)),_xll.qlSwapRateHelperSpread($D5))</f>
@@ -8174,14 +8191,14 @@
       </c>
       <c r="G5" s="38">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H5" s="37">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41771</v>
+        <v>41773</v>
       </c>
       <c r="I5" s="190">
-        <v>0.9999526127925612</v>
+        <v>0.99995427957690763</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="0"/>
@@ -8207,7 +8224,7 @@
       </c>
       <c r="E6" s="39">
         <f>_xll.qlRateHelperRate($D6)</f>
-        <v>8.0000000000000004E-4</v>
+        <v>9.7000000000000005E-4</v>
       </c>
       <c r="F6" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D6)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D6)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D6)),_xll.qlSwapRateHelperSpread($D6))</f>
@@ -8215,14 +8232,14 @@
       </c>
       <c r="G6" s="38">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H6" s="37">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41778</v>
+        <v>41780</v>
       </c>
       <c r="I6" s="190">
-        <v>0.99993666984781526</v>
+        <v>0.99993619809376078</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="0"/>
@@ -8238,7 +8255,7 @@
     <row r="7" spans="1:13" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_RateHelpersSelected#0000</v>
+        <v>USD_YCONRH_RateHelpersSelected#0001</v>
       </c>
       <c r="B7" s="41" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -8249,7 +8266,7 @@
       </c>
       <c r="E7" s="39">
         <f>_xll.qlRateHelperRate($D7)</f>
-        <v>8.1000000000000006E-4</v>
+        <v>9.6000000000000002E-4</v>
       </c>
       <c r="F7" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D7)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D7)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D7)),_xll.qlSwapRateHelperSpread($D7))</f>
@@ -8257,14 +8274,14 @@
       </c>
       <c r="G7" s="38">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H7" s="37">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41787</v>
+        <v>41789</v>
       </c>
       <c r="I7" s="190">
-        <v>0.99991583923990313</v>
+        <v>0.99991278479417467</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" si="0"/>
@@ -8283,7 +8300,7 @@
       </c>
       <c r="E8" s="39">
         <f>_xll.qlRateHelperRate($D8)</f>
-        <v>8.1999999999999998E-4</v>
+        <v>9.5E-4</v>
       </c>
       <c r="F8" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D8)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D8)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D8)),_xll.qlSwapRateHelperSpread($D8))</f>
@@ -8291,18 +8308,18 @@
       </c>
       <c r="G8" s="38">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H8" s="37">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
         <v>41820</v>
       </c>
       <c r="I8" s="190">
-        <v>0.99983985653954155</v>
+        <v>0.99983183266494535</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L8" s="177" t="s">
         <v>177</v>
@@ -8317,7 +8334,7 @@
       </c>
       <c r="E9" s="39">
         <f>_xll.qlRateHelperRate($D9)</f>
-        <v>8.7999999999999992E-4</v>
+        <v>9.5E-4</v>
       </c>
       <c r="F9" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D9)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D9)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D9)),_xll.qlSwapRateHelperSpread($D9))</f>
@@ -8325,18 +8342,18 @@
       </c>
       <c r="G9" s="38">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H9" s="37">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41848</v>
+        <v>41851</v>
       </c>
       <c r="I9" s="190">
-        <v>0.99976094229156964</v>
+        <v>0.99975006071890637</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L9" s="177" t="s">
         <v>178</v>
@@ -8351,7 +8368,7 @@
       </c>
       <c r="E10" s="39">
         <f>_xll.qlRateHelperRate($D10)</f>
-        <v>9.1E-4</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="F10" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D10)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D10)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D10)),_xll.qlSwapRateHelperSpread($D10))</f>
@@ -8359,18 +8376,18 @@
       </c>
       <c r="G10" s="38">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H10" s="37">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41879</v>
+        <v>41880</v>
       </c>
       <c r="I10" s="190">
-        <v>0.99967504488270098</v>
+        <v>0.99966349976744673</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L10" s="177" t="s">
         <v>179</v>
@@ -8385,7 +8402,7 @@
       </c>
       <c r="E11" s="39">
         <f>_xll.qlRateHelperRate($D11)</f>
-        <v>9.2999999999999995E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F11" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D11)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D11)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D11)),_xll.qlSwapRateHelperSpread($D11))</f>
@@ -8393,14 +8410,14 @@
       </c>
       <c r="G11" s="38">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H11" s="37">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
-        <v>41911</v>
+        <v>41912</v>
       </c>
       <c r="I11" s="190">
-        <v>0.99958566506204005</v>
+        <v>0.99956796143333781</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="0"/>
@@ -8419,7 +8436,7 @@
       </c>
       <c r="E12" s="39">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>9.6000000000000002E-4</v>
+        <v>1.0200000000000001E-3</v>
       </c>
       <c r="F12" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -8427,18 +8444,18 @@
       </c>
       <c r="G12" s="38">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H12" s="37">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41940</v>
+        <v>41943</v>
       </c>
       <c r="I12" s="190">
-        <v>0.99949557971605363</v>
+        <v>0.9994717198935934</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L12" s="177" t="s">
         <v>181</v>
@@ -8453,7 +8470,7 @@
       </c>
       <c r="E13" s="39">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>1.01E-3</v>
+        <v>1.0499999999999999E-3</v>
       </c>
       <c r="F13" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -8461,18 +8478,18 @@
       </c>
       <c r="G13" s="38">
         <f>_xll.qlRateHelperEarliestDate($D13)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H13" s="37">
         <f>_xll.qlRateHelperLatestDate($D13)</f>
         <v>41971</v>
       </c>
       <c r="I13" s="190">
-        <v>0.99938331492093568</v>
+        <v>0.9993748310463676</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L13" s="177" t="s">
         <v>182</v>
@@ -8487,7 +8504,7 @@
       </c>
       <c r="E14" s="39">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>1.0499999999999999E-3</v>
+        <v>1.08E-3</v>
       </c>
       <c r="F14" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -8495,18 +8512,18 @@
       </c>
       <c r="G14" s="38">
         <f>_xll.qlRateHelperEarliestDate($D14)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H14" s="37">
         <f>_xll.qlRateHelperLatestDate($D14)</f>
-        <v>42002</v>
+        <v>42004</v>
       </c>
       <c r="I14" s="190">
-        <v>0.99926927239139207</v>
+        <v>0.9992583229495301</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L14" s="177" t="s">
         <v>183</v>
@@ -8521,7 +8538,7 @@
       </c>
       <c r="E15" s="39">
         <f>_xll.qlRateHelperRate($D15)</f>
-        <v>1.1100000000000001E-3</v>
+        <v>1.1200000000000001E-3</v>
       </c>
       <c r="F15" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D15)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D15)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D15)),_xll.qlSwapRateHelperSpread($D15))</f>
@@ -8529,14 +8546,14 @@
       </c>
       <c r="G15" s="38">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H15" s="37">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42032</v>
+        <v>42034</v>
       </c>
       <c r="I15" s="190">
-        <v>0.99913614936563888</v>
+        <v>0.99913795978463771</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="0"/>
@@ -8563,18 +8580,18 @@
       </c>
       <c r="G16" s="38">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H16" s="37">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
         <v>42062</v>
       </c>
       <c r="I16" s="190">
-        <v>0.99899308166675305</v>
+        <v>0.99900900370050383</v>
       </c>
       <c r="J16" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L16" s="177" t="s">
         <v>185</v>
@@ -8589,7 +8606,7 @@
       </c>
       <c r="E17" s="39">
         <f>_xll.qlRateHelperRate($D17)</f>
-        <v>1.2099999999999999E-3</v>
+        <v>1.23E-3</v>
       </c>
       <c r="F17" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D17)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D17)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D17)),_xll.qlSwapRateHelperSpread($D17))</f>
@@ -8597,18 +8614,18 @@
       </c>
       <c r="G17" s="38">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H17" s="37">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
-        <v>42093</v>
+        <v>42094</v>
       </c>
       <c r="I17" s="190">
-        <v>0.99885529298141484</v>
+        <v>0.99884951131374033</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L17" s="177" t="s">
         <v>186</v>
@@ -8623,7 +8640,7 @@
       </c>
       <c r="E18" s="39">
         <f>_xll.qlRateHelperRate($D18)</f>
-        <v>1.2900000000000001E-3</v>
+        <v>1.31E-3</v>
       </c>
       <c r="F18" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D18)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D18)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D18)),_xll.qlSwapRateHelperSpread($D18))</f>
@@ -8631,18 +8648,18 @@
       </c>
       <c r="G18" s="38">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H18" s="37">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
-        <v>42122</v>
+        <v>42124</v>
       </c>
       <c r="I18" s="190">
-        <v>0.9986771470736785</v>
+        <v>0.99866635471271514</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L18" s="177" t="s">
         <v>187</v>
@@ -8657,7 +8674,7 @@
       </c>
       <c r="E19" s="39">
         <f>_xll.qlRateHelperRate($D19)</f>
-        <v>1.3700000000000001E-3</v>
+        <v>1.4000000000000002E-3</v>
       </c>
       <c r="F19" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D19)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D19)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D19)),_xll.qlSwapRateHelperSpread($D19))</f>
@@ -8665,18 +8682,18 @@
       </c>
       <c r="G19" s="38">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H19" s="37">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>42152</v>
+        <v>42153</v>
       </c>
       <c r="I19" s="190">
-        <v>0.99848214988183881</v>
+        <v>0.99846262201212022</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L19" s="177" t="s">
         <v>188</v>
@@ -8691,7 +8708,7 @@
       </c>
       <c r="E20" s="39">
         <f>_xll.qlRateHelperRate($D20)</f>
-        <v>1.4599999999999999E-3</v>
+        <v>1.5200000000000003E-3</v>
       </c>
       <c r="F20" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D20)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D20)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D20)),_xll.qlSwapRateHelperSpread($D20))</f>
@@ -8699,14 +8716,14 @@
       </c>
       <c r="G20" s="38">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H20" s="37">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>42184</v>
+        <v>42185</v>
       </c>
       <c r="I20" s="190">
-        <v>0.99825400854613044</v>
+        <v>0.9981966309136151</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="0"/>
@@ -8725,7 +8742,7 @@
       </c>
       <c r="E21" s="39">
         <f>_xll.qlRateHelperRate($D21)</f>
-        <v>1.56E-3</v>
+        <v>1.6599999999999998E-3</v>
       </c>
       <c r="F21" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D21)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D21)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D21)),_xll.qlSwapRateHelperSpread($D21))</f>
@@ -8733,18 +8750,18 @@
       </c>
       <c r="G21" s="38">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H21" s="37">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>42213</v>
+        <v>42216</v>
       </c>
       <c r="I21" s="190">
-        <v>0.99801021051165528</v>
+        <v>0.99788864032392377</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L21" s="177" t="s">
         <v>190</v>
@@ -8759,7 +8776,7 @@
       </c>
       <c r="E22" s="39">
         <f>_xll.qlRateHelperRate($D22)</f>
-        <v>1.6800000000000001E-3</v>
+        <v>1.83E-3</v>
       </c>
       <c r="F22" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D22)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D22)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D22)),_xll.qlSwapRateHelperSpread($D22))</f>
@@ -8767,14 +8784,14 @@
       </c>
       <c r="G22" s="38">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H22" s="37">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>42244</v>
+        <v>42247</v>
       </c>
       <c r="I22" s="190">
-        <v>0.99771422152165334</v>
+        <v>0.99751613865223243</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" si="0"/>
@@ -8793,7 +8810,7 @@
       </c>
       <c r="E23" s="39">
         <f>_xll.qlRateHelperRate($D23)</f>
-        <v>1.81E-3</v>
+        <v>2.0100000000000001E-3</v>
       </c>
       <c r="F23" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D23)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D23)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D23)),_xll.qlSwapRateHelperSpread($D23))</f>
@@ -8801,18 +8818,18 @@
       </c>
       <c r="G23" s="38">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H23" s="37">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
-        <v>42275</v>
+        <v>42277</v>
       </c>
       <c r="I23" s="190">
-        <v>0.99738338511991209</v>
+        <v>0.99710580137736304</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L23" s="177" t="s">
         <v>192</v>
@@ -8827,7 +8844,7 @@
       </c>
       <c r="E24" s="39">
         <f>_xll.qlRateHelperRate($D24)</f>
-        <v>1.9500000000000001E-3</v>
+        <v>2.2099999999999997E-3</v>
       </c>
       <c r="F24" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D24)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D24)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D24)),_xll.qlSwapRateHelperSpread($D24))</f>
@@ -8835,14 +8852,14 @@
       </c>
       <c r="G24" s="38">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H24" s="37">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>42305</v>
+        <v>42307</v>
       </c>
       <c r="I24" s="190">
-        <v>0.99702056897709634</v>
+        <v>0.99663543480598804</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="0"/>
@@ -8861,7 +8878,7 @@
       </c>
       <c r="E25" s="39">
         <f>_xll.qlRateHelperRate($D25)</f>
-        <v>2.1099999999999999E-3</v>
+        <v>2.4499999999999999E-3</v>
       </c>
       <c r="F25" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D25)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D25)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D25)),_xll.qlSwapRateHelperSpread($D25))</f>
@@ -8869,18 +8886,18 @@
       </c>
       <c r="G25" s="38">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H25" s="37">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
         <v>42338</v>
       </c>
       <c r="I25" s="190">
-        <v>0.9965851811506774</v>
+        <v>0.99606141008076721</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L25" s="177" t="s">
         <v>194</v>
@@ -8895,7 +8912,7 @@
       </c>
       <c r="E26" s="39">
         <f>_xll.qlRateHelperRate($D26)</f>
-        <v>2.2899999999999999E-3</v>
+        <v>2.6900000000000001E-3</v>
       </c>
       <c r="F26" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D26)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D26)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D26)),_xll.qlSwapRateHelperSpread($D26))</f>
@@ -8903,18 +8920,18 @@
       </c>
       <c r="G26" s="38">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H26" s="37">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>42366</v>
+        <v>42369</v>
       </c>
       <c r="I26" s="190">
-        <v>0.99611851279897445</v>
+        <v>0.9954466953032477</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L26" s="177" t="s">
         <v>195</v>
@@ -8929,7 +8946,7 @@
       </c>
       <c r="E27" s="39">
         <f>_xll.qlRateHelperRate($D27)</f>
-        <v>2.48E-3</v>
+        <v>2.9500000000000004E-3</v>
       </c>
       <c r="F27" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D27)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D27)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D27)),_xll.qlSwapRateHelperSpread($D27))</f>
@@ -8937,18 +8954,18 @@
       </c>
       <c r="G27" s="38">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H27" s="37">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>42397</v>
+        <v>42398</v>
       </c>
       <c r="I27" s="190">
-        <v>0.99558613273657359</v>
+        <v>0.9947722544538099</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L27" s="177" t="s">
         <v>196</v>
@@ -8963,7 +8980,7 @@
       </c>
       <c r="E28" s="39">
         <f>_xll.qlRateHelperRate($D28)</f>
-        <v>2.6800000000000001E-3</v>
+        <v>3.2400000000000003E-3</v>
       </c>
       <c r="F28" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D28)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D28)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D28)),_xll.qlSwapRateHelperSpread($D28))</f>
@@ -8971,18 +8988,18 @@
       </c>
       <c r="G28" s="38">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H28" s="37">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
         <v>42429</v>
       </c>
       <c r="I28" s="190">
-        <v>0.99499569843087665</v>
+        <v>0.99398367365747853</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L28" s="177" t="s">
         <v>197</v>
@@ -8997,7 +9014,7 @@
       </c>
       <c r="E29" s="39">
         <f>_xll.qlRateHelperRate($D29)</f>
-        <v>2.8899999999999998E-3</v>
+        <v>3.5499999999999998E-3</v>
       </c>
       <c r="F29" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D29)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D29)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D29)),_xll.qlSwapRateHelperSpread($D29))</f>
@@ -9005,18 +9022,18 @@
       </c>
       <c r="G29" s="38">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H29" s="37">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>42458</v>
+        <v>42460</v>
       </c>
       <c r="I29" s="190">
-        <v>0.99437491022169933</v>
+        <v>0.99310777536253569</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L29" s="177" t="s">
         <v>198</v>
@@ -9031,7 +9048,7 @@
       </c>
       <c r="E30" s="39">
         <f>_xll.qlRateHelperRate($D30)</f>
-        <v>3.14E-3</v>
+        <v>3.8500000000000001E-3</v>
       </c>
       <c r="F30" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D30)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D30)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D30)),_xll.qlSwapRateHelperSpread($D30))</f>
@@ -9039,18 +9056,18 @@
       </c>
       <c r="G30" s="38">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H30" s="37">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>42488</v>
+        <v>42489</v>
       </c>
       <c r="I30" s="190">
-        <v>0.99363192956729851</v>
+        <v>0.99222140275805149</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L30" s="177" t="s">
         <v>199</v>
@@ -9065,7 +9082,7 @@
       </c>
       <c r="E31" s="39">
         <f>_xll.qlRateHelperRate($D31)</f>
-        <v>6.7900000000000009E-3</v>
+        <v>8.1799999999999998E-3</v>
       </c>
       <c r="F31" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D31)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D31)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D31)),_xll.qlSwapRateHelperSpread($D31))</f>
@@ -9073,18 +9090,18 @@
       </c>
       <c r="G31" s="38">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H31" s="37">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
         <v>42853</v>
       </c>
       <c r="I31" s="190">
-        <v>0.97950571150064347</v>
+        <v>0.97541359155410901</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L31" s="177" t="s">
         <v>200</v>
@@ -9099,7 +9116,7 @@
       </c>
       <c r="E32" s="39">
         <f>_xll.qlRateHelperRate($D32)</f>
-        <v>1.1089999999999999E-2</v>
+        <v>1.2460000000000001E-2</v>
       </c>
       <c r="F32" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D32)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D32)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D32)),_xll.qlSwapRateHelperSpread($D32))</f>
@@ -9107,14 +9124,14 @@
       </c>
       <c r="G32" s="38">
         <f>_xll.qlRateHelperEarliestDate($D32)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H32" s="37">
         <f>_xll.qlRateHelperLatestDate($D32)</f>
         <v>43220</v>
       </c>
       <c r="I32" s="190">
-        <v>0.95573239086157702</v>
+        <v>0.95047982941296616</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="0"/>
@@ -9133,7 +9150,7 @@
       </c>
       <c r="E33" s="39">
         <f>_xll.qlRateHelperRate($D33)</f>
-        <v>1.5069999999999998E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F33" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D33)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D33)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D33)),_xll.qlSwapRateHelperSpread($D33))</f>
@@ -9141,18 +9158,18 @@
       </c>
       <c r="G33" s="38">
         <f>_xll.qlRateHelperEarliestDate($D33)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H33" s="37">
         <f>_xll.qlRateHelperLatestDate($D33)</f>
-        <v>43584</v>
+        <v>43585</v>
       </c>
       <c r="I33" s="190">
-        <v>0.92574553341576982</v>
+        <v>0.92146454514249376</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="0"/>
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L33" s="177" t="s">
         <v>202</v>
@@ -9167,7 +9184,7 @@
       </c>
       <c r="E34" s="39">
         <f>_xll.qlRateHelperRate($D34)</f>
-        <v>1.8530000000000001E-2</v>
+        <v>1.881E-2</v>
       </c>
       <c r="F34" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D34)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D34)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D34)),_xll.qlSwapRateHelperSpread($D34))</f>
@@ -9175,18 +9192,18 @@
       </c>
       <c r="G34" s="38">
         <f>_xll.qlRateHelperEarliestDate($D34)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H34" s="37">
         <f>_xll.qlRateHelperLatestDate($D34)</f>
-        <v>43949</v>
+        <v>43951</v>
       </c>
       <c r="I34" s="190">
-        <v>0.89194362226685286</v>
+        <v>0.89064085390931669</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L34" s="177" t="s">
         <v>203</v>
@@ -9201,7 +9218,7 @@
       </c>
       <c r="E35" s="39">
         <f>_xll.qlRateHelperRate($D35)</f>
-        <v>2.1360000000000001E-2</v>
+        <v>2.0979999999999999E-2</v>
       </c>
       <c r="F35" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D35)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D35)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D35)),_xll.qlSwapRateHelperSpread($D35))</f>
@@ -9209,14 +9226,14 @@
       </c>
       <c r="G35" s="38">
         <f>_xll.qlRateHelperEarliestDate($D35)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H35" s="37">
         <f>_xll.qlRateHelperLatestDate($D35)</f>
-        <v>44314</v>
+        <v>44316</v>
       </c>
       <c r="I35" s="190">
-        <v>0.85688593085826803</v>
+        <v>0.85973774428778293</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="0"/>
@@ -9235,7 +9252,7 @@
       </c>
       <c r="E36" s="39">
         <f>_xll.qlRateHelperRate($D36)</f>
-        <v>2.3700000000000002E-2</v>
+        <v>2.274E-2</v>
       </c>
       <c r="F36" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D36)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D36)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D36)),_xll.qlSwapRateHelperSpread($D36))</f>
@@ -9243,18 +9260,18 @@
       </c>
       <c r="G36" s="38">
         <f>_xll.qlRateHelperEarliestDate($D36)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H36" s="37">
         <f>_xll.qlRateHelperLatestDate($D36)</f>
-        <v>44679</v>
+        <v>44680</v>
       </c>
       <c r="I36" s="190">
-        <v>0.82147028364323149</v>
+        <v>0.82891291278483903</v>
       </c>
       <c r="J36" s="1">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L36" s="177" t="s">
         <v>205</v>
@@ -9269,7 +9286,7 @@
       </c>
       <c r="E37" s="39">
         <f>_xll.qlRateHelperRate($D37)</f>
-        <v>2.5600000000000001E-2</v>
+        <v>2.4150000000000001E-2</v>
       </c>
       <c r="F37" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D37)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D37)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D37)),_xll.qlSwapRateHelperSpread($D37))</f>
@@ -9277,18 +9294,18 @@
       </c>
       <c r="G37" s="38">
         <f>_xll.qlRateHelperEarliestDate($D37)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H37" s="37">
         <f>_xll.qlRateHelperLatestDate($D37)</f>
         <v>45044</v>
       </c>
       <c r="I37" s="190">
-        <v>0.78673886650781921</v>
+        <v>0.79879970099135589</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="0"/>
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L37" s="177" t="s">
         <v>206</v>
@@ -9303,7 +9320,7 @@
       </c>
       <c r="E38" s="39">
         <f>_xll.qlRateHelperRate($D38)</f>
-        <v>2.7160000000000004E-2</v>
+        <v>2.5329999999999998E-2</v>
       </c>
       <c r="F38" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D38)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D38)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D38)),_xll.qlSwapRateHelperSpread($D38))</f>
@@ -9311,14 +9328,14 @@
       </c>
       <c r="G38" s="38">
         <f>_xll.qlRateHelperEarliestDate($D38)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H38" s="37">
         <f>_xll.qlRateHelperLatestDate($D38)</f>
-        <v>45411</v>
+        <v>45412</v>
       </c>
       <c r="I38" s="190">
-        <v>0.75289795944057114</v>
+        <v>0.76905606573791763</v>
       </c>
       <c r="L38" s="177" t="s">
         <v>207</v>
@@ -9333,7 +9350,7 @@
       </c>
       <c r="E39" s="39">
         <f>_xll.qlRateHelperRate($D39)</f>
-        <v>2.9679999999999998E-2</v>
+        <v>2.724E-2</v>
       </c>
       <c r="F39" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D39)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D39)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D39)),_xll.qlSwapRateHelperSpread($D39))</f>
@@ -9341,14 +9358,14 @@
       </c>
       <c r="G39" s="38">
         <f>_xll.qlRateHelperEarliestDate($D39)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H39" s="37">
         <f>_xll.qlRateHelperLatestDate($D39)</f>
-        <v>46140</v>
+        <v>46142</v>
       </c>
       <c r="I39" s="190">
-        <v>0.68767738449036797</v>
+        <v>0.71155340907264242</v>
       </c>
       <c r="L39" s="177" t="s">
         <v>208</v>
@@ -9363,7 +9380,7 @@
       </c>
       <c r="E40" s="39">
         <f>_xll.qlRateHelperRate($D40)</f>
-        <v>3.2070000000000001E-2</v>
+        <v>2.92E-2</v>
       </c>
       <c r="F40" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D40)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D40)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D40)),_xll.qlSwapRateHelperSpread($D40))</f>
@@ -9371,14 +9388,14 @@
       </c>
       <c r="G40" s="38">
         <f>_xll.qlRateHelperEarliestDate($D40)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H40" s="37">
         <f>_xll.qlRateHelperLatestDate($D40)</f>
         <v>47238</v>
       </c>
       <c r="I40" s="190">
-        <v>0.6010204069840539</v>
+        <v>0.63230663100627083</v>
       </c>
       <c r="L40" s="177" t="s">
         <v>209</v>
@@ -9393,7 +9410,7 @@
       </c>
       <c r="E41" s="39">
         <f>_xll.qlRateHelperRate($D41)</f>
-        <v>3.4079999999999999E-2</v>
+        <v>3.0869999999999998E-2</v>
       </c>
       <c r="F41" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D41)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D41)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D41)),_xll.qlSwapRateHelperSpread($D41))</f>
@@ -9401,14 +9418,14 @@
       </c>
       <c r="G41" s="38">
         <f>_xll.qlRateHelperEarliestDate($D41)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H41" s="37">
         <f>_xll.qlRateHelperLatestDate($D41)</f>
         <v>49062</v>
       </c>
       <c r="I41" s="190">
-        <v>0.48471539557630899</v>
+        <v>0.52296904035024483</v>
       </c>
       <c r="L41" s="177" t="s">
         <v>210</v>
@@ -9423,7 +9440,7 @@
       </c>
       <c r="E42" s="39">
         <f>_xll.qlRateHelperRate($D42)</f>
-        <v>3.4970000000000001E-2</v>
+        <v>3.1600000000000003E-2</v>
       </c>
       <c r="F42" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D42)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D42)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D42)),_xll.qlSwapRateHelperSpread($D42))</f>
@@ -9431,14 +9448,14 @@
       </c>
       <c r="G42" s="38">
         <f>_xll.qlRateHelperEarliestDate($D42)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H42" s="37">
         <f>_xll.qlRateHelperLatestDate($D42)</f>
-        <v>50888</v>
+        <v>50889</v>
       </c>
       <c r="I42" s="190">
-        <v>0.39512527969412525</v>
+        <v>0.43641118383599042</v>
       </c>
       <c r="L42" s="177" t="s">
         <v>211</v>
@@ -9453,7 +9470,7 @@
       </c>
       <c r="E43" s="39">
         <f>_xll.qlRateHelperRate($D43)</f>
-        <v>3.567E-2</v>
+        <v>3.1959999999999995E-2</v>
       </c>
       <c r="F43" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D43)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D43)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D43)),_xll.qlSwapRateHelperSpread($D43))</f>
@@ -9461,14 +9478,14 @@
       </c>
       <c r="G43" s="38">
         <f>_xll.qlRateHelperEarliestDate($D43)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H43" s="37">
         <f>_xll.qlRateHelperLatestDate($D43)</f>
-        <v>54541</v>
+        <v>54543</v>
       </c>
       <c r="I43" s="190">
-        <v>0.26725880738088237</v>
+        <v>0.31197030353297411</v>
       </c>
       <c r="L43" s="177" t="s">
         <v>212</v>
@@ -9483,7 +9500,7 @@
       </c>
       <c r="E44" s="39">
         <f>_xll.qlRateHelperRate($D44)</f>
-        <v>3.5680000000000003E-2</v>
+        <v>3.1989999999999998E-2</v>
       </c>
       <c r="F44" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D44)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D44)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D44)),_xll.qlSwapRateHelperSpread($D44))</f>
@@ -9491,14 +9508,14 @@
       </c>
       <c r="G44" s="38">
         <f>_xll.qlRateHelperEarliestDate($D44)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H44" s="37">
         <f>_xll.qlRateHelperLatestDate($D44)</f>
-        <v>56367</v>
+        <v>56369</v>
       </c>
       <c r="I44" s="190">
-        <v>0.2235873037676859</v>
+        <v>0.26536442509905256</v>
       </c>
       <c r="L44" s="177" t="s">
         <v>213</v>
@@ -9513,7 +9530,7 @@
       </c>
       <c r="E45" s="39">
         <f>_xll.qlRateHelperRate($D45)</f>
-        <v>3.5590000000000004E-2</v>
+        <v>3.1910000000000001E-2</v>
       </c>
       <c r="F45" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D45)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D45)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D45)),_xll.qlSwapRateHelperSpread($D45))</f>
@@ -9521,14 +9538,14 @@
       </c>
       <c r="G45" s="38">
         <f>_xll.qlRateHelperEarliestDate($D45)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H45" s="37">
         <f>_xll.qlRateHelperLatestDate($D45)</f>
-        <v>58193</v>
+        <v>58195</v>
       </c>
       <c r="I45" s="190">
-        <v>0.18902957744587393</v>
+        <v>0.22798429343299909</v>
       </c>
       <c r="L45" s="177" t="s">
         <v>214</v>
@@ -9543,7 +9560,7 @@
       </c>
       <c r="E46" s="39">
         <f>_xll.qlRateHelperRate($D46)</f>
-        <v>3.5499999999999997E-2</v>
+        <v>3.1799999999999995E-2</v>
       </c>
       <c r="F46" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D46)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D46)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D46)),_xll.qlSwapRateHelperSpread($D46))</f>
@@ -9551,14 +9568,14 @@
       </c>
       <c r="G46" s="38">
         <f>_xll.qlRateHelperEarliestDate($D46)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="H46" s="37">
         <f>_xll.qlRateHelperLatestDate($D46)</f>
-        <v>60020</v>
+        <v>60022</v>
       </c>
       <c r="I46" s="190">
-        <v>0.16020945108279799</v>
+        <v>0.19692498522639698</v>
       </c>
       <c r="L46" s="177" t="s">
         <v>215</v>
@@ -11533,7 +11550,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11607,7 +11624,7 @@
       </c>
       <c r="F3" s="103" t="str">
         <f>_xll.qlDepositRateHelper(E3,D3,C3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OND#0000</v>
+        <v>USD_YCONRH_OND#0001</v>
       </c>
       <c r="G3" s="102" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -11638,7 +11655,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11723,7 +11740,7 @@
       </c>
       <c r="H3" s="144" t="str">
         <f>_xll.qlFraRateHelper(G3,F3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_TND#0000</v>
+        <v>USD_YCONRH_TND#0001</v>
       </c>
       <c r="I3" s="143" t="str">
         <f>_xll.ohRangeRetrieveError(H3)</f>
@@ -11755,7 +11772,7 @@
       </c>
       <c r="H4" s="141" t="str">
         <f>_xll.qlFraRateHelper(G4,F4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_SND#0000</v>
+        <v>USD_YCONRH_SND#0001</v>
       </c>
       <c r="I4" s="140" t="str">
         <f>_xll.ohRangeRetrieveError(H4)</f>
@@ -11793,7 +11810,7 @@
   <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11913,7 +11930,7 @@
       </c>
       <c r="L4" s="170" t="str">
         <f>_xll.qlEonia(K4,,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS_LiborON#0000</v>
+        <v>USD_YCONRH_OIS_LiborON#0001</v>
       </c>
       <c r="M4" s="169" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -11972,7 +11989,7 @@
       </c>
       <c r="L6" s="162" t="str">
         <f>_xll.qlOISRateHelper(K6,2,C6,J6,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OISSW#0000</v>
+        <v>USD_YCONRH_OISSW#0004</v>
       </c>
       <c r="M6" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -11981,11 +11998,11 @@
       <c r="N6" s="159"/>
       <c r="P6" s="161">
         <f>_xll.qlRateHelperEarliestDate($L6)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q6" s="161">
         <f>_xll.qlRateHelperLatestDate($L6)</f>
-        <v>41764</v>
+        <v>41766</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -12024,7 +12041,7 @@
       </c>
       <c r="L7" s="162" t="str">
         <f>_xll.qlOISRateHelper(K7,2,C7,J7,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2W#0000</v>
+        <v>USD_YCONRH_OIS2W#0001</v>
       </c>
       <c r="M7" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -12033,11 +12050,11 @@
       <c r="N7" s="159"/>
       <c r="P7" s="161">
         <f>_xll.qlRateHelperEarliestDate(L7)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q7" s="161">
         <f>_xll.qlRateHelperLatestDate($L7)</f>
-        <v>41771</v>
+        <v>41773</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -12076,7 +12093,7 @@
       </c>
       <c r="L8" s="162" t="str">
         <f>_xll.qlOISRateHelper(K8,2,C8,J8,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3W#0000</v>
+        <v>USD_YCONRH_OIS3W#0001</v>
       </c>
       <c r="M8" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -12085,11 +12102,11 @@
       <c r="N8" s="159"/>
       <c r="P8" s="161">
         <f>_xll.qlRateHelperEarliestDate(L8)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q8" s="161">
         <f>_xll.qlRateHelperLatestDate($L8)</f>
-        <v>41778</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -12128,7 +12145,7 @@
       </c>
       <c r="L9" s="162" t="str">
         <f>_xll.qlOISRateHelper(K9,2,C9,J9,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS1M#0000</v>
+        <v>USD_YCONRH_OIS1M#0001</v>
       </c>
       <c r="M9" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -12137,11 +12154,11 @@
       <c r="N9" s="159"/>
       <c r="P9" s="161">
         <f>_xll.qlRateHelperEarliestDate(L9)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q9" s="161">
         <f>_xll.qlRateHelperLatestDate($L9)</f>
-        <v>41787</v>
+        <v>41789</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -12180,7 +12197,7 @@
       </c>
       <c r="L10" s="162" t="str">
         <f>_xll.qlOISRateHelper(K10,2,C10,J10,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2M#0000</v>
+        <v>USD_YCONRH_OIS2M#0001</v>
       </c>
       <c r="M10" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -12189,7 +12206,7 @@
       <c r="N10" s="159"/>
       <c r="P10" s="161">
         <f>_xll.qlRateHelperEarliestDate(L10)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q10" s="161">
         <f>_xll.qlRateHelperLatestDate($L10)</f>
@@ -12232,7 +12249,7 @@
       </c>
       <c r="L11" s="162" t="str">
         <f>_xll.qlOISRateHelper(K11,2,C11,J11,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3M#0000</v>
+        <v>USD_YCONRH_OIS3M#0001</v>
       </c>
       <c r="M11" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -12241,11 +12258,11 @@
       <c r="N11" s="159"/>
       <c r="P11" s="161">
         <f>_xll.qlRateHelperEarliestDate(L11)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q11" s="161">
         <f>_xll.qlRateHelperLatestDate($L11)</f>
-        <v>41848</v>
+        <v>41851</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -12284,7 +12301,7 @@
       </c>
       <c r="L12" s="162" t="str">
         <f>_xll.qlOISRateHelper(K12,2,C12,J12,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS4M#0000</v>
+        <v>USD_YCONRH_OIS4M#0001</v>
       </c>
       <c r="M12" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -12293,11 +12310,11 @@
       <c r="N12" s="159"/>
       <c r="P12" s="161">
         <f>_xll.qlRateHelperEarliestDate(L12)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q12" s="161">
         <f>_xll.qlRateHelperLatestDate($L12)</f>
-        <v>41879</v>
+        <v>41880</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -12336,7 +12353,7 @@
       </c>
       <c r="L13" s="162" t="str">
         <f>_xll.qlOISRateHelper(K13,2,C13,J13,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS5M#0000</v>
+        <v>USD_YCONRH_OIS5M#0001</v>
       </c>
       <c r="M13" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -12345,11 +12362,11 @@
       <c r="N13" s="159"/>
       <c r="P13" s="161">
         <f>_xll.qlRateHelperEarliestDate(L13)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q13" s="161">
         <f>_xll.qlRateHelperLatestDate($L13)</f>
-        <v>41911</v>
+        <v>41912</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -12388,7 +12405,7 @@
       </c>
       <c r="L14" s="162" t="str">
         <f>_xll.qlOISRateHelper(K14,2,C14,J14,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS6M#0000</v>
+        <v>USD_YCONRH_OIS6M#0001</v>
       </c>
       <c r="M14" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -12397,11 +12414,11 @@
       <c r="N14" s="159"/>
       <c r="P14" s="161">
         <f>_xll.qlRateHelperEarliestDate(L14)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q14" s="161">
         <f>_xll.qlRateHelperLatestDate($L14)</f>
-        <v>41940</v>
+        <v>41943</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -12440,7 +12457,7 @@
       </c>
       <c r="L15" s="162" t="str">
         <f>_xll.qlOISRateHelper(K15,2,C15,J15,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS7M#0000</v>
+        <v>USD_YCONRH_OIS7M#0001</v>
       </c>
       <c r="M15" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -12449,7 +12466,7 @@
       <c r="N15" s="159"/>
       <c r="P15" s="161">
         <f>_xll.qlRateHelperEarliestDate(L15)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q15" s="161">
         <f>_xll.qlRateHelperLatestDate($L15)</f>
@@ -12492,7 +12509,7 @@
       </c>
       <c r="L16" s="162" t="str">
         <f>_xll.qlOISRateHelper(K16,2,C16,J16,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS8M#0000</v>
+        <v>USD_YCONRH_OIS8M#0001</v>
       </c>
       <c r="M16" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -12501,11 +12518,11 @@
       <c r="N16" s="159"/>
       <c r="P16" s="161">
         <f>_xll.qlRateHelperEarliestDate(L16)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q16" s="161">
         <f>_xll.qlRateHelperLatestDate($L16)</f>
-        <v>42002</v>
+        <v>42004</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -12544,7 +12561,7 @@
       </c>
       <c r="L17" s="162" t="str">
         <f>_xll.qlOISRateHelper(K17,2,C17,J17,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS9M#0000</v>
+        <v>USD_YCONRH_OIS9M#0001</v>
       </c>
       <c r="M17" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -12553,11 +12570,11 @@
       <c r="N17" s="159"/>
       <c r="P17" s="161">
         <f>_xll.qlRateHelperEarliestDate(L17)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q17" s="161">
         <f>_xll.qlRateHelperLatestDate($L17)</f>
-        <v>42032</v>
+        <v>42034</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -12596,7 +12613,7 @@
       </c>
       <c r="L18" s="162" t="str">
         <f>_xll.qlOISRateHelper(K18,2,C18,J18,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS10M#0000</v>
+        <v>USD_YCONRH_OIS10M#0001</v>
       </c>
       <c r="M18" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -12605,7 +12622,7 @@
       <c r="N18" s="159"/>
       <c r="P18" s="161">
         <f>_xll.qlRateHelperEarliestDate(L18)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q18" s="161">
         <f>_xll.qlRateHelperLatestDate($L18)</f>
@@ -12648,7 +12665,7 @@
       </c>
       <c r="L19" s="162" t="str">
         <f>_xll.qlOISRateHelper(K19,2,C19,J19,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS11M#0000</v>
+        <v>USD_YCONRH_OIS11M#0001</v>
       </c>
       <c r="M19" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -12657,11 +12674,11 @@
       <c r="N19" s="159"/>
       <c r="P19" s="161">
         <f>_xll.qlRateHelperEarliestDate(L19)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q19" s="161">
         <f>_xll.qlRateHelperLatestDate($L19)</f>
-        <v>42093</v>
+        <v>42094</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -12700,7 +12717,7 @@
       </c>
       <c r="L20" s="162" t="str">
         <f>_xll.qlOISRateHelper(K20,2,C20,J20,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS1Y#0000</v>
+        <v>USD_YCONRH_OIS1Y#0001</v>
       </c>
       <c r="M20" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -12709,11 +12726,11 @@
       <c r="N20" s="159"/>
       <c r="P20" s="161">
         <f>_xll.qlRateHelperEarliestDate(L20)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q20" s="161">
         <f>_xll.qlRateHelperLatestDate($L20)</f>
-        <v>42122</v>
+        <v>42124</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -12752,7 +12769,7 @@
       </c>
       <c r="L21" s="162" t="str">
         <f>_xll.qlOISRateHelper(K21,2,C21,J21,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS13M#0000</v>
+        <v>USD_YCONRH_OIS13M#0001</v>
       </c>
       <c r="M21" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -12761,11 +12778,11 @@
       <c r="N21" s="159"/>
       <c r="P21" s="161">
         <f>_xll.qlRateHelperEarliestDate(L21)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q21" s="161">
         <f>_xll.qlRateHelperLatestDate($L21)</f>
-        <v>42152</v>
+        <v>42153</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -12804,7 +12821,7 @@
       </c>
       <c r="L22" s="162" t="str">
         <f>_xll.qlOISRateHelper(K22,2,C22,J22,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS14M#0000</v>
+        <v>USD_YCONRH_OIS14M#0001</v>
       </c>
       <c r="M22" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -12813,11 +12830,11 @@
       <c r="N22" s="159"/>
       <c r="P22" s="161">
         <f>_xll.qlRateHelperEarliestDate(L22)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q22" s="161">
         <f>_xll.qlRateHelperLatestDate($L22)</f>
-        <v>42184</v>
+        <v>42185</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -12856,7 +12873,7 @@
       </c>
       <c r="L23" s="162" t="str">
         <f>_xll.qlOISRateHelper(K23,2,C23,J23,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS15M#0000</v>
+        <v>USD_YCONRH_OIS15M#0001</v>
       </c>
       <c r="M23" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -12865,11 +12882,11 @@
       <c r="N23" s="159"/>
       <c r="P23" s="161">
         <f>_xll.qlRateHelperEarliestDate(L23)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q23" s="161">
         <f>_xll.qlRateHelperLatestDate($L23)</f>
-        <v>42213</v>
+        <v>42216</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -12908,7 +12925,7 @@
       </c>
       <c r="L24" s="162" t="str">
         <f>_xll.qlOISRateHelper(K24,2,C24,J24,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS16M#0000</v>
+        <v>USD_YCONRH_OIS16M#0001</v>
       </c>
       <c r="M24" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -12917,11 +12934,11 @@
       <c r="N24" s="159"/>
       <c r="P24" s="161">
         <f>_xll.qlRateHelperEarliestDate(L24)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q24" s="161">
         <f>_xll.qlRateHelperLatestDate($L24)</f>
-        <v>42244</v>
+        <v>42247</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -12960,7 +12977,7 @@
       </c>
       <c r="L25" s="162" t="str">
         <f>_xll.qlOISRateHelper(K25,2,C25,J25,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS17M#0000</v>
+        <v>USD_YCONRH_OIS17M#0001</v>
       </c>
       <c r="M25" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -12969,11 +12986,11 @@
       <c r="N25" s="159"/>
       <c r="P25" s="161">
         <f>_xll.qlRateHelperEarliestDate(L25)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q25" s="161">
         <f>_xll.qlRateHelperLatestDate($L25)</f>
-        <v>42275</v>
+        <v>42277</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -13012,7 +13029,7 @@
       </c>
       <c r="L26" s="162" t="str">
         <f>_xll.qlOISRateHelper(K26,2,C26,J26,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS18M#0000</v>
+        <v>USD_YCONRH_OIS18M#0001</v>
       </c>
       <c r="M26" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -13021,11 +13038,11 @@
       <c r="N26" s="159"/>
       <c r="P26" s="161">
         <f>_xll.qlRateHelperEarliestDate(L26)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q26" s="161">
         <f>_xll.qlRateHelperLatestDate($L26)</f>
-        <v>42305</v>
+        <v>42307</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
@@ -13064,7 +13081,7 @@
       </c>
       <c r="L27" s="162" t="str">
         <f>_xll.qlOISRateHelper(K27,2,C27,J27,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS19M#0000</v>
+        <v>USD_YCONRH_OIS19M#0001</v>
       </c>
       <c r="M27" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -13073,7 +13090,7 @@
       <c r="N27" s="159"/>
       <c r="P27" s="161">
         <f>_xll.qlRateHelperEarliestDate(L27)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q27" s="161">
         <f>_xll.qlRateHelperLatestDate($L27)</f>
@@ -13116,7 +13133,7 @@
       </c>
       <c r="L28" s="162" t="str">
         <f>_xll.qlOISRateHelper(K28,2,C28,J28,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS20M#0000</v>
+        <v>USD_YCONRH_OIS20M#0001</v>
       </c>
       <c r="M28" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -13125,11 +13142,11 @@
       <c r="N28" s="159"/>
       <c r="P28" s="161">
         <f>_xll.qlRateHelperEarliestDate(L28)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q28" s="161">
         <f>_xll.qlRateHelperLatestDate($L28)</f>
-        <v>42366</v>
+        <v>42369</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
@@ -13168,7 +13185,7 @@
       </c>
       <c r="L29" s="162" t="str">
         <f>_xll.qlOISRateHelper(K29,2,C29,J29,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS21M#0000</v>
+        <v>USD_YCONRH_OIS21M#0001</v>
       </c>
       <c r="M29" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -13177,11 +13194,11 @@
       <c r="N29" s="159"/>
       <c r="P29" s="161">
         <f>_xll.qlRateHelperEarliestDate(L29)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q29" s="161">
         <f>_xll.qlRateHelperLatestDate($L29)</f>
-        <v>42397</v>
+        <v>42398</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -13220,7 +13237,7 @@
       </c>
       <c r="L30" s="162" t="str">
         <f>_xll.qlOISRateHelper(K30,2,C30,J30,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS22M#0000</v>
+        <v>USD_YCONRH_OIS22M#0001</v>
       </c>
       <c r="M30" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -13229,7 +13246,7 @@
       <c r="N30" s="159"/>
       <c r="P30" s="161">
         <f>_xll.qlRateHelperEarliestDate(L30)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q30" s="161">
         <f>_xll.qlRateHelperLatestDate($L30)</f>
@@ -13272,7 +13289,7 @@
       </c>
       <c r="L31" s="162" t="str">
         <f>_xll.qlOISRateHelper(K31,2,C31,J31,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS23M#0000</v>
+        <v>USD_YCONRH_OIS23M#0001</v>
       </c>
       <c r="M31" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -13281,11 +13298,11 @@
       <c r="N31" s="159"/>
       <c r="P31" s="161">
         <f>_xll.qlRateHelperEarliestDate(L31)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q31" s="161">
         <f>_xll.qlRateHelperLatestDate($L31)</f>
-        <v>42458</v>
+        <v>42460</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -13324,7 +13341,7 @@
       </c>
       <c r="L32" s="162" t="str">
         <f>_xll.qlOISRateHelper(K32,2,C32,J32,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS2Y#0000</v>
+        <v>USD_YCONRH_OIS2Y#0001</v>
       </c>
       <c r="M32" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -13333,11 +13350,11 @@
       <c r="N32" s="159"/>
       <c r="P32" s="161">
         <f>_xll.qlRateHelperEarliestDate(L32)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q32" s="161">
         <f>_xll.qlRateHelperLatestDate($L32)</f>
-        <v>42488</v>
+        <v>42489</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
@@ -13376,7 +13393,7 @@
       </c>
       <c r="L33" s="162" t="str">
         <f>_xll.qlOISRateHelper(K33,2,C33,J33,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS27M#0000</v>
+        <v>USD_YCONRH_OIS27M#0001</v>
       </c>
       <c r="M33" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -13385,11 +13402,11 @@
       <c r="N33" s="159"/>
       <c r="P33" s="161">
         <f>_xll.qlRateHelperEarliestDate(L33)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q33" s="161">
         <f>_xll.qlRateHelperLatestDate($L33)</f>
-        <v>42579</v>
+        <v>42580</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
@@ -13428,7 +13445,7 @@
       </c>
       <c r="L34" s="162" t="str">
         <f>_xll.qlOISRateHelper(K34,2,C34,J34,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS30M#0000</v>
+        <v>USD_YCONRH_OIS30M#0001</v>
       </c>
       <c r="M34" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -13437,11 +13454,11 @@
       <c r="N34" s="159"/>
       <c r="P34" s="161">
         <f>_xll.qlRateHelperEarliestDate(L34)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q34" s="161">
         <f>_xll.qlRateHelperLatestDate($L34)</f>
-        <v>42671</v>
+        <v>42674</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
@@ -13480,7 +13497,7 @@
       </c>
       <c r="L35" s="162" t="str">
         <f>_xll.qlOISRateHelper(K35,2,C35,J35,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS33M#0000</v>
+        <v>USD_YCONRH_OIS33M#0001</v>
       </c>
       <c r="M35" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -13489,7 +13506,7 @@
       <c r="N35" s="159"/>
       <c r="P35" s="161">
         <f>_xll.qlRateHelperEarliestDate(L35)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q35" s="161">
         <f>_xll.qlRateHelperLatestDate($L35)</f>
@@ -13532,7 +13549,7 @@
       </c>
       <c r="L36" s="162" t="str">
         <f>_xll.qlOISRateHelper(K36,2,C36,J36,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS3Y#0000</v>
+        <v>USD_YCONRH_OIS3Y#0001</v>
       </c>
       <c r="M36" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -13541,7 +13558,7 @@
       <c r="N36" s="159"/>
       <c r="P36" s="161">
         <f>_xll.qlRateHelperEarliestDate(L36)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q36" s="161">
         <f>_xll.qlRateHelperLatestDate($L36)</f>
@@ -13584,7 +13601,7 @@
       </c>
       <c r="L37" s="162" t="str">
         <f>_xll.qlOISRateHelper(K37,2,C37,J37,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS39M#0000</v>
+        <v>USD_YCONRH_OIS39M#0001</v>
       </c>
       <c r="M37" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -13593,11 +13610,11 @@
       <c r="N37" s="159"/>
       <c r="P37" s="161">
         <f>_xll.qlRateHelperEarliestDate(L37)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q37" s="161">
         <f>_xll.qlRateHelperLatestDate($L37)</f>
-        <v>42944</v>
+        <v>42947</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -13636,7 +13653,7 @@
       </c>
       <c r="L38" s="162" t="str">
         <f>_xll.qlOISRateHelper(K38,2,C38,J38,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS42M#0000</v>
+        <v>USD_YCONRH_OIS42M#0001</v>
       </c>
       <c r="M38" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -13682,7 +13699,7 @@
       </c>
       <c r="L39" s="162" t="str">
         <f>_xll.qlOISRateHelper(K39,2,C39,J39,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS45M#0000</v>
+        <v>USD_YCONRH_OIS45M#0001</v>
       </c>
       <c r="M39" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -13728,7 +13745,7 @@
       </c>
       <c r="L40" s="162" t="str">
         <f>_xll.qlOISRateHelper(K40,2,C40,J40,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS4Y#0000</v>
+        <v>USD_YCONRH_OIS4Y#0001</v>
       </c>
       <c r="M40" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -13774,7 +13791,7 @@
       </c>
       <c r="L41" s="162" t="str">
         <f>_xll.qlOISRateHelper(K41,2,C41,J41,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS51M#0000</v>
+        <v>USD_YCONRH_OIS51M#0001</v>
       </c>
       <c r="M41" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -13820,7 +13837,7 @@
       </c>
       <c r="L42" s="162" t="str">
         <f>_xll.qlOISRateHelper(K42,2,C42,J42,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS54M#0000</v>
+        <v>USD_YCONRH_OIS54M#0001</v>
       </c>
       <c r="M42" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>
@@ -13866,7 +13883,7 @@
       </c>
       <c r="L43" s="162" t="str">
         <f>_xll.qlOISRateHelper(K43,2,C43,J43,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS57M#0000</v>
+        <v>USD_YCONRH_OIS57M#0001</v>
       </c>
       <c r="M43" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L43)</f>
@@ -13912,7 +13929,7 @@
       </c>
       <c r="L44" s="162" t="str">
         <f>_xll.qlOISRateHelper(K44,2,C44,J44,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS5Y#0000</v>
+        <v>USD_YCONRH_OIS5Y#0001</v>
       </c>
       <c r="M44" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L44)</f>
@@ -13958,7 +13975,7 @@
       </c>
       <c r="L45" s="162" t="str">
         <f>_xll.qlOISRateHelper(K45,2,C45,J45,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS6Y#0000</v>
+        <v>USD_YCONRH_OIS6Y#0001</v>
       </c>
       <c r="M45" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L45)</f>
@@ -14004,7 +14021,7 @@
       </c>
       <c r="L46" s="162" t="str">
         <f>_xll.qlOISRateHelper(K46,2,C46,J46,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS7Y#0000</v>
+        <v>USD_YCONRH_OIS7Y#0001</v>
       </c>
       <c r="M46" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L46)</f>
@@ -14050,7 +14067,7 @@
       </c>
       <c r="L47" s="162" t="str">
         <f>_xll.qlOISRateHelper(K47,2,C47,J47,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS8Y#0000</v>
+        <v>USD_YCONRH_OIS8Y#0001</v>
       </c>
       <c r="M47" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L47)</f>
@@ -14096,7 +14113,7 @@
       </c>
       <c r="L48" s="162" t="str">
         <f>_xll.qlOISRateHelper(K48,2,C48,J48,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS9Y#0000</v>
+        <v>USD_YCONRH_OIS9Y#0001</v>
       </c>
       <c r="M48" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L48)</f>
@@ -14142,7 +14159,7 @@
       </c>
       <c r="L49" s="162" t="str">
         <f>_xll.qlOISRateHelper(K49,2,C49,J49,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS10Y#0000</v>
+        <v>USD_YCONRH_OIS10Y#0001</v>
       </c>
       <c r="M49" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L49)</f>
@@ -14188,7 +14205,7 @@
       </c>
       <c r="L50" s="162" t="str">
         <f>_xll.qlOISRateHelper(K50,2,C50,J50,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS12Y#0000</v>
+        <v>USD_YCONRH_OIS12Y#0001</v>
       </c>
       <c r="M50" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L50)</f>
@@ -14234,7 +14251,7 @@
       </c>
       <c r="L51" s="162" t="str">
         <f>_xll.qlOISRateHelper(K51,2,C51,J51,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS15Y#0000</v>
+        <v>USD_YCONRH_OIS15Y#0001</v>
       </c>
       <c r="M51" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L51)</f>
@@ -14280,7 +14297,7 @@
       </c>
       <c r="L52" s="162" t="str">
         <f>_xll.qlOISRateHelper(K52,2,C52,J52,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS20Y#0000</v>
+        <v>USD_YCONRH_OIS20Y#0001</v>
       </c>
       <c r="M52" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L52)</f>
@@ -14326,7 +14343,7 @@
       </c>
       <c r="L53" s="162" t="str">
         <f>_xll.qlOISRateHelper(K53,2,C53,J53,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS25Y#0000</v>
+        <v>USD_YCONRH_OIS25Y#0001</v>
       </c>
       <c r="M53" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L53)</f>
@@ -14372,7 +14389,7 @@
       </c>
       <c r="L54" s="162" t="str">
         <f>_xll.qlOISRateHelper(K54,2,C54,J54,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS27Y#0000</v>
+        <v>USD_YCONRH_OIS27Y#0001</v>
       </c>
       <c r="M54" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L54)</f>
@@ -14418,7 +14435,7 @@
       </c>
       <c r="L55" s="162" t="str">
         <f>_xll.qlOISRateHelper(K55,2,C55,J55,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS30Y#0000</v>
+        <v>USD_YCONRH_OIS30Y#0001</v>
       </c>
       <c r="M55" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L55)</f>
@@ -14464,7 +14481,7 @@
       </c>
       <c r="L56" s="162" t="str">
         <f>_xll.qlOISRateHelper(K56,2,C56,J56,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS35Y#0000</v>
+        <v>USD_YCONRH_OIS35Y#0001</v>
       </c>
       <c r="M56" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L56)</f>
@@ -14510,7 +14527,7 @@
       </c>
       <c r="L57" s="162" t="str">
         <f>_xll.qlOISRateHelper(K57,2,C57,J57,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS40Y#0000</v>
+        <v>USD_YCONRH_OIS40Y#0001</v>
       </c>
       <c r="M57" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L57)</f>
@@ -14556,7 +14573,7 @@
       </c>
       <c r="L58" s="162" t="str">
         <f>_xll.qlOISRateHelper(K58,2,C58,J58,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS45Y#0000</v>
+        <v>USD_YCONRH_OIS45Y#0001</v>
       </c>
       <c r="M58" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L58)</f>
@@ -14602,7 +14619,7 @@
       </c>
       <c r="L59" s="162" t="str">
         <f>_xll.qlOISRateHelper(K59,2,C59,J59,$L$4,,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YCONRH_OIS50Y#0000</v>
+        <v>USD_YCONRH_OIS50Y#0001</v>
       </c>
       <c r="M59" s="93" t="str">
         <f>_xll.ohRangeRetrieveError(L59)</f>
@@ -14611,11 +14628,11 @@
       <c r="N59" s="159"/>
       <c r="P59" s="161">
         <f>_xll.qlRateHelperEarliestDate(L59)</f>
-        <v>41757</v>
+        <v>41759</v>
       </c>
       <c r="Q59" s="161">
         <f>_xll.qlRateHelperLatestDate($L59)</f>
-        <v>60020</v>
+        <v>60022</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>